<commit_message>
Solve the issue of empty unit
Add code to check active label, and generate label for active unit
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Network_Data_Sync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1B6F06B1-24CA-4EA0-A53E-9BD7924D674B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EB43710D-0536-4734-8A6F-6F3B4EC6A227}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840"/>
   </bookViews>
@@ -2106,8 +2106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:IV41"/>
+    <sheetView tabSelected="1" topLeftCell="C128" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5249,6 +5249,9 @@
       <c r="D131" s="5" t="s">
         <v>524</v>
       </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
       <c r="G131">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
add Exp Stats and code for excel processing
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Network_Data_Sync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EB43710D-0536-4734-8A6F-6F3B4EC6A227}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F899C825-78A9-4C06-8FD8-A12663BB2972}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840"/>
+    <workbookView xWindow="17970" yWindow="525" windowWidth="20355" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="528">
   <si>
     <t>ephysFN</t>
   </si>
@@ -836,9 +836,6 @@
   </si>
   <si>
     <t>CMA Evolution of Ch 50 (V4) evolution 191114(CRP). ch 50 (-5,-6) 3 -degrees  generate PCs for later PC space tuning</t>
-  </si>
-  <si>
-    <t>CMA Evolution of Ch 57 (V4) evolution 191114(CRP). ch 57 (-3,-6) 3 1, SU 2/5 generate PCs for later PC space tuning</t>
   </si>
   <si>
     <t>Derived from PCs of Ch 57 (V4) evolution 191115(CRP). ch 57 (-3,-4) 4 -degrees  121 images from PC23 space, add the pasupathy images to it. white background 4 rotations.</t>
@@ -1692,6 +1689,12 @@
   </si>
   <si>
     <t>\\storage1.ris.wustl.edu\crponce\Active\Stimuli\2019-Manifold\beto-191111b\backup_11_11_2019_14_04_49</t>
+  </si>
+  <si>
+    <t>CMA Evolution of Ch 57 (V4) evolution 191114(CRP). ch 57 (-3,-6) 3 1, SU 2/5 generate PCs for later PC space tuning (this exp failed to pair with Manifold)</t>
+  </si>
+  <si>
+    <t>Freeview</t>
   </si>
 </sst>
 </file>
@@ -2106,8 +2109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C128" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G131" sqref="G131"/>
+    <sheetView tabSelected="1" topLeftCell="D99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2115,7 +2118,7 @@
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="70.5703125" customWidth="1"/>
-    <col min="4" max="4" width="108.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="8" width="9.28515625" customWidth="1"/>
@@ -2135,16 +2138,16 @@
         <v>217</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2161,7 +2164,7 @@
         <v>218</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2184,7 +2187,7 @@
         <v>219</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2207,7 +2210,7 @@
         <v>220</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -2230,7 +2233,7 @@
         <v>221</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2253,7 +2256,7 @@
         <v>222</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2276,7 +2279,7 @@
         <v>223</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -2299,7 +2302,7 @@
         <v>224</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2322,7 +2325,7 @@
         <v>225</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2345,7 +2348,7 @@
         <v>226</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2368,7 +2371,7 @@
         <v>227</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -2391,7 +2394,7 @@
         <v>228</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -2414,7 +2417,7 @@
         <v>229</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -2437,7 +2440,7 @@
         <v>230</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -2460,7 +2463,7 @@
         <v>231</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -2483,7 +2486,7 @@
         <v>232</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -2492,7 +2495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>233</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -2515,7 +2518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>234</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -2538,7 +2541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>235</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -2561,7 +2564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>236</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -2584,7 +2587,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>237</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -2607,7 +2610,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>238</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -2630,7 +2633,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2644,7 +2647,7 @@
         <v>239</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -2653,7 +2656,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>240</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -2676,7 +2679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2690,7 +2693,7 @@
         <v>241</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -2699,7 +2702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>242</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -2722,7 +2725,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -2736,7 +2739,7 @@
         <v>243</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -2745,7 +2748,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>244</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -2768,7 +2771,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -2782,7 +2785,7 @@
         <v>245</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -2791,7 +2794,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>246</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -2814,7 +2817,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>247</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -2836,8 +2839,11 @@
       <c r="G31">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2851,7 +2857,7 @@
         <v>248</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -2860,7 +2866,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>249</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -2882,8 +2888,11 @@
       <c r="G33">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2897,7 +2906,7 @@
         <v>250</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -2906,7 +2915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2920,7 +2929,7 @@
         <v>251</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -2928,8 +2937,11 @@
       <c r="G35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -2943,7 +2955,7 @@
         <v>252</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -2952,7 +2964,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2966,7 +2978,7 @@
         <v>253</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -2974,8 +2986,11 @@
       <c r="G37">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -2989,7 +3004,7 @@
         <v>254</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -2998,7 +3013,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -3012,7 +3027,7 @@
         <v>255</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -3020,8 +3035,11 @@
       <c r="G39">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -3035,7 +3053,7 @@
         <v>256</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -3044,7 +3062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -3052,13 +3070,13 @@
         <v>113</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>257</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -3066,8 +3084,11 @@
       <c r="G41">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -3081,7 +3102,7 @@
         <v>258</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -3089,8 +3110,11 @@
       <c r="G42">
         <v>56</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -3104,7 +3128,7 @@
         <v>259</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -3112,8 +3136,11 @@
       <c r="G43">
         <v>56</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -3127,7 +3154,7 @@
         <v>260</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -3135,8 +3162,11 @@
       <c r="G44">
         <v>54</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -3150,7 +3180,7 @@
         <v>261</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -3158,8 +3188,11 @@
       <c r="G45">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -3173,7 +3206,7 @@
         <v>262</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -3181,8 +3214,11 @@
       <c r="G46">
         <v>54</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -3196,7 +3232,7 @@
         <v>263</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -3204,8 +3240,11 @@
       <c r="G47">
         <v>58</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -3219,13 +3258,16 @@
         <v>264</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F48">
         <v>23</v>
       </c>
       <c r="G48">
         <v>58</v>
+      </c>
+      <c r="H48">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -3242,13 +3284,16 @@
         <v>265</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F49">
         <v>23</v>
       </c>
       <c r="G49">
         <v>58</v>
+      </c>
+      <c r="H49">
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -3265,13 +3310,16 @@
         <v>266</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F50">
         <v>24</v>
       </c>
       <c r="G50">
         <v>50</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -3288,13 +3336,16 @@
         <v>267</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F51">
         <v>24</v>
       </c>
       <c r="G51">
         <v>50</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -3311,13 +3362,16 @@
         <v>268</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F52">
         <v>24</v>
       </c>
       <c r="G52">
         <v>50</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -3331,16 +3385,17 @@
         <v>197</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>496</v>
-      </c>
+        <v>526</v>
+      </c>
+      <c r="E53" s="6"/>
       <c r="F53">
         <v>24</v>
       </c>
       <c r="G53">
         <v>57</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -3354,16 +3409,19 @@
         <v>198</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F54">
         <v>25</v>
       </c>
       <c r="G54">
         <v>57</v>
+      </c>
+      <c r="H54">
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -3377,16 +3435,19 @@
         <v>199</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F55">
         <v>25</v>
       </c>
       <c r="G55">
         <v>57</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -3400,16 +3461,19 @@
         <v>200</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F56">
         <v>25</v>
       </c>
       <c r="G56">
         <v>57</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -3423,10 +3487,10 @@
         <v>201</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -3449,10 +3513,10 @@
         <v>202</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -3475,10 +3539,10 @@
         <v>203</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -3501,16 +3565,19 @@
         <v>204</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F60">
         <v>27</v>
       </c>
       <c r="G60">
         <v>26</v>
+      </c>
+      <c r="H60">
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -3524,16 +3591,19 @@
         <v>205</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F61">
         <v>27</v>
       </c>
       <c r="G61">
         <v>26</v>
+      </c>
+      <c r="H61">
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -3547,16 +3617,19 @@
         <v>206</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F62">
         <v>27</v>
       </c>
       <c r="G62">
         <v>26</v>
+      </c>
+      <c r="H62">
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -3570,10 +3643,10 @@
         <v>207</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -3596,10 +3669,10 @@
         <v>208</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -3622,10 +3695,10 @@
         <v>209</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -3648,10 +3721,10 @@
         <v>210</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -3674,10 +3747,10 @@
         <v>208</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -3700,10 +3773,10 @@
         <v>211</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -3726,10 +3799,10 @@
         <v>212</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -3752,10 +3825,10 @@
         <v>213</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -3778,10 +3851,10 @@
         <v>214</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -3804,10 +3877,10 @@
         <v>215</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -3830,10 +3903,10 @@
         <v>216</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -3847,19 +3920,19 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="E74" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -3873,19 +3946,19 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="E75" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -3899,19 +3972,19 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="E76" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -3925,19 +3998,19 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="E77" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -3951,19 +4024,19 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="E78" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -3977,19 +4050,19 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>323</v>
-      </c>
       <c r="D79" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -4003,19 +4076,19 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="D80" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -4029,19 +4102,19 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>326</v>
-      </c>
       <c r="D81" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -4055,19 +4128,19 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="C82" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -4081,19 +4154,19 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="D83" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -4107,19 +4180,19 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D84" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -4133,19 +4206,19 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="D85" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F85">
         <v>36</v>
@@ -4159,19 +4232,19 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>337</v>
-      </c>
       <c r="D86" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -4185,19 +4258,19 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>349</v>
-      </c>
       <c r="D87" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F87">
         <v>37</v>
@@ -4211,19 +4284,19 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>343</v>
-      </c>
       <c r="D88" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -4237,19 +4310,19 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="D89" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -4263,19 +4336,19 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="D90" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F90">
         <v>38</v>
@@ -4289,19 +4362,19 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="D91" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -4315,19 +4388,19 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>369</v>
-      </c>
       <c r="D92" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F92">
         <v>39</v>
@@ -4341,19 +4414,19 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>363</v>
-      </c>
       <c r="C93" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -4367,19 +4440,19 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>361</v>
-      </c>
       <c r="D94" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -4393,19 +4466,19 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>385</v>
-      </c>
       <c r="D95" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F95">
         <v>40</v>
@@ -4419,19 +4492,19 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="D96" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -4445,19 +4518,19 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="D97" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F97">
         <v>41</v>
@@ -4471,19 +4544,19 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>379</v>
-      </c>
       <c r="C98" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -4497,19 +4570,19 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="D99" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -4523,37 +4596,39 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>382</v>
-      </c>
       <c r="D100" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="E100" s="6"/>
+        <v>388</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>527</v>
+      </c>
       <c r="F100">
         <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>405</v>
-      </c>
       <c r="D101" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F101">
         <v>42</v>
@@ -4567,19 +4642,19 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="D102" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -4593,19 +4668,19 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>397</v>
-      </c>
       <c r="D103" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -4619,19 +4694,19 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>408</v>
-      </c>
       <c r="D104" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F104">
         <v>43</v>
@@ -4645,19 +4720,19 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>402</v>
-      </c>
       <c r="C105" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -4671,19 +4746,19 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="D106" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -4697,55 +4772,59 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="D107" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="E107" s="6"/>
+        <v>426</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>527</v>
+      </c>
       <c r="F107">
         <v>43</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="C108" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="E108" s="6"/>
+      <c r="E108" s="6" t="s">
+        <v>527</v>
+      </c>
       <c r="F108">
         <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>442</v>
-      </c>
       <c r="C109" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F109">
         <v>44</v>
@@ -4759,19 +4838,19 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>434</v>
-      </c>
       <c r="D110" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -4785,19 +4864,19 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="C111" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -4811,19 +4890,19 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>447</v>
-      </c>
       <c r="E112" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F112">
         <v>45</v>
@@ -4837,19 +4916,19 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>440</v>
-      </c>
       <c r="D113" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -4863,19 +4942,19 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>437</v>
-      </c>
       <c r="D114" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -4889,19 +4968,19 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>457</v>
-      </c>
       <c r="E115" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H115">
         <v>3</v>
@@ -4909,19 +4988,19 @@
     </row>
     <row r="116" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B116" t="s">
         <v>458</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>459</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>461</v>
-      </c>
       <c r="E116" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F116">
         <v>1</v>
@@ -4935,19 +5014,19 @@
     </row>
     <row r="117" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C117" t="s">
+        <v>463</v>
+      </c>
+      <c r="D117" t="s">
         <v>464</v>
       </c>
-      <c r="D117" t="s">
-        <v>465</v>
-      </c>
       <c r="E117" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H117">
         <v>2</v>
@@ -4955,19 +5034,19 @@
     </row>
     <row r="118" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D118" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F118">
         <v>2</v>
@@ -4981,19 +5060,19 @@
     </row>
     <row r="119" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F119">
         <v>3</v>
@@ -5007,19 +5086,19 @@
     </row>
     <row r="120" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>473</v>
+      </c>
+      <c r="B120" t="s">
         <v>474</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>475</v>
       </c>
-      <c r="C120" t="s">
-        <v>476</v>
-      </c>
       <c r="D120" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H120">
         <v>2</v>
@@ -5027,19 +5106,19 @@
     </row>
     <row r="121" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>476</v>
+      </c>
+      <c r="B121" t="s">
         <v>477</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>478</v>
       </c>
-      <c r="C121" t="s">
-        <v>479</v>
-      </c>
       <c r="D121" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F121">
         <v>4</v>
@@ -5053,16 +5132,16 @@
     </row>
     <row r="122" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>479</v>
+      </c>
+      <c r="B122" t="s">
         <v>480</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>481</v>
       </c>
-      <c r="C122" t="s">
-        <v>482</v>
-      </c>
       <c r="D122" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E122" s="6"/>
       <c r="G122">
@@ -5074,19 +5153,19 @@
     </row>
     <row r="123" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>482</v>
+      </c>
+      <c r="B123" t="s">
         <v>483</v>
       </c>
-      <c r="B123" t="s">
-        <v>484</v>
-      </c>
       <c r="C123" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H123">
         <v>3</v>
@@ -5094,19 +5173,19 @@
     </row>
     <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>484</v>
+      </c>
+      <c r="B124" t="s">
         <v>485</v>
       </c>
-      <c r="B124" t="s">
-        <v>486</v>
-      </c>
       <c r="C124" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -5114,19 +5193,19 @@
     </row>
     <row r="125" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>486</v>
+      </c>
+      <c r="B125" t="s">
         <v>487</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>488</v>
       </c>
-      <c r="C125" t="s">
-        <v>489</v>
-      </c>
       <c r="D125" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F125">
         <v>5</v>
@@ -5140,33 +5219,33 @@
     </row>
     <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="C126" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="C126" s="8" t="s">
-        <v>501</v>
-      </c>
       <c r="D126" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A127" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="B127" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="B127" s="8" t="s">
+      <c r="C127" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C127" s="8" t="s">
-        <v>504</v>
-      </c>
       <c r="D127" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E127" s="6"/>
       <c r="G127">
@@ -5178,19 +5257,19 @@
     </row>
     <row r="128" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="C128" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="C128" s="8" t="s">
-        <v>507</v>
-      </c>
       <c r="D128" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F128">
         <v>6</v>
@@ -5204,16 +5283,16 @@
     </row>
     <row r="129" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A129" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>511</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="C129" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="C129" s="8" t="s">
-        <v>513</v>
-      </c>
       <c r="D129" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H129">
         <v>2</v>
@@ -5221,16 +5300,16 @@
     </row>
     <row r="130" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>514</v>
       </c>
-      <c r="B130" s="8" t="s">
-        <v>515</v>
-      </c>
       <c r="C130" s="8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H130">
         <v>1</v>
@@ -5238,16 +5317,16 @@
     </row>
     <row r="131" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="B131" s="8" t="s">
         <v>516</v>
       </c>
-      <c r="B131" s="8" t="s">
+      <c r="C131" s="8" t="s">
         <v>517</v>
       </c>
-      <c r="C131" s="8" t="s">
-        <v>518</v>
-      </c>
       <c r="D131" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F131">
         <v>1</v>
@@ -5261,19 +5340,19 @@
     </row>
     <row r="132" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="B132" s="8" t="s">
         <v>519</v>
       </c>
-      <c r="B132" s="8" t="s">
+      <c r="C132" s="8" t="s">
         <v>520</v>
       </c>
-      <c r="C132" s="8" t="s">
-        <v>521</v>
-      </c>
       <c r="D132" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F132">
         <v>7</v>

</xml_diff>

<commit_message>
Add code to tackle different unit in channel
Add LFP as well
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F50AD9D-56A8-46F0-8CE0-AF1946AAC9FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="568">
   <si>
     <t>ephysFN</t>
   </si>
@@ -1219,7 +1225,7 @@
     <t>N:\Stimuli\2019-12-Evolutions\2020-01-23-Beto-01\2020-01-23-12-36-03</t>
   </si>
   <si>
-    <t xml:space="preserve">. </t>
+    <t>. </t>
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-01-27-Beto-01\2020-01-27-11-23-03</t>
@@ -1684,13 +1690,13 @@
 Blasting him, 300 ms, going to block 50 then calling it a day</t>
   </si>
   <si>
-    <t xml:space="preserve">Rf basic Start 11:11, 35 ms reward. New units in 41, rf looks weird tho Stopped at 11:17, 4 blocks complete </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generate integrate. Ch 5 hash (1/5) [-1.5, 1] 3 1; GA vs CMAES, bigset05 first 10 images Start at 11:23. Carlos recalibrated eye at block 2. working well 45 ms reward . Evolved images are climbing…..block 16, #1(black line) is top line Block 27: Black line is wayyy above the rest and still climbing. Reward at 50 at block 30,  Stopped at 12:04, 40 blocks completed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generate integrated. Ch 20. hash 1/5. [-2, 1.5] 3 1. start at 12:06 Bigset20 first 10 images, reward at 90. starting to shake chair Upped to 130 reward. Added aq reward at block 16. 170 ms at block 20. Evolved images are climbing, both above natural now Hmm, nether really taking off yet. Block 28, 220+30 One image is more contrasting (white background, pink and dark colored object) Other image is more gray/pink and blended. monkey quitting. Experiment has enough blocks to call it completed, but we're really struggling to get the last few trials. Let's see if we make it to block 35.  </t>
+    <t>Rf basic Start 11:11, 35 ms reward. New units in 41, rf looks weird tho Stopped at 11:17, 4 blocks complete </t>
+  </si>
+  <si>
+    <t>Generate integrate. Ch 5 hash (1/5) [-1.5, 1] 3 1; GA vs CMAES, bigset05 first 10 images Start at 11:23. Carlos recalibrated eye at block 2. working well 45 ms reward . Evolved images are climbing…..block 16, #1(black line) is top line Block 27: Black line is wayyy above the rest and still climbing. Reward at 50 at block 30,  Stopped at 12:04, 40 blocks completed </t>
+  </si>
+  <si>
+    <t>Generate integrated. Ch 20. hash 1/5. [-2, 1.5] 3 1. start at 12:06 Bigset20 first 10 images, reward at 90. starting to shake chair Upped to 130 reward. Added aq reward at block 16. 170 ms at block 20. Evolved images are climbing, both above natural now Hmm, nether really taking off yet. Block 28, 220+30 One image is more contrasting (white background, pink and dark colored object) Other image is more gray/pink and blended. monkey quitting. Experiment has enough blocks to call it completed, but we're really struggling to get the last few trials. Let's see if we make it to block 35.  </t>
   </si>
   <si>
     <t>001 RFMapper 11:02 AM starts 
@@ -1851,8 +1857,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1911,15 +1917,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1961,7 +1975,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1993,9 +2007,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2027,6 +2059,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2202,14 +2252,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="J141" sqref="J141"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2261,7 +2313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2287,7 +2339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2313,7 +2365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2339,7 +2391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2365,7 +2417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2391,7 +2443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2417,7 +2469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2443,7 +2495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2469,7 +2521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2495,7 +2547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2521,7 +2573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2547,7 +2599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2573,7 +2625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2599,7 +2651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2625,7 +2677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2651,7 +2703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2677,7 +2729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -2703,7 +2755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2729,7 +2781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2755,7 +2807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -2781,7 +2833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -2807,7 +2859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2833,7 +2885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2859,7 +2911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -2885,7 +2937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -2911,7 +2963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2937,7 +2989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -2963,7 +3015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2989,7 +3041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -3015,7 +3067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -3041,7 +3093,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3067,7 +3119,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -3093,7 +3145,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -3119,7 +3171,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -3145,7 +3197,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -3171,7 +3223,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -3197,7 +3249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -3223,7 +3275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -3249,7 +3301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -3275,7 +3327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -3301,7 +3353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3327,7 +3379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -3353,7 +3405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -3379,7 +3431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -3405,7 +3457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -3431,7 +3483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -3457,7 +3509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -3483,7 +3535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -3509,7 +3561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -3535,7 +3587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -3561,7 +3613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -3584,7 +3636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -3610,7 +3662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -3636,7 +3688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -3662,7 +3714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3688,7 +3740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -3714,7 +3766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -3740,7 +3792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -3766,7 +3818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3792,7 +3844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -3818,7 +3870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -3844,7 +3896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -3870,7 +3922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -3896,7 +3948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -3922,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -3948,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -3974,7 +4026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -4000,7 +4052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -4026,7 +4078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -4052,7 +4104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -4078,7 +4130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -4104,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -4130,7 +4182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -4156,7 +4208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -4182,7 +4234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -4208,7 +4260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -4234,7 +4286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -4260,7 +4312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -4286,7 +4338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -4309,7 +4361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -4332,7 +4384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -4355,7 +4407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -4381,7 +4433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -4407,7 +4459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -4433,7 +4485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -4459,7 +4511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -4485,7 +4537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -4511,7 +4563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -4537,7 +4589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -4563,7 +4615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -4589,7 +4641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -4615,7 +4667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -4641,7 +4693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -4667,7 +4719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -4693,7 +4745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -4719,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -4745,7 +4797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -4771,7 +4823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -4797,7 +4849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -4817,7 +4869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -4843,7 +4895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -4869,7 +4921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -4895,7 +4947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -4921,7 +4973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -4947,7 +4999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -4973,7 +5025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -4993,7 +5045,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -5013,7 +5065,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -5039,7 +5091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -5065,7 +5117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -5091,7 +5143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -5117,7 +5169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -5143,7 +5195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -5169,7 +5221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -5189,7 +5241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -5215,7 +5267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -5235,7 +5287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -5261,7 +5313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -5287,7 +5339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -5307,7 +5359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -5333,7 +5385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -5353,7 +5405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -5373,7 +5425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -5393,7 +5445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -5419,7 +5471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -5436,7 +5488,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -5456,7 +5508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -5482,7 +5534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>136</v>
       </c>
@@ -5499,7 +5551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -5516,7 +5568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -5539,7 +5591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -5565,7 +5617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -5585,7 +5637,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>141</v>
       </c>
@@ -5605,7 +5657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>142</v>
       </c>
@@ -5631,7 +5683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -5657,7 +5709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -5683,7 +5735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -5709,7 +5761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>146</v>
       </c>
@@ -5722,8 +5774,14 @@
       <c r="D140" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="E140" t="s">
+        <v>567</v>
+      </c>
+      <c r="H140">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -5736,8 +5794,14 @@
       <c r="D141" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="142" spans="1:8">
+      <c r="E141" t="s">
+        <v>567</v>
+      </c>
+      <c r="H141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>148</v>
       </c>
@@ -5750,8 +5814,20 @@
       <c r="D142" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="143" spans="1:8">
+      <c r="E142" t="s">
+        <v>567</v>
+      </c>
+      <c r="F142">
+        <v>5</v>
+      </c>
+      <c r="G142">
+        <v>5</v>
+      </c>
+      <c r="H142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -5763,6 +5839,18 @@
       </c>
       <c r="D143" t="s">
         <v>563</v>
+      </c>
+      <c r="E143" t="s">
+        <v>567</v>
+      </c>
+      <c r="F143">
+        <v>6</v>
+      </c>
+      <c r="G143">
+        <v>20</v>
+      </c>
+      <c r="H143">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debug the Optimizer comparison code for Alfa
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01995C10-8197-4D42-ACB9-F704D65D14F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41571AD4-D234-4FF0-A3D4-C4FF0B4F1A69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="656">
   <si>
     <t>ephysFN</t>
   </si>
@@ -487,6 +487,63 @@
     <t>Beto-03032020-006</t>
   </si>
   <si>
+    <t>Beto-06032020-001</t>
+  </si>
+  <si>
+    <t>Beto-06032020-004</t>
+  </si>
+  <si>
+    <t>Beto-09032020-001</t>
+  </si>
+  <si>
+    <t>Beto-09032020-002</t>
+  </si>
+  <si>
+    <t>Beto-09032020-004</t>
+  </si>
+  <si>
+    <t>Beto-09032020-005</t>
+  </si>
+  <si>
+    <t>Beto-10022020-001</t>
+  </si>
+  <si>
+    <t>Beto-10022020-002</t>
+  </si>
+  <si>
+    <t>Beto-10022020-005</t>
+  </si>
+  <si>
+    <t>Beto64chan-10022020-004</t>
+  </si>
+  <si>
+    <t>Beto64chan-10022020-006</t>
+  </si>
+  <si>
+    <t>Beto-07022020-004</t>
+  </si>
+  <si>
+    <t>Beto-14022020-001</t>
+  </si>
+  <si>
+    <t>Beto-14022020-002</t>
+  </si>
+  <si>
+    <t>Beto-14022020-003</t>
+  </si>
+  <si>
+    <t>Beto-19022020-004</t>
+  </si>
+  <si>
+    <t>Beto-20022020-001</t>
+  </si>
+  <si>
+    <t>Beto-20022020-002</t>
+  </si>
+  <si>
+    <t>Beto-20022020-003</t>
+  </si>
+  <si>
     <t>191002_Beto_selectivity_basic(1)</t>
   </si>
   <si>
@@ -925,6 +982,60 @@
     <t>200303_Beto_generate_integrated(6)</t>
   </si>
   <si>
+    <t>200306_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200306_Beto_generate_integrated(3)</t>
+  </si>
+  <si>
+    <t>200309_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200309_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200309_Beto_generate_integrated(3)</t>
+  </si>
+  <si>
+    <t>200309_Beto_generate_integrated(4)</t>
+  </si>
+  <si>
+    <t>200210_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200210_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200210_Beto_generate_integrated(6)</t>
+  </si>
+  <si>
+    <t>200210_Beto_selectivity_basic(1)</t>
+  </si>
+  <si>
+    <t>200207_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200214_Beto_rfMapper_basic(3)</t>
+  </si>
+  <si>
+    <t>200214_Beto_rfMapper_basic(4)</t>
+  </si>
+  <si>
+    <t>200214_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200219_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200220_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200220_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200220_Beto_generate_integrated</t>
+  </si>
+  <si>
     <t>\\storage1.ris.wustl.edu\crponce\Active\Stimuli\2019-Selectivity\2019-10-02a-beto</t>
   </si>
   <si>
@@ -1328,6 +1439,39 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-03-Beto-03\2020-03-03-13-36-50</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-06-Beto-01\2020-03-06-12-11-33</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-09-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-09-Beto-01\2020-03-09-14-58-23</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-09-Beto-02\2020-03-09-15-44-10</t>
+  </si>
+  <si>
+    <t>Stimuli\2019-12-Evolutions\2020-02-10-Beto-01\2020-02-10-14-18-32</t>
+  </si>
+  <si>
+    <t>Stimuli\2019-12-Evolutions\2020-02-10-Beto-02\2020-02-10-14-43-14</t>
+  </si>
+  <si>
+    <t>Stimuli\2019-12-Evolutions\2020-02-07-Beto-02\2020-02-07-10-23-49</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-02-14-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-02-14-Beto-01\2020-02-14-14-23-26</t>
+  </si>
+  <si>
+    <t>Stimuli\2019-12-Evolutions\2020-02-19-Beto-01\2020-02-19-14-23-48</t>
+  </si>
+  <si>
+    <t>Stimuli\2019-12-Evolutions\2020-02-20-Beto-01\2020-02-20-10-29-18</t>
   </si>
   <si>
     <t>Derived from PCs of Ch 29 evolution 191002. 373 images {11*11 in PC2,PC3; PC49 PC50; RND RND space respectively, +10 last gen}</t>
@@ -1937,6 +2081,158 @@
 Completed</t>
   </si>
   <si>
+    <t>Start 1147 rf map.
+Maybe try su vs hash in 24
+4 blocks complete at 1159</t>
+  </si>
+  <si>
+    <t>Generate integrated start at 12:11
+24 [-0.5, 1.5] 3 1 CMAES
+24 [-0.5, 1.5] 3 2 CMAES
+Reward at 60
+Block 7, 1 is starting to climb!!
+Block 29, still climbing
+Stop at 1:16</t>
+  </si>
+  <si>
+    <t>001 RF mapping 14:29 started
+Takes a while to get Beto started.
+-1.5:0.5:1.5 0.75deg
+Completed</t>
+  </si>
+  <si>
+    <t>002 RF mapping starts 14:38
+-8:2:8 2deg
+works great!
+Completed</t>
+  </si>
+  <si>
+    <t>004 Generate Integrated
+5 [-0.5 1 ] 1 CMAES
+5 [-0.5 1 ] 1 ZOHA_Sphere_lr
+ZOHA is fast at first, but later it became slower and wandering around get passed by CMAES at around ~20 gens. (Seems the learning rate decay is too fast? Or not fast enough?)
+mu is 36.67 deg, exponentially converge to 7.33 deg at 50 generation
+Finish with 40mins, 40gens!
+Completed</t>
+  </si>
+  <si>
+    <t>005 Generate Integrated
+5 [-0.5 1 ] 1 CMAES
+5 [-0.5 1 ] 1 ZOHA_Sphere_lr
+Tune the Optimizer! Tune the exploration range, to make it more variable the intial mu is 50 deg, exponentially converge to 7.33 deg at 50 generation
+ZOHA and CMAES stay very close to each other!
+Make it to 30 gens
+Completed
+Completed</t>
+  </si>
+  <si>
+    <t>001 RFMapping  13:35 starts
+The Eye calibration takes a lot of time
+Monkey seems not in its mood in the Alfa's rig.
+Eye signal very bouncy/noisy</t>
+  </si>
+  <si>
+    <t>002
+2nd rf mapping with smaller image
+Seems like a 2 peaks under equator, may be 2 different RF from 2 different unit?
+Or is it edge effect, that it's the edge instead of the image center that excites the neuron?</t>
+  </si>
+  <si>
+    <t>005
+2:18 start, carlos moved eye scan, changed setting in both MonkLogic and iscan computer… looks so much better.
+Channel 39 SU, has 2 SU and 1 hash. Doing hash vs SU trial
+39 [0,  -0.5]  3 1 CMAES
+39 [0,  -0.5]  3 2 CMAES
+02:35:00</t>
+  </si>
+  <si>
+    <t>004 at 243 PM better isolation
+(6)?
+now it says alfa….
+Evolved images climbing, made it to block 20.
+Upped to 200 mL,
+Stopped at 3:19, plateaued. We were not using gabor stimuli
+complete</t>
+  </si>
+  <si>
+    <t>Selectivity basic, start at 3:22.
+Channel 39 [0, -0.5] 3 with gabors
+ended</t>
+  </si>
+  <si>
+    <t>004 at 1023
+SU VS HASH
+39 (0,-0.5) 3 1 CMAES, SU 1/5
+39 (0,-0.5) 3 2 CMAES
+MATLAB CRASHED!!!!!
+File seems intact, though</t>
+  </si>
+  <si>
+    <t>001 RFMapper starts 13:53
+Monkey is just not working ….. Sleep for a while
+-8:2:8 2 deg image!
+Coarse level mapping
+RFMapper Basic (3)
+Completed</t>
+  </si>
+  <si>
+    <t>002 RFMapping
+Monkey
+-1.5:0.5:1.5 1deg image
+It works well!!
+Also a 2 peak 2 spot Receptive field, This time there is a major one and a minor one.
+Finish 4 blocks in 5 mins!
+RFMapper Basic (4)
+Completed</t>
+  </si>
+  <si>
+    <t>003 generate_integrated 48 mins
+39 [0, -0.2] 3 1 CMAES
+39 [0, -0.2] 3 2 CMAES
+Start at 2:23
+This will be the only experiment for the day, so giving him lots of water
+Seems The reference images are not copied correctly but seems fine!(forget to use Gabor stimuli)
+Nice Evolution.
+Finished 15:13 Completed</t>
+  </si>
+  <si>
+    <t>004 generate_integrated starts 14:23 (go for 90 mins)
+ITI 390-500ms it's normal!
+25 [0 0 ] 3 1 CMAES
+25 [0 0 ] 3 2 CMAES
+seems the Hash is not very evolvable.???
+PSTH have visually responsive component but not very large?
+25 A evolves as normal, and 25 B is not very responsive….? But starts to evolve at 13
+Hash evolution is just not very successful .
+Complete</t>
+  </si>
+  <si>
+    <t>Hp at 930
+001 at 950 AM
+GOTTA FIX THAT WAITING FOR DATA ACQUISITION TO START TIMEOUT
+nice SU in 41
+still getting header words do not match error sometimes.
+he's not that engaged. 21 correct trials in 7 minutes. Yikes.
+850 ITI. Gotta fix that.
+15 minutes in, 65 trials. Oof.
+that 41 is not super responsive</t>
+  </si>
+  <si>
+    <t>002 at 1012 AM
+rf mapping, finer grid</t>
+  </si>
+  <si>
+    <t>003 at 1030 AM
+integrated, SU vs hash
+41, (0,-0.5) 3 1 'CMAES'
+41 (0,-0.5) 3 2 'CMAES'
+Block 23, still climbing, added 30 aq reward with 100 ms
+Stopped at 11:26, 28 blocks complete</t>
+  </si>
+  <si>
+    <t>SUHash</t>
+  </si>
+  <si>
     <t>Manifold</t>
   </si>
   <si>
@@ -1947,6 +2243,9 @@
   </si>
   <si>
     <t>RedDim_Evol</t>
+  </si>
+  <si>
+    <t>200210_Beto_generate_integrated(2)</t>
   </si>
 </sst>
 </file>
@@ -2005,10 +2304,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2348,15 +2650,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="I148" sqref="I148"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
+    <col min="4" max="4" width="81.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2390,16 +2695,16 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>301</v>
+        <v>338</v>
       </c>
       <c r="D2" t="s">
-        <v>436</v>
+        <v>484</v>
       </c>
       <c r="E2" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2416,16 +2721,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>302</v>
+        <v>339</v>
       </c>
       <c r="D3" t="s">
-        <v>437</v>
+        <v>485</v>
       </c>
       <c r="E3" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2442,16 +2747,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>303</v>
+        <v>340</v>
       </c>
       <c r="D4" t="s">
-        <v>438</v>
+        <v>486</v>
       </c>
       <c r="E4" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -2468,16 +2773,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>487</v>
       </c>
       <c r="E5" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2494,16 +2799,16 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>305</v>
+        <v>342</v>
       </c>
       <c r="D6" t="s">
-        <v>440</v>
+        <v>488</v>
       </c>
       <c r="E6" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2520,16 +2825,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="C7" t="s">
-        <v>306</v>
+        <v>343</v>
       </c>
       <c r="D7" t="s">
-        <v>441</v>
+        <v>489</v>
       </c>
       <c r="E7" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -2546,16 +2851,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>344</v>
       </c>
       <c r="D8" t="s">
-        <v>442</v>
+        <v>490</v>
       </c>
       <c r="E8" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2572,16 +2877,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s">
-        <v>308</v>
+        <v>345</v>
       </c>
       <c r="D9" t="s">
-        <v>443</v>
+        <v>491</v>
       </c>
       <c r="E9" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2598,16 +2903,16 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
-        <v>309</v>
+        <v>346</v>
       </c>
       <c r="D10" t="s">
-        <v>444</v>
+        <v>492</v>
       </c>
       <c r="E10" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2624,16 +2929,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
-        <v>310</v>
+        <v>347</v>
       </c>
       <c r="D11" t="s">
-        <v>445</v>
+        <v>493</v>
       </c>
       <c r="E11" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -2650,16 +2955,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="C12" t="s">
-        <v>311</v>
+        <v>348</v>
       </c>
       <c r="D12" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="E12" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -2676,16 +2981,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s">
-        <v>312</v>
+        <v>349</v>
       </c>
       <c r="D13" t="s">
-        <v>447</v>
+        <v>495</v>
       </c>
       <c r="E13" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -2702,16 +3007,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
       <c r="D14" t="s">
-        <v>448</v>
+        <v>496</v>
       </c>
       <c r="E14" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -2728,16 +3033,16 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>351</v>
       </c>
       <c r="D15" t="s">
-        <v>449</v>
+        <v>497</v>
       </c>
       <c r="E15" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -2754,16 +3059,16 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="C16" t="s">
-        <v>315</v>
+        <v>352</v>
       </c>
       <c r="D16" t="s">
-        <v>450</v>
+        <v>498</v>
       </c>
       <c r="E16" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -2780,16 +3085,16 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="C17" t="s">
-        <v>316</v>
+        <v>353</v>
       </c>
       <c r="D17" t="s">
-        <v>451</v>
+        <v>499</v>
       </c>
       <c r="E17" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -2806,16 +3111,16 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="C18" t="s">
-        <v>317</v>
+        <v>354</v>
       </c>
       <c r="D18" t="s">
-        <v>452</v>
+        <v>500</v>
       </c>
       <c r="E18" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -2832,16 +3137,16 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="D19" t="s">
-        <v>453</v>
+        <v>501</v>
       </c>
       <c r="E19" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -2858,16 +3163,16 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="C20" t="s">
-        <v>319</v>
+        <v>356</v>
       </c>
       <c r="D20" t="s">
-        <v>454</v>
+        <v>502</v>
       </c>
       <c r="E20" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -2884,16 +3189,16 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
-        <v>320</v>
+        <v>357</v>
       </c>
       <c r="D21" t="s">
-        <v>455</v>
+        <v>503</v>
       </c>
       <c r="E21" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -2910,16 +3215,16 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="C22" t="s">
-        <v>321</v>
+        <v>358</v>
       </c>
       <c r="D22" t="s">
-        <v>456</v>
+        <v>504</v>
       </c>
       <c r="E22" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -2936,16 +3241,16 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="C23" t="s">
-        <v>322</v>
+        <v>359</v>
       </c>
       <c r="D23" t="s">
-        <v>457</v>
+        <v>505</v>
       </c>
       <c r="E23" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -2962,16 +3267,16 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>323</v>
+        <v>360</v>
       </c>
       <c r="D24" t="s">
-        <v>458</v>
+        <v>506</v>
       </c>
       <c r="E24" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -2988,16 +3293,16 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
-        <v>324</v>
+        <v>361</v>
       </c>
       <c r="D25" t="s">
-        <v>459</v>
+        <v>507</v>
       </c>
       <c r="E25" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -3014,16 +3319,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="C26" t="s">
-        <v>325</v>
+        <v>362</v>
       </c>
       <c r="D26" t="s">
-        <v>460</v>
+        <v>508</v>
       </c>
       <c r="E26" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -3040,16 +3345,16 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C27" t="s">
-        <v>326</v>
+        <v>363</v>
       </c>
       <c r="D27" t="s">
-        <v>461</v>
+        <v>509</v>
       </c>
       <c r="E27" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -3066,16 +3371,16 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="C28" t="s">
-        <v>327</v>
+        <v>364</v>
       </c>
       <c r="D28" t="s">
-        <v>462</v>
+        <v>510</v>
       </c>
       <c r="E28" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -3092,16 +3397,16 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
       <c r="D29" t="s">
-        <v>463</v>
+        <v>511</v>
       </c>
       <c r="E29" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -3118,16 +3423,16 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>329</v>
+        <v>366</v>
       </c>
       <c r="D30" t="s">
-        <v>464</v>
+        <v>512</v>
       </c>
       <c r="E30" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -3144,16 +3449,16 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="C31" t="s">
-        <v>330</v>
+        <v>367</v>
       </c>
       <c r="D31" t="s">
-        <v>465</v>
+        <v>513</v>
       </c>
       <c r="E31" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -3170,16 +3475,16 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="C32" t="s">
-        <v>331</v>
+        <v>368</v>
       </c>
       <c r="D32" t="s">
-        <v>466</v>
+        <v>514</v>
       </c>
       <c r="E32" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -3196,16 +3501,16 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="C33" t="s">
-        <v>332</v>
+        <v>369</v>
       </c>
       <c r="D33" t="s">
-        <v>467</v>
+        <v>515</v>
       </c>
       <c r="E33" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -3222,16 +3527,16 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="C34" t="s">
-        <v>333</v>
+        <v>370</v>
       </c>
       <c r="D34" t="s">
-        <v>468</v>
+        <v>516</v>
       </c>
       <c r="E34" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -3248,16 +3553,16 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="C35" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="D35" t="s">
-        <v>469</v>
+        <v>517</v>
       </c>
       <c r="E35" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -3274,16 +3579,16 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="C36" t="s">
-        <v>335</v>
+        <v>372</v>
       </c>
       <c r="D36" t="s">
-        <v>470</v>
+        <v>518</v>
       </c>
       <c r="E36" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -3300,16 +3605,16 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
-        <v>336</v>
+        <v>373</v>
       </c>
       <c r="D37" t="s">
-        <v>471</v>
+        <v>519</v>
       </c>
       <c r="E37" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -3326,16 +3631,16 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="C38" t="s">
-        <v>337</v>
+        <v>374</v>
       </c>
       <c r="D38" t="s">
-        <v>472</v>
+        <v>520</v>
       </c>
       <c r="E38" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -3352,16 +3657,16 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="C39" t="s">
-        <v>338</v>
+        <v>375</v>
       </c>
       <c r="D39" t="s">
-        <v>473</v>
+        <v>521</v>
       </c>
       <c r="E39" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -3378,16 +3683,16 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="C40" t="s">
-        <v>339</v>
+        <v>376</v>
       </c>
       <c r="D40" t="s">
-        <v>474</v>
+        <v>522</v>
       </c>
       <c r="E40" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -3404,16 +3709,16 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="C41" t="s">
-        <v>340</v>
+        <v>377</v>
       </c>
       <c r="D41" t="s">
-        <v>475</v>
+        <v>523</v>
       </c>
       <c r="E41" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -3430,16 +3735,16 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="C42" t="s">
-        <v>341</v>
+        <v>378</v>
       </c>
       <c r="D42" t="s">
-        <v>476</v>
+        <v>524</v>
       </c>
       <c r="E42" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -3456,16 +3761,16 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="C43" t="s">
-        <v>342</v>
+        <v>379</v>
       </c>
       <c r="D43" t="s">
-        <v>477</v>
+        <v>525</v>
       </c>
       <c r="E43" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -3482,16 +3787,16 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="C44" t="s">
-        <v>343</v>
+        <v>380</v>
       </c>
       <c r="D44" t="s">
-        <v>478</v>
+        <v>526</v>
       </c>
       <c r="E44" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -3508,16 +3813,16 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="C45" t="s">
-        <v>344</v>
+        <v>381</v>
       </c>
       <c r="D45" t="s">
-        <v>479</v>
+        <v>527</v>
       </c>
       <c r="E45" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -3534,16 +3839,16 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="C46" t="s">
-        <v>345</v>
+        <v>382</v>
       </c>
       <c r="D46" t="s">
-        <v>480</v>
+        <v>528</v>
       </c>
       <c r="E46" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -3560,16 +3865,16 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="C47" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="D47" t="s">
-        <v>481</v>
+        <v>529</v>
       </c>
       <c r="E47" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -3586,16 +3891,16 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="C48" t="s">
-        <v>347</v>
+        <v>384</v>
       </c>
       <c r="D48" t="s">
-        <v>482</v>
+        <v>530</v>
       </c>
       <c r="E48" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F48">
         <v>23</v>
@@ -3612,16 +3917,16 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="C49" t="s">
-        <v>348</v>
+        <v>385</v>
       </c>
       <c r="D49" t="s">
-        <v>483</v>
+        <v>531</v>
       </c>
       <c r="E49" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F49">
         <v>23</v>
@@ -3638,16 +3943,16 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="C50" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="D50" t="s">
-        <v>484</v>
+        <v>532</v>
       </c>
       <c r="E50" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F50">
         <v>24</v>
@@ -3664,16 +3969,16 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="C51" t="s">
-        <v>350</v>
+        <v>387</v>
       </c>
       <c r="D51" t="s">
-        <v>485</v>
+        <v>533</v>
       </c>
       <c r="E51" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -3690,16 +3995,16 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="C52" t="s">
-        <v>351</v>
+        <v>388</v>
       </c>
       <c r="D52" t="s">
-        <v>486</v>
+        <v>534</v>
       </c>
       <c r="E52" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F52">
         <v>24</v>
@@ -3716,13 +4021,13 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="C53" t="s">
-        <v>352</v>
+        <v>389</v>
       </c>
       <c r="D53" t="s">
-        <v>487</v>
+        <v>535</v>
       </c>
       <c r="F53">
         <v>24</v>
@@ -3739,16 +4044,16 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="C54" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="D54" t="s">
-        <v>488</v>
+        <v>536</v>
       </c>
       <c r="E54" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -3765,16 +4070,16 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="C55" t="s">
-        <v>354</v>
+        <v>391</v>
       </c>
       <c r="D55" t="s">
-        <v>489</v>
+        <v>537</v>
       </c>
       <c r="E55" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F55">
         <v>25</v>
@@ -3791,16 +4096,16 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="C56" t="s">
-        <v>355</v>
+        <v>392</v>
       </c>
       <c r="D56" t="s">
-        <v>490</v>
+        <v>538</v>
       </c>
       <c r="E56" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F56">
         <v>25</v>
@@ -3817,16 +4122,16 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="C57" t="s">
-        <v>356</v>
+        <v>393</v>
       </c>
       <c r="D57" t="s">
-        <v>491</v>
+        <v>539</v>
       </c>
       <c r="E57" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -3843,16 +4148,16 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="C58" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="D58" t="s">
-        <v>492</v>
+        <v>540</v>
       </c>
       <c r="E58" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -3869,16 +4174,16 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="C59" t="s">
-        <v>358</v>
+        <v>395</v>
       </c>
       <c r="D59" t="s">
-        <v>493</v>
+        <v>541</v>
       </c>
       <c r="E59" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -3895,16 +4200,16 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C60" t="s">
-        <v>359</v>
+        <v>396</v>
       </c>
       <c r="D60" t="s">
-        <v>494</v>
+        <v>542</v>
       </c>
       <c r="E60" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F60">
         <v>27</v>
@@ -3921,16 +4226,16 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="C61" t="s">
-        <v>360</v>
+        <v>397</v>
       </c>
       <c r="D61" t="s">
-        <v>495</v>
+        <v>543</v>
       </c>
       <c r="E61" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F61">
         <v>27</v>
@@ -3947,16 +4252,16 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="C62" t="s">
-        <v>361</v>
+        <v>398</v>
       </c>
       <c r="D62" t="s">
-        <v>496</v>
+        <v>544</v>
       </c>
       <c r="E62" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F62">
         <v>27</v>
@@ -3973,16 +4278,16 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="C63" t="s">
-        <v>362</v>
+        <v>399</v>
       </c>
       <c r="D63" t="s">
-        <v>497</v>
+        <v>545</v>
       </c>
       <c r="E63" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -3999,16 +4304,16 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="C64" t="s">
-        <v>363</v>
+        <v>400</v>
       </c>
       <c r="D64" t="s">
-        <v>498</v>
+        <v>546</v>
       </c>
       <c r="E64" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -4025,16 +4330,16 @@
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="C65" t="s">
-        <v>364</v>
+        <v>401</v>
       </c>
       <c r="D65" t="s">
-        <v>499</v>
+        <v>547</v>
       </c>
       <c r="E65" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -4051,16 +4356,16 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="C66" t="s">
-        <v>365</v>
+        <v>402</v>
       </c>
       <c r="D66" t="s">
-        <v>500</v>
+        <v>548</v>
       </c>
       <c r="E66" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -4077,16 +4382,16 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C67" t="s">
-        <v>363</v>
+        <v>400</v>
       </c>
       <c r="D67" t="s">
-        <v>501</v>
+        <v>549</v>
       </c>
       <c r="E67" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -4103,16 +4408,16 @@
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C68" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="D68" t="s">
-        <v>502</v>
+        <v>550</v>
       </c>
       <c r="E68" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -4129,16 +4434,16 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="C69" t="s">
-        <v>367</v>
+        <v>404</v>
       </c>
       <c r="D69" t="s">
-        <v>503</v>
+        <v>551</v>
       </c>
       <c r="E69" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -4155,16 +4460,16 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="C70" t="s">
-        <v>368</v>
+        <v>405</v>
       </c>
       <c r="D70" t="s">
-        <v>504</v>
+        <v>552</v>
       </c>
       <c r="E70" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -4181,16 +4486,16 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="C71" t="s">
-        <v>369</v>
+        <v>406</v>
       </c>
       <c r="D71" t="s">
-        <v>505</v>
+        <v>553</v>
       </c>
       <c r="E71" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -4207,16 +4512,16 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="C72" t="s">
-        <v>370</v>
+        <v>407</v>
       </c>
       <c r="D72" t="s">
-        <v>506</v>
+        <v>554</v>
       </c>
       <c r="E72" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -4233,16 +4538,16 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="C73" t="s">
-        <v>371</v>
+        <v>408</v>
       </c>
       <c r="D73" t="s">
-        <v>507</v>
+        <v>555</v>
       </c>
       <c r="E73" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -4259,16 +4564,16 @@
         <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="C74" t="s">
-        <v>372</v>
+        <v>409</v>
       </c>
       <c r="D74" t="s">
-        <v>508</v>
+        <v>556</v>
       </c>
       <c r="E74" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -4285,16 +4590,16 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="C75" t="s">
-        <v>373</v>
+        <v>410</v>
       </c>
       <c r="D75" t="s">
-        <v>509</v>
+        <v>557</v>
       </c>
       <c r="E75" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -4311,16 +4616,16 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="C76" t="s">
-        <v>374</v>
+        <v>411</v>
       </c>
       <c r="D76" t="s">
-        <v>510</v>
+        <v>558</v>
       </c>
       <c r="E76" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -4337,16 +4642,16 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="C77" t="s">
-        <v>375</v>
+        <v>412</v>
       </c>
       <c r="D77" t="s">
-        <v>511</v>
+        <v>559</v>
       </c>
       <c r="E77" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -4363,16 +4668,16 @@
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="C78" t="s">
-        <v>376</v>
+        <v>413</v>
       </c>
       <c r="D78" t="s">
-        <v>512</v>
+        <v>560</v>
       </c>
       <c r="E78" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -4389,16 +4694,16 @@
         <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="C79" t="s">
-        <v>377</v>
+        <v>414</v>
       </c>
       <c r="D79" t="s">
-        <v>513</v>
+        <v>561</v>
       </c>
       <c r="E79" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -4415,16 +4720,16 @@
         <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="C80" t="s">
-        <v>378</v>
-      </c>
-      <c r="D80" t="s">
-        <v>514</v>
+        <v>415</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>562</v>
       </c>
       <c r="E80" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -4441,13 +4746,13 @@
         <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="C81" t="s">
-        <v>379</v>
+        <v>416</v>
       </c>
       <c r="D81" t="s">
-        <v>515</v>
+        <v>563</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -4464,13 +4769,13 @@
         <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="C82" t="s">
-        <v>379</v>
+        <v>416</v>
       </c>
       <c r="D82" t="s">
-        <v>516</v>
+        <v>564</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -4487,13 +4792,13 @@
         <v>89</v>
       </c>
       <c r="C83" t="s">
-        <v>379</v>
+        <v>416</v>
       </c>
       <c r="D83" t="s">
-        <v>517</v>
+        <v>565</v>
       </c>
       <c r="E83" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -4510,16 +4815,16 @@
         <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="C84" t="s">
-        <v>380</v>
+        <v>417</v>
       </c>
       <c r="D84" t="s">
-        <v>518</v>
+        <v>566</v>
       </c>
       <c r="E84" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -4536,16 +4841,16 @@
         <v>91</v>
       </c>
       <c r="B85" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="C85" t="s">
-        <v>381</v>
+        <v>418</v>
       </c>
       <c r="D85" t="s">
-        <v>519</v>
+        <v>567</v>
       </c>
       <c r="E85" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F85">
         <v>35</v>
@@ -4562,16 +4867,16 @@
         <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
       <c r="C86" t="s">
-        <v>382</v>
+        <v>419</v>
       </c>
       <c r="D86" t="s">
-        <v>520</v>
+        <v>568</v>
       </c>
       <c r="E86" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -4588,16 +4893,16 @@
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="C87" t="s">
-        <v>383</v>
+        <v>420</v>
       </c>
       <c r="D87" t="s">
-        <v>521</v>
+        <v>569</v>
       </c>
       <c r="E87" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F87">
         <v>36</v>
@@ -4614,16 +4919,16 @@
         <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="C88" t="s">
-        <v>384</v>
+        <v>421</v>
       </c>
       <c r="D88" t="s">
-        <v>522</v>
+        <v>570</v>
       </c>
       <c r="E88" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -4640,16 +4945,16 @@
         <v>95</v>
       </c>
       <c r="B89" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="C89" t="s">
-        <v>385</v>
+        <v>422</v>
       </c>
       <c r="D89" t="s">
-        <v>523</v>
+        <v>571</v>
       </c>
       <c r="E89" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -4666,16 +4971,16 @@
         <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="C90" t="s">
-        <v>386</v>
+        <v>423</v>
       </c>
       <c r="D90" t="s">
-        <v>524</v>
+        <v>572</v>
       </c>
       <c r="E90" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F90">
         <v>37</v>
@@ -4692,16 +4997,16 @@
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="C91" t="s">
-        <v>387</v>
-      </c>
-      <c r="D91" t="s">
-        <v>525</v>
+        <v>424</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>573</v>
       </c>
       <c r="E91" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -4718,16 +5023,16 @@
         <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="C92" t="s">
-        <v>388</v>
+        <v>425</v>
       </c>
       <c r="D92" t="s">
-        <v>526</v>
+        <v>574</v>
       </c>
       <c r="E92" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F92">
         <v>38</v>
@@ -4744,16 +5049,16 @@
         <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="C93" t="s">
-        <v>389</v>
-      </c>
-      <c r="D93" t="s">
-        <v>527</v>
+        <v>426</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>575</v>
       </c>
       <c r="E93" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -4770,16 +5075,16 @@
         <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="C94" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="D94" t="s">
-        <v>528</v>
+        <v>576</v>
       </c>
       <c r="E94" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -4796,16 +5101,16 @@
         <v>101</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="C95" t="s">
-        <v>391</v>
-      </c>
-      <c r="D95" t="s">
-        <v>529</v>
+        <v>428</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>577</v>
       </c>
       <c r="E95" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F95">
         <v>39</v>
@@ -4822,16 +5127,16 @@
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="C96" t="s">
-        <v>392</v>
-      </c>
-      <c r="D96" t="s">
-        <v>530</v>
+        <v>429</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>578</v>
       </c>
       <c r="E96" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -4848,16 +5153,16 @@
         <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="C97" t="s">
-        <v>393</v>
-      </c>
-      <c r="D97" t="s">
-        <v>531</v>
+        <v>430</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>579</v>
       </c>
       <c r="E97" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -4874,16 +5179,16 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="C98" t="s">
-        <v>394</v>
-      </c>
-      <c r="D98" t="s">
-        <v>532</v>
+        <v>431</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>580</v>
       </c>
       <c r="E98" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -4900,16 +5205,16 @@
         <v>105</v>
       </c>
       <c r="B99" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="C99" t="s">
-        <v>395</v>
-      </c>
-      <c r="D99" t="s">
-        <v>533</v>
+        <v>432</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>581</v>
       </c>
       <c r="E99" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -4926,16 +5231,16 @@
         <v>106</v>
       </c>
       <c r="B100" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="C100" t="s">
-        <v>396</v>
-      </c>
-      <c r="D100" t="s">
-        <v>534</v>
+        <v>433</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>582</v>
       </c>
       <c r="E100" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F100">
         <v>41</v>
@@ -4952,16 +5257,16 @@
         <v>107</v>
       </c>
       <c r="B101" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="C101" t="s">
-        <v>397</v>
+        <v>434</v>
       </c>
       <c r="D101" t="s">
-        <v>535</v>
+        <v>583</v>
       </c>
       <c r="E101" t="s">
-        <v>584</v>
+        <v>652</v>
       </c>
       <c r="F101">
         <v>41</v>
@@ -4972,16 +5277,16 @@
         <v>108</v>
       </c>
       <c r="B102" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="C102" t="s">
-        <v>398</v>
-      </c>
-      <c r="D102" t="s">
-        <v>536</v>
+        <v>435</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>584</v>
       </c>
       <c r="E102" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -4998,16 +5303,16 @@
         <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="C103" t="s">
-        <v>399</v>
+        <v>436</v>
       </c>
       <c r="D103" t="s">
-        <v>537</v>
+        <v>585</v>
       </c>
       <c r="E103" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -5024,16 +5329,16 @@
         <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="C104" t="s">
-        <v>400</v>
-      </c>
-      <c r="D104" t="s">
-        <v>538</v>
+        <v>437</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>586</v>
       </c>
       <c r="E104" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F104">
         <v>42</v>
@@ -5050,16 +5355,16 @@
         <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="C105" t="s">
-        <v>401</v>
-      </c>
-      <c r="D105" t="s">
-        <v>539</v>
+        <v>438</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>587</v>
       </c>
       <c r="E105" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -5076,16 +5381,16 @@
         <v>112</v>
       </c>
       <c r="B106" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="C106" t="s">
-        <v>399</v>
+        <v>436</v>
       </c>
       <c r="D106" t="s">
-        <v>540</v>
+        <v>588</v>
       </c>
       <c r="E106" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -5102,16 +5407,16 @@
         <v>113</v>
       </c>
       <c r="B107" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="C107" t="s">
-        <v>402</v>
-      </c>
-      <c r="D107" t="s">
-        <v>541</v>
+        <v>439</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>589</v>
       </c>
       <c r="E107" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F107">
         <v>43</v>
@@ -5128,16 +5433,16 @@
         <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="C108" t="s">
-        <v>403</v>
+        <v>440</v>
       </c>
       <c r="D108" t="s">
-        <v>542</v>
+        <v>590</v>
       </c>
       <c r="E108" t="s">
-        <v>584</v>
+        <v>652</v>
       </c>
       <c r="F108">
         <v>43</v>
@@ -5148,16 +5453,16 @@
         <v>115</v>
       </c>
       <c r="B109" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="C109" t="s">
-        <v>403</v>
+        <v>440</v>
       </c>
       <c r="D109" t="s">
-        <v>543</v>
+        <v>591</v>
       </c>
       <c r="E109" t="s">
-        <v>584</v>
+        <v>652</v>
       </c>
       <c r="F109">
         <v>43</v>
@@ -5168,16 +5473,16 @@
         <v>116</v>
       </c>
       <c r="B110" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="C110" t="s">
-        <v>404</v>
+        <v>441</v>
       </c>
       <c r="D110" t="s">
-        <v>544</v>
+        <v>592</v>
       </c>
       <c r="E110" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -5194,16 +5499,16 @@
         <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="C111" t="s">
-        <v>405</v>
-      </c>
-      <c r="D111" t="s">
-        <v>545</v>
+        <v>442</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>593</v>
       </c>
       <c r="E111" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -5220,16 +5525,16 @@
         <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="C112" t="s">
-        <v>404</v>
+        <v>441</v>
       </c>
       <c r="D112" t="s">
-        <v>546</v>
+        <v>594</v>
       </c>
       <c r="E112" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F112">
         <v>44</v>
@@ -5246,16 +5551,16 @@
         <v>119</v>
       </c>
       <c r="B113" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="C113" t="s">
-        <v>406</v>
+        <v>443</v>
       </c>
       <c r="D113" t="s">
-        <v>547</v>
+        <v>595</v>
       </c>
       <c r="E113" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -5272,16 +5577,16 @@
         <v>120</v>
       </c>
       <c r="B114" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="C114" t="s">
-        <v>407</v>
+        <v>444</v>
       </c>
       <c r="D114" t="s">
-        <v>548</v>
+        <v>596</v>
       </c>
       <c r="E114" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -5298,16 +5603,16 @@
         <v>121</v>
       </c>
       <c r="B115" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="C115" t="s">
-        <v>408</v>
+        <v>445</v>
       </c>
       <c r="D115" t="s">
-        <v>549</v>
+        <v>597</v>
       </c>
       <c r="E115" t="s">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="F115">
         <v>45</v>
@@ -5324,16 +5629,16 @@
         <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="C116" t="s">
-        <v>409</v>
+        <v>446</v>
       </c>
       <c r="D116" t="s">
-        <v>550</v>
+        <v>598</v>
       </c>
       <c r="E116" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -5344,16 +5649,16 @@
         <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="C117" t="s">
-        <v>410</v>
-      </c>
-      <c r="D117" t="s">
-        <v>551</v>
+        <v>447</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>599</v>
       </c>
       <c r="E117" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -5370,16 +5675,16 @@
         <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="C118" t="s">
-        <v>411</v>
+        <v>448</v>
       </c>
       <c r="D118" t="s">
-        <v>552</v>
+        <v>600</v>
       </c>
       <c r="E118" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="H118">
         <v>2</v>
@@ -5390,16 +5695,16 @@
         <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="C119" t="s">
-        <v>412</v>
+        <v>449</v>
       </c>
       <c r="D119" t="s">
-        <v>553</v>
+        <v>601</v>
       </c>
       <c r="E119" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -5416,16 +5721,16 @@
         <v>126</v>
       </c>
       <c r="B120" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="C120" t="s">
-        <v>413</v>
+        <v>450</v>
       </c>
       <c r="D120" t="s">
-        <v>554</v>
+        <v>602</v>
       </c>
       <c r="E120" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -5442,16 +5747,16 @@
         <v>127</v>
       </c>
       <c r="B121" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="C121" t="s">
-        <v>414</v>
-      </c>
-      <c r="D121" t="s">
-        <v>555</v>
+        <v>451</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>603</v>
       </c>
       <c r="E121" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="H121">
         <v>2</v>
@@ -5462,16 +5767,16 @@
         <v>128</v>
       </c>
       <c r="B122" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
       <c r="C122" t="s">
-        <v>415</v>
-      </c>
-      <c r="D122" t="s">
-        <v>556</v>
+        <v>452</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>604</v>
       </c>
       <c r="E122" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -5488,13 +5793,13 @@
         <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="C123" t="s">
-        <v>416</v>
+        <v>453</v>
       </c>
       <c r="D123" t="s">
-        <v>557</v>
+        <v>605</v>
       </c>
       <c r="G123">
         <v>41</v>
@@ -5508,16 +5813,16 @@
         <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="C124" t="s">
-        <v>414</v>
-      </c>
-      <c r="D124" t="s">
-        <v>558</v>
+        <v>451</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>606</v>
       </c>
       <c r="E124" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="H124">
         <v>3</v>
@@ -5528,16 +5833,16 @@
         <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="C125" t="s">
-        <v>414</v>
+        <v>451</v>
       </c>
       <c r="D125" t="s">
-        <v>559</v>
+        <v>607</v>
       </c>
       <c r="E125" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -5548,16 +5853,16 @@
         <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="C126" t="s">
-        <v>417</v>
-      </c>
-      <c r="D126" t="s">
-        <v>560</v>
+        <v>454</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>608</v>
       </c>
       <c r="E126" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="F126">
         <v>5</v>
@@ -5574,16 +5879,16 @@
         <v>133</v>
       </c>
       <c r="B127" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="C127" t="s">
-        <v>418</v>
+        <v>455</v>
       </c>
       <c r="D127" t="s">
-        <v>561</v>
+        <v>609</v>
       </c>
       <c r="E127" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5591,13 +5896,13 @@
         <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="C128" t="s">
-        <v>419</v>
-      </c>
-      <c r="D128" t="s">
-        <v>562</v>
+        <v>456</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>610</v>
       </c>
       <c r="G128">
         <v>26</v>
@@ -5611,16 +5916,16 @@
         <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
       <c r="C129" t="s">
-        <v>420</v>
-      </c>
-      <c r="D129" t="s">
-        <v>563</v>
+        <v>457</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>611</v>
       </c>
       <c r="E129" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -5637,13 +5942,13 @@
         <v>136</v>
       </c>
       <c r="B130" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C130" t="s">
-        <v>421</v>
-      </c>
-      <c r="D130" t="s">
-        <v>564</v>
+        <v>458</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>612</v>
       </c>
       <c r="H130">
         <v>2</v>
@@ -5654,13 +5959,13 @@
         <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>283</v>
+        <v>302</v>
       </c>
       <c r="C131" t="s">
-        <v>421</v>
-      </c>
-      <c r="D131" t="s">
-        <v>565</v>
+        <v>458</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>613</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -5671,13 +5976,16 @@
         <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="C132" t="s">
-        <v>422</v>
-      </c>
-      <c r="D132" t="s">
-        <v>566</v>
+        <v>459</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="E132" t="s">
+        <v>650</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -5694,16 +6002,16 @@
         <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="C133" t="s">
-        <v>423</v>
-      </c>
-      <c r="D133" t="s">
-        <v>567</v>
+        <v>460</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>615</v>
       </c>
       <c r="E133" t="s">
-        <v>585</v>
+        <v>653</v>
       </c>
       <c r="F133">
         <v>7</v>
@@ -5720,16 +6028,16 @@
         <v>140</v>
       </c>
       <c r="B134" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
       <c r="C134" t="s">
-        <v>424</v>
-      </c>
-      <c r="D134" t="s">
-        <v>568</v>
+        <v>461</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>616</v>
       </c>
       <c r="E134" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="H134">
         <v>0.75</v>
@@ -5740,16 +6048,16 @@
         <v>141</v>
       </c>
       <c r="B135" t="s">
-        <v>287</v>
+        <v>306</v>
       </c>
       <c r="C135" t="s">
-        <v>424</v>
-      </c>
-      <c r="D135" t="s">
-        <v>569</v>
+        <v>461</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>617</v>
       </c>
       <c r="E135" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="H135">
         <v>2</v>
@@ -5760,16 +6068,16 @@
         <v>142</v>
       </c>
       <c r="B136" t="s">
-        <v>288</v>
+        <v>307</v>
       </c>
       <c r="C136" t="s">
-        <v>425</v>
-      </c>
-      <c r="D136" t="s">
-        <v>570</v>
+        <v>462</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>618</v>
       </c>
       <c r="E136" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -5786,16 +6094,16 @@
         <v>143</v>
       </c>
       <c r="B137" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="C137" t="s">
-        <v>426</v>
-      </c>
-      <c r="D137" t="s">
-        <v>571</v>
+        <v>463</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>619</v>
       </c>
       <c r="E137" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="F137">
         <v>2</v>
@@ -5812,16 +6120,16 @@
         <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="C138" t="s">
-        <v>427</v>
-      </c>
-      <c r="D138" t="s">
-        <v>572</v>
+        <v>464</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>620</v>
       </c>
       <c r="E138" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="F138">
         <v>3</v>
@@ -5838,16 +6146,16 @@
         <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C139" t="s">
-        <v>428</v>
-      </c>
-      <c r="D139" t="s">
-        <v>573</v>
+        <v>465</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>621</v>
       </c>
       <c r="E139" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="F139">
         <v>4</v>
@@ -5864,16 +6172,16 @@
         <v>146</v>
       </c>
       <c r="B140" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
       <c r="C140" t="s">
-        <v>429</v>
-      </c>
-      <c r="D140" t="s">
-        <v>574</v>
+        <v>466</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>622</v>
       </c>
       <c r="E140" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="H140">
         <v>0.75</v>
@@ -5884,16 +6192,16 @@
         <v>147</v>
       </c>
       <c r="B141" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="C141" t="s">
-        <v>429</v>
-      </c>
-      <c r="D141" t="s">
-        <v>575</v>
+        <v>466</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>623</v>
       </c>
       <c r="E141" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="H141">
         <v>2</v>
@@ -5904,16 +6212,16 @@
         <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="C142" t="s">
-        <v>430</v>
-      </c>
-      <c r="D142" t="s">
-        <v>576</v>
+        <v>467</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="E142" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="F142">
         <v>5</v>
@@ -5930,16 +6238,16 @@
         <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="C143" t="s">
-        <v>431</v>
-      </c>
-      <c r="D143" t="s">
-        <v>577</v>
+        <v>468</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>625</v>
       </c>
       <c r="E143" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="F143">
         <v>6</v>
@@ -5956,16 +6264,16 @@
         <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="C144" t="s">
-        <v>432</v>
-      </c>
-      <c r="D144" t="s">
-        <v>578</v>
+        <v>469</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>626</v>
       </c>
       <c r="E144" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="H144">
         <v>0.75</v>
@@ -5976,16 +6284,16 @@
         <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
       <c r="C145" t="s">
-        <v>432</v>
-      </c>
-      <c r="D145" t="s">
-        <v>579</v>
+        <v>469</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>627</v>
       </c>
       <c r="E145" t="s">
-        <v>586</v>
+        <v>654</v>
       </c>
       <c r="H145">
         <v>2</v>
@@ -5996,16 +6304,22 @@
         <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="C146" t="s">
-        <v>433</v>
-      </c>
-      <c r="D146" t="s">
-        <v>580</v>
+        <v>470</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>628</v>
       </c>
       <c r="E146" t="s">
-        <v>586</v>
+        <v>654</v>
+      </c>
+      <c r="F146">
+        <v>101</v>
+      </c>
+      <c r="G146">
+        <v>24</v>
       </c>
       <c r="H146">
         <v>3</v>
@@ -6016,39 +6330,398 @@
         <v>153</v>
       </c>
       <c r="B147" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="C147" t="s">
-        <v>434</v>
-      </c>
-      <c r="D147" t="s">
-        <v>581</v>
+        <v>471</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>629</v>
       </c>
       <c r="E147" t="s">
-        <v>586</v>
+        <v>650</v>
+      </c>
+      <c r="G147">
+        <v>24</v>
       </c>
       <c r="H147">
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>154</v>
       </c>
       <c r="B148" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="C148" t="s">
-        <v>435</v>
-      </c>
-      <c r="D148" t="s">
-        <v>582</v>
+        <v>472</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>630</v>
       </c>
       <c r="E148" t="s">
-        <v>586</v>
+        <v>653</v>
+      </c>
+      <c r="F148">
+        <v>101</v>
+      </c>
+      <c r="G148">
+        <v>59</v>
       </c>
       <c r="H148">
         <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>157</v>
+      </c>
+      <c r="B149" t="s">
+        <v>322</v>
+      </c>
+      <c r="C149" t="s">
+        <v>474</v>
+      </c>
+      <c r="D149" t="s">
+        <v>633</v>
+      </c>
+      <c r="E149" t="s">
+        <v>653</v>
+      </c>
+      <c r="H149">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>158</v>
+      </c>
+      <c r="B150" t="s">
+        <v>323</v>
+      </c>
+      <c r="C150" t="s">
+        <v>474</v>
+      </c>
+      <c r="D150" t="s">
+        <v>634</v>
+      </c>
+      <c r="E150" t="s">
+        <v>653</v>
+      </c>
+      <c r="H150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>159</v>
+      </c>
+      <c r="B151" t="s">
+        <v>324</v>
+      </c>
+      <c r="C151" t="s">
+        <v>475</v>
+      </c>
+      <c r="D151" t="s">
+        <v>635</v>
+      </c>
+      <c r="E151" t="s">
+        <v>653</v>
+      </c>
+      <c r="F151">
+        <v>102</v>
+      </c>
+      <c r="G151">
+        <v>5</v>
+      </c>
+      <c r="H151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>160</v>
+      </c>
+      <c r="B152" t="s">
+        <v>325</v>
+      </c>
+      <c r="C152" t="s">
+        <v>476</v>
+      </c>
+      <c r="D152" t="s">
+        <v>636</v>
+      </c>
+      <c r="E152" t="s">
+        <v>653</v>
+      </c>
+      <c r="F152">
+        <v>103</v>
+      </c>
+      <c r="G152">
+        <v>5</v>
+      </c>
+      <c r="H152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>155</v>
+      </c>
+      <c r="B153" t="s">
+        <v>320</v>
+      </c>
+      <c r="D153" t="s">
+        <v>631</v>
+      </c>
+      <c r="E153" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>156</v>
+      </c>
+      <c r="B154" t="s">
+        <v>321</v>
+      </c>
+      <c r="C154" t="s">
+        <v>473</v>
+      </c>
+      <c r="D154" t="s">
+        <v>632</v>
+      </c>
+      <c r="E154" t="s">
+        <v>650</v>
+      </c>
+      <c r="G154">
+        <v>24</v>
+      </c>
+      <c r="H154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>161</v>
+      </c>
+      <c r="B155" t="s">
+        <v>326</v>
+      </c>
+      <c r="D155" t="s">
+        <v>637</v>
+      </c>
+      <c r="E155" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>162</v>
+      </c>
+      <c r="B156" t="s">
+        <v>327</v>
+      </c>
+      <c r="D156" t="s">
+        <v>638</v>
+      </c>
+      <c r="E156" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>163</v>
+      </c>
+      <c r="B157" t="s">
+        <v>655</v>
+      </c>
+      <c r="C157" t="s">
+        <v>477</v>
+      </c>
+      <c r="D157" t="s">
+        <v>639</v>
+      </c>
+      <c r="E157" t="s">
+        <v>650</v>
+      </c>
+      <c r="G157">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>164</v>
+      </c>
+      <c r="B158" t="s">
+        <v>328</v>
+      </c>
+      <c r="C158" t="s">
+        <v>478</v>
+      </c>
+      <c r="D158" t="s">
+        <v>640</v>
+      </c>
+      <c r="E158" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>165</v>
+      </c>
+      <c r="B159" t="s">
+        <v>329</v>
+      </c>
+      <c r="D159" t="s">
+        <v>641</v>
+      </c>
+      <c r="E159" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>166</v>
+      </c>
+      <c r="B160" t="s">
+        <v>330</v>
+      </c>
+      <c r="C160" t="s">
+        <v>479</v>
+      </c>
+      <c r="D160" t="s">
+        <v>642</v>
+      </c>
+      <c r="E160" t="s">
+        <v>650</v>
+      </c>
+      <c r="G160">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>167</v>
+      </c>
+      <c r="B161" t="s">
+        <v>331</v>
+      </c>
+      <c r="C161" t="s">
+        <v>480</v>
+      </c>
+      <c r="D161" t="s">
+        <v>643</v>
+      </c>
+      <c r="E161" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>168</v>
+      </c>
+      <c r="B162" t="s">
+        <v>332</v>
+      </c>
+      <c r="C162" t="s">
+        <v>480</v>
+      </c>
+      <c r="D162" t="s">
+        <v>644</v>
+      </c>
+      <c r="E162" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>169</v>
+      </c>
+      <c r="B163" t="s">
+        <v>333</v>
+      </c>
+      <c r="C163" t="s">
+        <v>481</v>
+      </c>
+      <c r="D163" t="s">
+        <v>645</v>
+      </c>
+      <c r="E163" t="s">
+        <v>650</v>
+      </c>
+      <c r="G163">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>170</v>
+      </c>
+      <c r="B164" t="s">
+        <v>334</v>
+      </c>
+      <c r="C164" t="s">
+        <v>482</v>
+      </c>
+      <c r="D164" t="s">
+        <v>646</v>
+      </c>
+      <c r="E164" t="s">
+        <v>650</v>
+      </c>
+      <c r="G164">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>171</v>
+      </c>
+      <c r="B165" t="s">
+        <v>335</v>
+      </c>
+      <c r="D165" t="s">
+        <v>647</v>
+      </c>
+      <c r="E165" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>172</v>
+      </c>
+      <c r="B166" t="s">
+        <v>336</v>
+      </c>
+      <c r="D166" t="s">
+        <v>648</v>
+      </c>
+      <c r="E166" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>173</v>
+      </c>
+      <c r="B167" t="s">
+        <v>337</v>
+      </c>
+      <c r="C167" t="s">
+        <v>483</v>
+      </c>
+      <c r="D167" t="s">
+        <v>649</v>
+      </c>
+      <c r="E167" t="s">
+        <v>650</v>
+      </c>
+      <c r="G167">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add latent code loading
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41571AD4-D234-4FF0-A3D4-C4FF0B4F1A69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE2CA02-A834-4049-A7B6-F2C5AB76D3D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="657">
   <si>
     <t>ephysFN</t>
   </si>
@@ -2246,6 +2246,9 @@
   </si>
   <si>
     <t>200210_Beto_generate_integrated(2)</t>
+  </si>
+  <si>
+    <t>Optim_tuning</t>
   </si>
 </sst>
 </file>
@@ -2652,8 +2655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F147" sqref="F147"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6362,10 +6365,10 @@
         <v>630</v>
       </c>
       <c r="E148" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="F148">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="G148">
         <v>59</v>
@@ -6388,7 +6391,7 @@
         <v>633</v>
       </c>
       <c r="E149" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="H149">
         <v>0.75</v>
@@ -6408,7 +6411,7 @@
         <v>634</v>
       </c>
       <c r="E150" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="H150">
         <v>2</v>
@@ -6428,10 +6431,10 @@
         <v>635</v>
       </c>
       <c r="E151" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="F151">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="G151">
         <v>5</v>
@@ -6454,10 +6457,10 @@
         <v>636</v>
       </c>
       <c r="E152" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="F152">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="G152">
         <v>5</v>

</xml_diff>

<commit_message>
add codes for gradient visualization
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE2CA02-A834-4049-A7B6-F2C5AB76D3D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26282F2-BF27-4FA8-9319-ACBB59FFE559}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="676">
   <si>
     <t>ephysFN</t>
   </si>
@@ -487,24 +487,24 @@
     <t>Beto-03032020-006</t>
   </si>
   <si>
+    <t>Beto-09032020-001</t>
+  </si>
+  <si>
+    <t>Beto-09032020-002</t>
+  </si>
+  <si>
+    <t>Beto-09032020-004</t>
+  </si>
+  <si>
+    <t>Beto-09032020-005</t>
+  </si>
+  <si>
     <t>Beto-06032020-001</t>
   </si>
   <si>
     <t>Beto-06032020-004</t>
   </si>
   <si>
-    <t>Beto-09032020-001</t>
-  </si>
-  <si>
-    <t>Beto-09032020-002</t>
-  </si>
-  <si>
-    <t>Beto-09032020-004</t>
-  </si>
-  <si>
-    <t>Beto-09032020-005</t>
-  </si>
-  <si>
     <t>Beto-10022020-001</t>
   </si>
   <si>
@@ -544,6 +544,21 @@
     <t>Beto-20022020-003</t>
   </si>
   <si>
+    <t>Beto-11032020-001</t>
+  </si>
+  <si>
+    <t>Beto-11032020-002</t>
+  </si>
+  <si>
+    <t>Beto-11032020-003</t>
+  </si>
+  <si>
+    <t>Beto-11032020-004</t>
+  </si>
+  <si>
+    <t>Beto-11032020-005</t>
+  </si>
+  <si>
     <t>191002_Beto_selectivity_basic(1)</t>
   </si>
   <si>
@@ -982,30 +997,33 @@
     <t>200303_Beto_generate_integrated(6)</t>
   </si>
   <si>
+    <t>200309_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200309_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200309_Beto_generate_integrated(3)</t>
+  </si>
+  <si>
+    <t>200309_Beto_generate_integrated(4)</t>
+  </si>
+  <si>
     <t>200306_Beto_rfMapper_basic</t>
   </si>
   <si>
     <t>200306_Beto_generate_integrated(3)</t>
   </si>
   <si>
-    <t>200309_Beto_rfMapper_basic</t>
-  </si>
-  <si>
-    <t>200309_Beto_rfMapper_basic(1)</t>
-  </si>
-  <si>
-    <t>200309_Beto_generate_integrated(3)</t>
-  </si>
-  <si>
-    <t>200309_Beto_generate_integrated(4)</t>
-  </si>
-  <si>
     <t>200210_Beto_rfMapper_basic</t>
   </si>
   <si>
     <t>200210_Beto_rfMapper_basic(1)</t>
   </si>
   <si>
+    <t>200210_Beto_generate_integrated(2)</t>
+  </si>
+  <si>
     <t>200210_Beto_generate_integrated(6)</t>
   </si>
   <si>
@@ -1036,6 +1054,21 @@
     <t>200220_Beto_generate_integrated</t>
   </si>
   <si>
+    <t>200311_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200311_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200311_Beto_generate_integrated</t>
+  </si>
+  <si>
+    <t>200311_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200311_Beto_generate_integrated(2)</t>
+  </si>
+  <si>
     <t>\\storage1.ris.wustl.edu\crponce\Active\Stimuli\2019-Selectivity\2019-10-02a-beto</t>
   </si>
   <si>
@@ -1441,18 +1474,18 @@
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-03-Beto-03\2020-03-03-13-36-50</t>
   </si>
   <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-09-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-09-Beto-01\2020-03-09-14-58-23</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-09-Beto-02\2020-03-09-15-44-10</t>
+  </si>
+  <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-06-Beto-01\2020-03-06-12-11-33</t>
   </si>
   <si>
-    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-09-Beto</t>
-  </si>
-  <si>
-    <t>N:\Stimuli\2019-12-Evolutions\2020-03-09-Beto-01\2020-03-09-14-58-23</t>
-  </si>
-  <si>
-    <t>N:\Stimuli\2019-12-Evolutions\2020-03-09-Beto-02\2020-03-09-15-44-10</t>
-  </si>
-  <si>
     <t>Stimuli\2019-12-Evolutions\2020-02-10-Beto-01\2020-02-10-14-18-32</t>
   </si>
   <si>
@@ -1472,6 +1505,18 @@
   </si>
   <si>
     <t>Stimuli\2019-12-Evolutions\2020-02-20-Beto-01\2020-02-20-10-29-18</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-11-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-11-Beto-01\2020-03-11-13-16-23</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-11-Beto-02\2020-03-11-14-18-56</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-11-Beto-03\2020-03-11-14-52-05</t>
   </si>
   <si>
     <t>Derived from PCs of Ch 29 evolution 191002. 373 images {11*11 in PC2,PC3; PC49 PC50; RND RND space respectively, +10 last gen}</t>
@@ -2081,20 +2126,6 @@
 Completed</t>
   </si>
   <si>
-    <t>Start 1147 rf map.
-Maybe try su vs hash in 24
-4 blocks complete at 1159</t>
-  </si>
-  <si>
-    <t>Generate integrated start at 12:11
-24 [-0.5, 1.5] 3 1 CMAES
-24 [-0.5, 1.5] 3 2 CMAES
-Reward at 60
-Block 7, 1 is starting to climb!!
-Block 29, still climbing
-Stop at 1:16</t>
-  </si>
-  <si>
     <t>001 RF mapping 14:29 started
 Takes a while to get Beto started.
 -1.5:0.5:1.5 0.75deg
@@ -2124,6 +2155,20 @@
 Make it to 30 gens
 Completed
 Completed</t>
+  </si>
+  <si>
+    <t>Start 1147 rf map.
+Maybe try su vs hash in 24
+4 blocks complete at 1159</t>
+  </si>
+  <si>
+    <t>Generate integrated start at 12:11
+24 [-0.5, 1.5] 3 1 CMAES
+24 [-0.5, 1.5] 3 2 CMAES
+Reward at 60
+Block 7, 1 is starting to climb!!
+Block 29, still climbing
+Stop at 1:16</t>
   </si>
   <si>
     <t>001 RFMapping  13:35 starts
@@ -2230,22 +2275,84 @@
 Stopped at 11:26, 28 blocks complete</t>
   </si>
   <si>
+    <t>001 starts 12:49
+RFMapping  -8:2:8  2 deg,
+2cv
+Completed</t>
+  </si>
+  <si>
+    <t>002  starts
+6mins
+RFMapping  -1.5:.5:1.5 0.75 deg,
+Completed</t>
+  </si>
+  <si>
+    <t>003 starts  13:16
+IT channel
+30 [-0.6 1] 3 1 CMAES
+30 [-0.6 1] 3 1 ZOHA_Sphere_lr
+30 is a Really Hashy unit
+See what happens
+Decrease the convergence rate, decay from 50 to 7.33 deg at 100 generations instead of 50 generations (Slower decay facilitate exploration ~ 40 gens. )
+ZOHA_Sphere is doing really well! Outperform CMAES early on.
+At about gen 25 the 2 evolution crossed and seems CMAES starts to get more spike esp. later sustained spikes. (probablu the norm is higher )
+At gen 30 the exploration is around 28.5 deg and the mean response is higher than ZOHA
+Sigma is 2.66, 2.33
+Exploration mu is 28
+Maybe we still decay too fast?
+Or we really needs a high norm to get the neuron interested.
+At generation 36,
+Sigma = 2.36
+Spherical Exploration range = 25.9 deg 
+Spherical's step size is too small at this point, we are inferior
+Should use inverse function decay instead of exponential decay?
+Step 37
+Sigma 2.35
+Sphere degree 23.9
+ZOHA_Sphere_lr seems to be worse at after evolving for a while,
+Recorded the Matlab output! See we can reconstruct the sample diversity curve post hoc.
+Random thoughts:
+What's neuronal noise? How can that help or hinder evolution. Can we think about Hash as a weighted sum of a bunch of neurons with similar but different selectivity?
+45 gens for 58mins!
+Super Informative!
+Completed</t>
+  </si>
+  <si>
+    <t>004 starts  14:19
+30 [-0.6 1] 3 1 CMAES
+30 [-0.6 1] 3 1 ZOHA_Sphere_lr
+Exactly same as 003, but just change the decay rate of ZOHA_Sphere_lr to be linear instead of exponential, see slower decay will facilitate exploration at around 20-40 gens.
+However, neither CMA nor ZOHA evolves ~ 18 gens, not that informative.
+Actually the step size should be a function of evolving score! Not a function of generations. As many generations passed but score doesn't change much then you shouldn't tune your step size, you have to keep trying and moving.
+Completed, not very informative</t>
+  </si>
+  <si>
+    <t>005 starts 14:52
+20 [-0.6 1] 3 1 CMAES
+20 [-0.6 1] 3 1 ZOHA_Sphere_lr
+Linear decay from 50 to 7.33 in 100 generations, facilitates exploration.
+Finally try a unit with more signal. (PSTH looks super healthy! Low baseline high response.)
+(Eye signal lose again. Have to recalibrate from time to time. )
+In gen 8, gen 9 the scores of 2 optimizers goes up together. Quite correlated~ Seems promissing
+Add 100mL to finish this up.
+Around gen 12 CMA starts to look better than ZOHA, not sure why. Have to look deeper into both.
+Is that true that linear exploration is easier to memorize the evolved features than the Spherical one.
+Completed, quite informative</t>
+  </si>
+  <si>
+    <t>Manifold</t>
+  </si>
+  <si>
+    <t>Freeview</t>
+  </si>
+  <si>
+    <t>Optimizer_cmp</t>
+  </si>
+  <si>
     <t>SUHash</t>
   </si>
   <si>
-    <t>Manifold</t>
-  </si>
-  <si>
-    <t>Freeview</t>
-  </si>
-  <si>
-    <t>Optimizer_cmp</t>
-  </si>
-  <si>
     <t>RedDim_Evol</t>
-  </si>
-  <si>
-    <t>200210_Beto_generate_integrated(2)</t>
   </si>
   <si>
     <t>Optim_tuning</t>
@@ -2307,13 +2414,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2653,18 +2757,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H167"/>
+  <dimension ref="A1:H172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="F154" sqref="F154"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="F173" sqref="F173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" customWidth="1"/>
-    <col min="4" max="4" width="81.7109375" customWidth="1"/>
+    <col min="4" max="4" width="100.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2698,16 +2800,16 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="D2" t="s">
-        <v>484</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2724,16 +2826,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="D3" t="s">
-        <v>485</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2750,16 +2852,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="D4" t="s">
-        <v>486</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -2776,16 +2878,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="D5" t="s">
-        <v>487</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2802,16 +2904,16 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="D6" t="s">
-        <v>488</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2828,16 +2930,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="D7" t="s">
-        <v>489</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -2854,16 +2956,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="D8" t="s">
-        <v>490</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2880,16 +2982,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="D9" t="s">
-        <v>491</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2906,16 +3008,16 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="D10" t="s">
-        <v>492</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2932,16 +3034,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c r="D11" t="s">
-        <v>493</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -2958,16 +3060,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="D12" t="s">
-        <v>494</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -2984,16 +3086,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="D13" t="s">
-        <v>495</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3010,16 +3112,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="D14" t="s">
-        <v>496</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -3036,16 +3138,16 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="D15" t="s">
-        <v>497</v>
+        <v>512</v>
       </c>
       <c r="E15" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -3062,16 +3164,16 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="D16" t="s">
-        <v>498</v>
+        <v>513</v>
       </c>
       <c r="E16" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -3088,16 +3190,16 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="D17" t="s">
-        <v>499</v>
+        <v>514</v>
       </c>
       <c r="E17" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -3114,16 +3216,16 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="D18" t="s">
-        <v>500</v>
+        <v>515</v>
       </c>
       <c r="E18" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -3140,16 +3242,16 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="D19" t="s">
-        <v>501</v>
+        <v>516</v>
       </c>
       <c r="E19" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -3166,16 +3268,16 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C20" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="D20" t="s">
-        <v>502</v>
+        <v>517</v>
       </c>
       <c r="E20" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3192,16 +3294,16 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="D21" t="s">
-        <v>503</v>
+        <v>518</v>
       </c>
       <c r="E21" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3218,16 +3320,16 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="D22" t="s">
-        <v>504</v>
+        <v>519</v>
       </c>
       <c r="E22" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -3244,16 +3346,16 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C23" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
       <c r="D23" t="s">
-        <v>505</v>
+        <v>520</v>
       </c>
       <c r="E23" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -3270,16 +3372,16 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C24" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="D24" t="s">
-        <v>506</v>
+        <v>521</v>
       </c>
       <c r="E24" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -3296,16 +3398,16 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
       <c r="D25" t="s">
-        <v>507</v>
+        <v>522</v>
       </c>
       <c r="E25" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -3322,16 +3424,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="D26" t="s">
-        <v>508</v>
+        <v>523</v>
       </c>
       <c r="E26" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -3348,16 +3450,16 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C27" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="D27" t="s">
-        <v>509</v>
+        <v>524</v>
       </c>
       <c r="E27" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -3374,16 +3476,16 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="D28" t="s">
-        <v>510</v>
+        <v>525</v>
       </c>
       <c r="E28" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -3400,16 +3502,16 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C29" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="D29" t="s">
-        <v>511</v>
+        <v>526</v>
       </c>
       <c r="E29" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -3426,16 +3528,16 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="D30" t="s">
-        <v>512</v>
+        <v>527</v>
       </c>
       <c r="E30" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -3452,16 +3554,16 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="D31" t="s">
-        <v>513</v>
+        <v>528</v>
       </c>
       <c r="E31" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -3478,16 +3580,16 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="D32" t="s">
-        <v>514</v>
+        <v>529</v>
       </c>
       <c r="E32" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -3504,16 +3606,16 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C33" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="D33" t="s">
-        <v>515</v>
+        <v>530</v>
       </c>
       <c r="E33" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -3530,16 +3632,16 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C34" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="D34" t="s">
-        <v>516</v>
+        <v>531</v>
       </c>
       <c r="E34" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -3556,16 +3658,16 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="D35" t="s">
-        <v>517</v>
+        <v>532</v>
       </c>
       <c r="E35" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -3582,16 +3684,16 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C36" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="D36" t="s">
-        <v>518</v>
+        <v>533</v>
       </c>
       <c r="E36" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -3608,16 +3710,16 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C37" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="D37" t="s">
-        <v>519</v>
+        <v>534</v>
       </c>
       <c r="E37" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -3634,16 +3736,16 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C38" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="D38" t="s">
-        <v>520</v>
+        <v>535</v>
       </c>
       <c r="E38" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -3660,16 +3762,16 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C39" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="D39" t="s">
-        <v>521</v>
+        <v>536</v>
       </c>
       <c r="E39" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -3686,16 +3788,16 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C40" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="D40" t="s">
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="E40" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -3712,16 +3814,16 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C41" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="D41" t="s">
-        <v>523</v>
+        <v>538</v>
       </c>
       <c r="E41" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -3738,16 +3840,16 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C42" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="D42" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="E42" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -3764,16 +3866,16 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C43" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="D43" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
       <c r="E43" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -3790,16 +3892,16 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C44" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="D44" t="s">
-        <v>526</v>
+        <v>541</v>
       </c>
       <c r="E44" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -3816,16 +3918,16 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C45" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="D45" t="s">
-        <v>527</v>
+        <v>542</v>
       </c>
       <c r="E45" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -3842,16 +3944,16 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C46" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="D46" t="s">
-        <v>528</v>
+        <v>543</v>
       </c>
       <c r="E46" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -3868,16 +3970,16 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C47" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="D47" t="s">
-        <v>529</v>
+        <v>544</v>
       </c>
       <c r="E47" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -3894,16 +3996,16 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C48" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="D48" t="s">
-        <v>530</v>
+        <v>545</v>
       </c>
       <c r="E48" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F48">
         <v>23</v>
@@ -3920,16 +4022,16 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C49" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="D49" t="s">
-        <v>531</v>
+        <v>546</v>
       </c>
       <c r="E49" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F49">
         <v>23</v>
@@ -3946,16 +4048,16 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C50" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="D50" t="s">
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="E50" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F50">
         <v>24</v>
@@ -3972,16 +4074,16 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C51" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="D51" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="E51" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -3998,16 +4100,16 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C52" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="D52" t="s">
-        <v>534</v>
+        <v>549</v>
       </c>
       <c r="E52" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F52">
         <v>24</v>
@@ -4024,13 +4126,13 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C53" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="D53" t="s">
-        <v>535</v>
+        <v>550</v>
       </c>
       <c r="F53">
         <v>24</v>
@@ -4047,16 +4149,16 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C54" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="D54" t="s">
-        <v>536</v>
+        <v>551</v>
       </c>
       <c r="E54" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -4073,16 +4175,16 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C55" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="D55" t="s">
-        <v>537</v>
+        <v>552</v>
       </c>
       <c r="E55" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F55">
         <v>25</v>
@@ -4099,16 +4201,16 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C56" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="D56" t="s">
-        <v>538</v>
+        <v>553</v>
       </c>
       <c r="E56" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F56">
         <v>25</v>
@@ -4125,16 +4227,16 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C57" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="D57" t="s">
-        <v>539</v>
+        <v>554</v>
       </c>
       <c r="E57" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -4151,16 +4253,16 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C58" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="D58" t="s">
-        <v>540</v>
+        <v>555</v>
       </c>
       <c r="E58" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -4177,16 +4279,16 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C59" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="D59" t="s">
-        <v>541</v>
+        <v>556</v>
       </c>
       <c r="E59" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -4203,16 +4305,16 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C60" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="D60" t="s">
-        <v>542</v>
+        <v>557</v>
       </c>
       <c r="E60" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F60">
         <v>27</v>
@@ -4229,16 +4331,16 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C61" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="D61" t="s">
-        <v>543</v>
+        <v>558</v>
       </c>
       <c r="E61" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F61">
         <v>27</v>
@@ -4255,16 +4357,16 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C62" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="D62" t="s">
-        <v>544</v>
+        <v>559</v>
       </c>
       <c r="E62" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F62">
         <v>27</v>
@@ -4281,16 +4383,16 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C63" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="D63" t="s">
-        <v>545</v>
+        <v>560</v>
       </c>
       <c r="E63" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -4307,16 +4409,16 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C64" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="D64" t="s">
-        <v>546</v>
+        <v>561</v>
       </c>
       <c r="E64" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -4333,16 +4435,16 @@
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C65" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="D65" t="s">
-        <v>547</v>
+        <v>562</v>
       </c>
       <c r="E65" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -4359,16 +4461,16 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="D66" t="s">
-        <v>548</v>
+        <v>563</v>
       </c>
       <c r="E66" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -4385,16 +4487,16 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C67" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="D67" t="s">
-        <v>549</v>
+        <v>564</v>
       </c>
       <c r="E67" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -4411,16 +4513,16 @@
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C68" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="D68" t="s">
-        <v>550</v>
+        <v>565</v>
       </c>
       <c r="E68" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -4437,16 +4539,16 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C69" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="D69" t="s">
-        <v>551</v>
+        <v>566</v>
       </c>
       <c r="E69" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -4463,16 +4565,16 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C70" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="D70" t="s">
-        <v>552</v>
+        <v>567</v>
       </c>
       <c r="E70" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -4489,16 +4591,16 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C71" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="D71" t="s">
-        <v>553</v>
+        <v>568</v>
       </c>
       <c r="E71" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -4515,16 +4617,16 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C72" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="D72" t="s">
-        <v>554</v>
+        <v>569</v>
       </c>
       <c r="E72" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -4541,16 +4643,16 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C73" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
       <c r="D73" t="s">
-        <v>555</v>
+        <v>570</v>
       </c>
       <c r="E73" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -4567,16 +4669,16 @@
         <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C74" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="D74" t="s">
-        <v>556</v>
+        <v>571</v>
       </c>
       <c r="E74" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -4593,16 +4695,16 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="C75" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="D75" t="s">
-        <v>557</v>
+        <v>572</v>
       </c>
       <c r="E75" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -4619,16 +4721,16 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C76" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="D76" t="s">
-        <v>558</v>
+        <v>573</v>
       </c>
       <c r="E76" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -4645,16 +4747,16 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C77" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="D77" t="s">
-        <v>559</v>
+        <v>574</v>
       </c>
       <c r="E77" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -4671,16 +4773,16 @@
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C78" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="D78" t="s">
-        <v>560</v>
+        <v>575</v>
       </c>
       <c r="E78" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -4697,16 +4799,16 @@
         <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C79" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="D79" t="s">
-        <v>561</v>
+        <v>576</v>
       </c>
       <c r="E79" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -4723,16 +4825,16 @@
         <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C80" t="s">
-        <v>415</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>562</v>
+        <v>426</v>
+      </c>
+      <c r="D80" t="s">
+        <v>577</v>
       </c>
       <c r="E80" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -4749,13 +4851,13 @@
         <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C81" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="D81" t="s">
-        <v>563</v>
+        <v>578</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -4772,13 +4874,13 @@
         <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C82" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="D82" t="s">
-        <v>564</v>
+        <v>579</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -4795,13 +4897,13 @@
         <v>89</v>
       </c>
       <c r="C83" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="D83" t="s">
-        <v>565</v>
+        <v>580</v>
       </c>
       <c r="E83" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -4818,16 +4920,16 @@
         <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C84" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="D84" t="s">
-        <v>566</v>
+        <v>581</v>
       </c>
       <c r="E84" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -4844,16 +4946,16 @@
         <v>91</v>
       </c>
       <c r="B85" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C85" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D85" t="s">
-        <v>567</v>
+        <v>582</v>
       </c>
       <c r="E85" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F85">
         <v>35</v>
@@ -4870,16 +4972,16 @@
         <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C86" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="D86" t="s">
-        <v>568</v>
+        <v>583</v>
       </c>
       <c r="E86" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -4896,16 +4998,16 @@
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C87" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D87" t="s">
-        <v>569</v>
+        <v>584</v>
       </c>
       <c r="E87" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F87">
         <v>36</v>
@@ -4922,16 +5024,16 @@
         <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C88" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D88" t="s">
-        <v>570</v>
+        <v>585</v>
       </c>
       <c r="E88" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -4948,16 +5050,16 @@
         <v>95</v>
       </c>
       <c r="B89" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C89" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="D89" t="s">
-        <v>571</v>
+        <v>586</v>
       </c>
       <c r="E89" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -4974,16 +5076,16 @@
         <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C90" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="D90" t="s">
-        <v>572</v>
+        <v>587</v>
       </c>
       <c r="E90" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F90">
         <v>37</v>
@@ -5000,16 +5102,16 @@
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C91" t="s">
-        <v>424</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>573</v>
+        <v>435</v>
+      </c>
+      <c r="D91" t="s">
+        <v>588</v>
       </c>
       <c r="E91" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -5026,16 +5128,16 @@
         <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C92" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="D92" t="s">
-        <v>574</v>
+        <v>589</v>
       </c>
       <c r="E92" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F92">
         <v>38</v>
@@ -5052,16 +5154,16 @@
         <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C93" t="s">
-        <v>426</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>575</v>
+        <v>437</v>
+      </c>
+      <c r="D93" t="s">
+        <v>590</v>
       </c>
       <c r="E93" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -5078,16 +5180,16 @@
         <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C94" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="D94" t="s">
-        <v>576</v>
+        <v>591</v>
       </c>
       <c r="E94" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -5104,16 +5206,16 @@
         <v>101</v>
       </c>
       <c r="B95" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C95" t="s">
-        <v>428</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>577</v>
+        <v>439</v>
+      </c>
+      <c r="D95" t="s">
+        <v>592</v>
       </c>
       <c r="E95" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F95">
         <v>39</v>
@@ -5130,16 +5232,16 @@
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C96" t="s">
-        <v>429</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>578</v>
+        <v>440</v>
+      </c>
+      <c r="D96" t="s">
+        <v>593</v>
       </c>
       <c r="E96" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -5156,16 +5258,16 @@
         <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C97" t="s">
-        <v>430</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>579</v>
+        <v>441</v>
+      </c>
+      <c r="D97" t="s">
+        <v>594</v>
       </c>
       <c r="E97" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -5182,16 +5284,16 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C98" t="s">
-        <v>431</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>580</v>
+        <v>442</v>
+      </c>
+      <c r="D98" t="s">
+        <v>595</v>
       </c>
       <c r="E98" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -5208,16 +5310,16 @@
         <v>105</v>
       </c>
       <c r="B99" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C99" t="s">
-        <v>432</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>581</v>
+        <v>443</v>
+      </c>
+      <c r="D99" t="s">
+        <v>596</v>
       </c>
       <c r="E99" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -5234,16 +5336,16 @@
         <v>106</v>
       </c>
       <c r="B100" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C100" t="s">
-        <v>433</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>582</v>
+        <v>444</v>
+      </c>
+      <c r="D100" t="s">
+        <v>597</v>
       </c>
       <c r="E100" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F100">
         <v>41</v>
@@ -5260,16 +5362,16 @@
         <v>107</v>
       </c>
       <c r="B101" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C101" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="D101" t="s">
-        <v>583</v>
+        <v>598</v>
       </c>
       <c r="E101" t="s">
-        <v>652</v>
+        <v>671</v>
       </c>
       <c r="F101">
         <v>41</v>
@@ -5280,16 +5382,16 @@
         <v>108</v>
       </c>
       <c r="B102" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C102" t="s">
-        <v>435</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>584</v>
+        <v>446</v>
+      </c>
+      <c r="D102" t="s">
+        <v>599</v>
       </c>
       <c r="E102" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -5306,16 +5408,16 @@
         <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C103" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="D103" t="s">
-        <v>585</v>
+        <v>600</v>
       </c>
       <c r="E103" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -5332,16 +5434,16 @@
         <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="C104" t="s">
-        <v>437</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>586</v>
+        <v>448</v>
+      </c>
+      <c r="D104" t="s">
+        <v>601</v>
       </c>
       <c r="E104" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F104">
         <v>42</v>
@@ -5358,16 +5460,16 @@
         <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C105" t="s">
-        <v>438</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>587</v>
+        <v>449</v>
+      </c>
+      <c r="D105" t="s">
+        <v>602</v>
       </c>
       <c r="E105" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -5384,16 +5486,16 @@
         <v>112</v>
       </c>
       <c r="B106" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C106" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="D106" t="s">
-        <v>588</v>
+        <v>603</v>
       </c>
       <c r="E106" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -5410,16 +5512,16 @@
         <v>113</v>
       </c>
       <c r="B107" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="C107" t="s">
-        <v>439</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>589</v>
+        <v>450</v>
+      </c>
+      <c r="D107" t="s">
+        <v>604</v>
       </c>
       <c r="E107" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F107">
         <v>43</v>
@@ -5436,16 +5538,16 @@
         <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C108" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="D108" t="s">
-        <v>590</v>
+        <v>605</v>
       </c>
       <c r="E108" t="s">
-        <v>652</v>
+        <v>671</v>
       </c>
       <c r="F108">
         <v>43</v>
@@ -5456,16 +5558,16 @@
         <v>115</v>
       </c>
       <c r="B109" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C109" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="D109" t="s">
-        <v>591</v>
+        <v>606</v>
       </c>
       <c r="E109" t="s">
-        <v>652</v>
+        <v>671</v>
       </c>
       <c r="F109">
         <v>43</v>
@@ -5476,16 +5578,16 @@
         <v>116</v>
       </c>
       <c r="B110" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C110" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="D110" t="s">
-        <v>592</v>
+        <v>607</v>
       </c>
       <c r="E110" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -5502,16 +5604,16 @@
         <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="C111" t="s">
-        <v>442</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>593</v>
+        <v>453</v>
+      </c>
+      <c r="D111" t="s">
+        <v>608</v>
       </c>
       <c r="E111" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -5528,16 +5630,16 @@
         <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C112" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="D112" t="s">
-        <v>594</v>
+        <v>609</v>
       </c>
       <c r="E112" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F112">
         <v>44</v>
@@ -5554,16 +5656,16 @@
         <v>119</v>
       </c>
       <c r="B113" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C113" t="s">
-        <v>443</v>
+        <v>454</v>
       </c>
       <c r="D113" t="s">
-        <v>595</v>
+        <v>610</v>
       </c>
       <c r="E113" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -5580,16 +5682,16 @@
         <v>120</v>
       </c>
       <c r="B114" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C114" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
       <c r="D114" t="s">
-        <v>596</v>
+        <v>611</v>
       </c>
       <c r="E114" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -5606,16 +5708,16 @@
         <v>121</v>
       </c>
       <c r="B115" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C115" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="D115" t="s">
-        <v>597</v>
+        <v>612</v>
       </c>
       <c r="E115" t="s">
-        <v>651</v>
+        <v>670</v>
       </c>
       <c r="F115">
         <v>45</v>
@@ -5632,16 +5734,16 @@
         <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C116" t="s">
-        <v>446</v>
+        <v>457</v>
       </c>
       <c r="D116" t="s">
-        <v>598</v>
+        <v>613</v>
       </c>
       <c r="E116" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -5652,16 +5754,16 @@
         <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C117" t="s">
-        <v>447</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>599</v>
+        <v>458</v>
+      </c>
+      <c r="D117" t="s">
+        <v>614</v>
       </c>
       <c r="E117" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -5678,16 +5780,16 @@
         <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C118" t="s">
-        <v>448</v>
+        <v>459</v>
       </c>
       <c r="D118" t="s">
-        <v>600</v>
+        <v>615</v>
       </c>
       <c r="E118" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="H118">
         <v>2</v>
@@ -5698,16 +5800,16 @@
         <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C119" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
       <c r="D119" t="s">
-        <v>601</v>
+        <v>616</v>
       </c>
       <c r="E119" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -5724,16 +5826,16 @@
         <v>126</v>
       </c>
       <c r="B120" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C120" t="s">
-        <v>450</v>
+        <v>461</v>
       </c>
       <c r="D120" t="s">
-        <v>602</v>
+        <v>617</v>
       </c>
       <c r="E120" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -5750,16 +5852,16 @@
         <v>127</v>
       </c>
       <c r="B121" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C121" t="s">
-        <v>451</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>603</v>
+        <v>462</v>
+      </c>
+      <c r="D121" t="s">
+        <v>618</v>
       </c>
       <c r="E121" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="H121">
         <v>2</v>
@@ -5770,16 +5872,16 @@
         <v>128</v>
       </c>
       <c r="B122" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C122" t="s">
-        <v>452</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>604</v>
+        <v>463</v>
+      </c>
+      <c r="D122" t="s">
+        <v>619</v>
       </c>
       <c r="E122" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -5796,13 +5898,13 @@
         <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="C123" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="D123" t="s">
-        <v>605</v>
+        <v>620</v>
       </c>
       <c r="G123">
         <v>41</v>
@@ -5816,16 +5918,16 @@
         <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C124" t="s">
-        <v>451</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>606</v>
+        <v>462</v>
+      </c>
+      <c r="D124" t="s">
+        <v>621</v>
       </c>
       <c r="E124" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="H124">
         <v>3</v>
@@ -5836,16 +5938,16 @@
         <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C125" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="D125" t="s">
-        <v>607</v>
+        <v>622</v>
       </c>
       <c r="E125" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -5856,16 +5958,16 @@
         <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C126" t="s">
-        <v>454</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>608</v>
+        <v>465</v>
+      </c>
+      <c r="D126" t="s">
+        <v>623</v>
       </c>
       <c r="E126" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="F126">
         <v>5</v>
@@ -5882,16 +5984,16 @@
         <v>133</v>
       </c>
       <c r="B127" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C127" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
       <c r="D127" t="s">
-        <v>609</v>
+        <v>624</v>
       </c>
       <c r="E127" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5899,13 +6001,13 @@
         <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C128" t="s">
-        <v>456</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>610</v>
+        <v>467</v>
+      </c>
+      <c r="D128" t="s">
+        <v>625</v>
       </c>
       <c r="G128">
         <v>26</v>
@@ -5919,16 +6021,16 @@
         <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C129" t="s">
-        <v>457</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>611</v>
+        <v>468</v>
+      </c>
+      <c r="D129" t="s">
+        <v>626</v>
       </c>
       <c r="E129" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -5945,13 +6047,13 @@
         <v>136</v>
       </c>
       <c r="B130" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C130" t="s">
-        <v>458</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>612</v>
+        <v>469</v>
+      </c>
+      <c r="D130" t="s">
+        <v>627</v>
       </c>
       <c r="H130">
         <v>2</v>
@@ -5962,13 +6064,13 @@
         <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="C131" t="s">
-        <v>458</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>613</v>
+        <v>469</v>
+      </c>
+      <c r="D131" t="s">
+        <v>628</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -5979,16 +6081,16 @@
         <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C132" t="s">
-        <v>459</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>614</v>
+        <v>470</v>
+      </c>
+      <c r="D132" t="s">
+        <v>629</v>
       </c>
       <c r="E132" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -6005,16 +6107,16 @@
         <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C133" t="s">
-        <v>460</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>615</v>
+        <v>471</v>
+      </c>
+      <c r="D133" t="s">
+        <v>630</v>
       </c>
       <c r="E133" t="s">
-        <v>653</v>
+        <v>672</v>
       </c>
       <c r="F133">
         <v>7</v>
@@ -6031,16 +6133,16 @@
         <v>140</v>
       </c>
       <c r="B134" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C134" t="s">
-        <v>461</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>616</v>
+        <v>472</v>
+      </c>
+      <c r="D134" t="s">
+        <v>631</v>
       </c>
       <c r="E134" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="H134">
         <v>0.75</v>
@@ -6051,16 +6153,16 @@
         <v>141</v>
       </c>
       <c r="B135" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C135" t="s">
-        <v>461</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>617</v>
+        <v>472</v>
+      </c>
+      <c r="D135" t="s">
+        <v>632</v>
       </c>
       <c r="E135" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="H135">
         <v>2</v>
@@ -6071,16 +6173,16 @@
         <v>142</v>
       </c>
       <c r="B136" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C136" t="s">
-        <v>462</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>618</v>
+        <v>473</v>
+      </c>
+      <c r="D136" t="s">
+        <v>633</v>
       </c>
       <c r="E136" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -6097,16 +6199,16 @@
         <v>143</v>
       </c>
       <c r="B137" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C137" t="s">
-        <v>463</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>619</v>
+        <v>474</v>
+      </c>
+      <c r="D137" t="s">
+        <v>634</v>
       </c>
       <c r="E137" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="F137">
         <v>2</v>
@@ -6123,16 +6225,16 @@
         <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C138" t="s">
-        <v>464</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>620</v>
+        <v>475</v>
+      </c>
+      <c r="D138" t="s">
+        <v>635</v>
       </c>
       <c r="E138" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="F138">
         <v>3</v>
@@ -6149,16 +6251,16 @@
         <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C139" t="s">
-        <v>465</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>621</v>
+        <v>476</v>
+      </c>
+      <c r="D139" t="s">
+        <v>636</v>
       </c>
       <c r="E139" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="F139">
         <v>4</v>
@@ -6175,16 +6277,16 @@
         <v>146</v>
       </c>
       <c r="B140" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C140" t="s">
-        <v>466</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>622</v>
+        <v>477</v>
+      </c>
+      <c r="D140" t="s">
+        <v>637</v>
       </c>
       <c r="E140" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="H140">
         <v>0.75</v>
@@ -6195,16 +6297,16 @@
         <v>147</v>
       </c>
       <c r="B141" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C141" t="s">
-        <v>466</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>623</v>
+        <v>477</v>
+      </c>
+      <c r="D141" t="s">
+        <v>638</v>
       </c>
       <c r="E141" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="H141">
         <v>2</v>
@@ -6215,16 +6317,16 @@
         <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C142" t="s">
-        <v>467</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>624</v>
+        <v>478</v>
+      </c>
+      <c r="D142" t="s">
+        <v>639</v>
       </c>
       <c r="E142" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="F142">
         <v>5</v>
@@ -6241,16 +6343,16 @@
         <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C143" t="s">
-        <v>468</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>625</v>
+        <v>479</v>
+      </c>
+      <c r="D143" t="s">
+        <v>640</v>
       </c>
       <c r="E143" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="F143">
         <v>6</v>
@@ -6267,16 +6369,16 @@
         <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C144" t="s">
-        <v>469</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>626</v>
+        <v>480</v>
+      </c>
+      <c r="D144" t="s">
+        <v>641</v>
       </c>
       <c r="E144" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="H144">
         <v>0.75</v>
@@ -6287,16 +6389,16 @@
         <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C145" t="s">
-        <v>469</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>627</v>
+        <v>480</v>
+      </c>
+      <c r="D145" t="s">
+        <v>642</v>
       </c>
       <c r="E145" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="H145">
         <v>2</v>
@@ -6307,16 +6409,16 @@
         <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C146" t="s">
-        <v>470</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>628</v>
+        <v>481</v>
+      </c>
+      <c r="D146" t="s">
+        <v>643</v>
       </c>
       <c r="E146" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="F146">
         <v>101</v>
@@ -6333,16 +6435,16 @@
         <v>153</v>
       </c>
       <c r="B147" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C147" t="s">
-        <v>471</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>629</v>
+        <v>482</v>
+      </c>
+      <c r="D147" t="s">
+        <v>644</v>
       </c>
       <c r="E147" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="G147">
         <v>24</v>
@@ -6351,21 +6453,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>154</v>
       </c>
       <c r="B148" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="C148" t="s">
-        <v>472</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>630</v>
+        <v>483</v>
+      </c>
+      <c r="D148" t="s">
+        <v>645</v>
       </c>
       <c r="E148" t="s">
-        <v>656</v>
+        <v>675</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -6379,19 +6481,19 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B149" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C149" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="D149" t="s">
-        <v>633</v>
+        <v>646</v>
       </c>
       <c r="E149" t="s">
-        <v>656</v>
+        <v>675</v>
       </c>
       <c r="H149">
         <v>0.75</v>
@@ -6399,19 +6501,19 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B150" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C150" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="D150" t="s">
-        <v>634</v>
+        <v>647</v>
       </c>
       <c r="E150" t="s">
-        <v>656</v>
+        <v>675</v>
       </c>
       <c r="H150">
         <v>2</v>
@@ -6419,19 +6521,19 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B151" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C151" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="D151" t="s">
-        <v>635</v>
+        <v>648</v>
       </c>
       <c r="E151" t="s">
-        <v>656</v>
+        <v>675</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -6445,19 +6547,19 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B152" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C152" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="D152" t="s">
-        <v>636</v>
+        <v>649</v>
       </c>
       <c r="E152" t="s">
-        <v>656</v>
+        <v>675</v>
       </c>
       <c r="F152">
         <v>3</v>
@@ -6471,33 +6573,33 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B153" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="D153" t="s">
-        <v>631</v>
+        <v>650</v>
       </c>
       <c r="E153" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B154" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="C154" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D154" t="s">
-        <v>632</v>
+        <v>651</v>
       </c>
       <c r="E154" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="G154">
         <v>24</v>
@@ -6511,13 +6613,13 @@
         <v>161</v>
       </c>
       <c r="B155" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="D155" t="s">
-        <v>637</v>
+        <v>652</v>
       </c>
       <c r="E155" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -6525,13 +6627,13 @@
         <v>162</v>
       </c>
       <c r="B156" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="D156" t="s">
-        <v>638</v>
+        <v>653</v>
       </c>
       <c r="E156" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -6539,16 +6641,16 @@
         <v>163</v>
       </c>
       <c r="B157" t="s">
-        <v>655</v>
+        <v>333</v>
       </c>
       <c r="C157" t="s">
-        <v>477</v>
+        <v>488</v>
       </c>
       <c r="D157" t="s">
-        <v>639</v>
+        <v>654</v>
       </c>
       <c r="E157" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="G157">
         <v>39</v>
@@ -6559,16 +6661,16 @@
         <v>164</v>
       </c>
       <c r="B158" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="C158" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="D158" t="s">
-        <v>640</v>
+        <v>655</v>
       </c>
       <c r="E158" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6576,13 +6678,13 @@
         <v>165</v>
       </c>
       <c r="B159" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D159" t="s">
-        <v>641</v>
+        <v>656</v>
       </c>
       <c r="E159" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6590,141 +6692,253 @@
         <v>166</v>
       </c>
       <c r="B160" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C160" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="D160" t="s">
-        <v>642</v>
+        <v>657</v>
       </c>
       <c r="E160" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="G160">
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>167</v>
       </c>
       <c r="B161" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C161" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="D161" t="s">
-        <v>643</v>
+        <v>658</v>
       </c>
       <c r="E161" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>168</v>
       </c>
       <c r="B162" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="C162" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="D162" t="s">
-        <v>644</v>
+        <v>659</v>
       </c>
       <c r="E162" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>169</v>
       </c>
       <c r="B163" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="C163" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="D163" t="s">
-        <v>645</v>
+        <v>660</v>
       </c>
       <c r="E163" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="G163">
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>170</v>
       </c>
       <c r="B164" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C164" t="s">
-        <v>482</v>
+        <v>493</v>
       </c>
       <c r="D164" t="s">
-        <v>646</v>
+        <v>661</v>
       </c>
       <c r="E164" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="G164">
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>171</v>
       </c>
       <c r="B165" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="D165" t="s">
-        <v>647</v>
+        <v>662</v>
       </c>
       <c r="E165" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>172</v>
       </c>
       <c r="B166" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="D166" t="s">
-        <v>648</v>
+        <v>663</v>
       </c>
       <c r="E166" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>173</v>
       </c>
       <c r="B167" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C167" t="s">
-        <v>483</v>
+        <v>494</v>
       </c>
       <c r="D167" t="s">
-        <v>649</v>
+        <v>664</v>
       </c>
       <c r="E167" t="s">
-        <v>650</v>
+        <v>673</v>
       </c>
       <c r="G167">
         <v>41</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>174</v>
+      </c>
+      <c r="B168" t="s">
+        <v>344</v>
+      </c>
+      <c r="C168" t="s">
+        <v>495</v>
+      </c>
+      <c r="D168" t="s">
+        <v>665</v>
+      </c>
+      <c r="E168" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>175</v>
+      </c>
+      <c r="B169" t="s">
+        <v>345</v>
+      </c>
+      <c r="C169" t="s">
+        <v>495</v>
+      </c>
+      <c r="D169" t="s">
+        <v>666</v>
+      </c>
+      <c r="E169" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>176</v>
+      </c>
+      <c r="B170" t="s">
+        <v>346</v>
+      </c>
+      <c r="C170" t="s">
+        <v>496</v>
+      </c>
+      <c r="D170" t="s">
+        <v>667</v>
+      </c>
+      <c r="E170" t="s">
+        <v>675</v>
+      </c>
+      <c r="F170">
+        <v>4</v>
+      </c>
+      <c r="G170">
+        <v>30</v>
+      </c>
+      <c r="H170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>177</v>
+      </c>
+      <c r="B171" t="s">
+        <v>347</v>
+      </c>
+      <c r="C171" t="s">
+        <v>497</v>
+      </c>
+      <c r="D171" t="s">
+        <v>668</v>
+      </c>
+      <c r="E171" t="s">
+        <v>675</v>
+      </c>
+      <c r="F171">
+        <v>5</v>
+      </c>
+      <c r="G171">
+        <v>30</v>
+      </c>
+      <c r="H171">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>178</v>
+      </c>
+      <c r="B172" t="s">
+        <v>348</v>
+      </c>
+      <c r="C172" t="s">
+        <v>498</v>
+      </c>
+      <c r="D172" t="s">
+        <v>669</v>
+      </c>
+      <c r="E172" t="s">
+        <v>675</v>
+      </c>
+      <c r="F172">
+        <v>6</v>
+      </c>
+      <c r="G172">
+        <v>20</v>
+      </c>
+      <c r="H172">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support single thread visualization
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3E8517-B5F4-4EE6-8B74-0B10EFB228D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="699">
   <si>
     <t>ephysFN</t>
   </si>
@@ -559,6 +553,24 @@
     <t>Beto-11032020-005</t>
   </si>
   <si>
+    <t>Beto-17032020-001</t>
+  </si>
+  <si>
+    <t>Beto-17032020-002</t>
+  </si>
+  <si>
+    <t>Beto-17032020-004</t>
+  </si>
+  <si>
+    <t>Beto-17032020-005</t>
+  </si>
+  <si>
+    <t>Beto-17032020-006</t>
+  </si>
+  <si>
+    <t>Beto-17032020-007</t>
+  </si>
+  <si>
     <t>191002_Beto_selectivity_basic(1)</t>
   </si>
   <si>
@@ -1069,6 +1081,24 @@
     <t>200311_Beto_generate_integrated(2)</t>
   </si>
   <si>
+    <t>200317_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200317_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200317_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200317_Beto_generate_integrated(2)</t>
+  </si>
+  <si>
+    <t>200317_Beto_generate_integrated(3)</t>
+  </si>
+  <si>
+    <t>200317_Beto_generate_integrated(4)</t>
+  </si>
+  <si>
     <t>\\storage1.ris.wustl.edu\crponce\Active\Stimuli\2019-Selectivity\2019-10-02a-beto</t>
   </si>
   <si>
@@ -1399,7 +1429,7 @@
     <t>N:\Stimuli\2019-12-Evolutions\2020-01-23-Beto-01\2020-01-23-12-36-03</t>
   </si>
   <si>
-    <t>. </t>
+    <t xml:space="preserve">. </t>
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-01-27-Beto-01\2020-01-27-11-23-03</t>
@@ -1517,6 +1547,21 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-11-Beto-03\2020-03-11-14-52-05</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-17-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-17-Beto-01\2020-03-17-13-04-35</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-17-Beto-02\2020-03-17-13-28-48</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-17-Beto-03\2020-03-17-14-04-57</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-17-Beto-04\2020-03-17-14-42-52</t>
   </si>
   <si>
     <t>Derived from PCs of Ch 29 evolution 191002. 373 images {11*11 in PC2,PC3; PC49 PC50; RND RND space respectively, +10 last gen}</t>
@@ -1921,13 +1966,13 @@
 Blasting him, 300 ms, going to block 50 then calling it a day</t>
   </si>
   <si>
-    <t>Rf basic Start 11:11, 35 ms reward. New units in 41, rf looks weird tho Stopped at 11:17, 4 blocks complete </t>
-  </si>
-  <si>
-    <t>Generate integrate. Ch 5 hash (1/5) [-1.5, 1] 3 1; GA vs CMAES, bigset05 first 10 images Start at 11:23. Carlos recalibrated eye at block 2. working well 45 ms reward . Evolved images are climbing…..block 16, #1(black line) is top line Block 27: Black line is wayyy above the rest and still climbing. Reward at 50 at block 30,  Stopped at 12:04, 40 blocks completed </t>
-  </si>
-  <si>
-    <t>Generate integrated. Ch 20. hash 1/5. [-2, 1.5] 3 1. start at 12:06 Bigset20 first 10 images, reward at 90. starting to shake chair Upped to 130 reward. Added aq reward at block 16. 170 ms at block 20. Evolved images are climbing, both above natural now Hmm, nether really taking off yet. Block 28, 220+30 One image is more contrasting (white background, pink and dark colored object) Other image is more gray/pink and blended. monkey quitting. Experiment has enough blocks to call it completed, but we're really struggling to get the last few trials. Let's see if we make it to block 35.  </t>
+    <t xml:space="preserve">Rf basic Start 11:11, 35 ms reward. New units in 41, rf looks weird tho Stopped at 11:17, 4 blocks complete </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate integrate. Ch 5 hash (1/5) [-1.5, 1] 3 1; GA vs CMAES, bigset05 first 10 images Start at 11:23. Carlos recalibrated eye at block 2. working well 45 ms reward . Evolved images are climbing…..block 16, #1(black line) is top line Block 27: Black line is wayyy above the rest and still climbing. Reward at 50 at block 30,  Stopped at 12:04, 40 blocks completed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate integrated. Ch 20. hash 1/5. [-2, 1.5] 3 1. start at 12:06 Bigset20 first 10 images, reward at 90. starting to shake chair Upped to 130 reward. Added aq reward at block 16. 170 ms at block 20. Evolved images are climbing, both above natural now Hmm, nether really taking off yet. Block 28, 220+30 One image is more contrasting (white background, pink and dark colored object) Other image is more gray/pink and blended. monkey quitting. Experiment has enough blocks to call it completed, but we're really struggling to get the last few trials. Let's see if we make it to block 35.  </t>
   </si>
   <si>
     <t>001 RFMapper 11:02 AM starts 
@@ -2340,6 +2385,82 @@
 Completed, quite informative</t>
   </si>
   <si>
+    <t>001 starts 12.
+-8:2:8</t>
+  </si>
+  <si>
+    <t>002 stars
+-1.5：0.75：1.5
+003 satar
+Trash.…</t>
+  </si>
+  <si>
+    <t>004  starts
+19 [0, 2.5] 5 1  ZOHA Sphere lr euclid
+Test the ZOHA Sphere lr euclid works on Beto
+He takes off pretty slow, around 25 gens
+23.2 deg
+Maybe switch to CMAES
+Unit 19 is super Hashy, maybe no clear selectivity
+Starts oscillation around 28 gens, maybe the step size  20deg is still too large here?
+22mins evolves a rounded thing there
+45 gens
+Completed</t>
+  </si>
+  <si>
+    <t>005 starts 13:28
+19 [0, 2.5] 5 1  CMAES
+Test the old fashion CMAES works. (Same setting )
+Evolves a Initial response in 3 rd gens
+CMA ES is not exceptionally good as well! So goo! We are comparable
+The rounded thing it got is quite different from the last one.
+10 mins 22 blocks
+Starts recruit more plateau and sustained activity !
+45 gens to match the last one
+Seems still CMAES has the power to recruit more activity
+Still works pretty well!
+45 gens, 25 mins
+Completed</t>
+  </si>
+  <si>
+    <t>6 starts
+19 [0, 2.5] 5 1  ZOHA_Sphere_Euclid_lr
+ZOHA Euclid lr
+Use the inverse law of exploration rate decay. From 70-15 in 100 gens
+Seems the PSTH evolution patten feels really like CMAES!
+9 gens, exploration ~ 48.4 deg. Step size 0.667
+So using huge step size can effectively get rid of the initialization effect.
+Starts growing at 16gens, current exploration 42.2 deg.
+20 gens 34.9 deg,
+at gen 28, it's around 30 deg, It's climbing very well just like CMAES.
+The growing trajectory looks very good.
+Seems still the eye thing in the image.
+Seems even more successful than the CMAES!
+Why no effect on the first 10 generations…… just random walk? Or is there something happening there.
+37 gens 27.6 deg
+End in 46 gens.
+This is very informative experiments
+Completed</t>
+  </si>
+  <si>
+    <t>007 starts 14:42
+19 [0, 2.5] 5 1  ZOHA_Sphere_Euclid_lr_RD
+Same inverse decaying rule as the last exp, just restricted to 50D subspace. , still can evolve, but seems cannot find the point.
+Gen 7 52.2 deg.
+# Maybe ZOHA reduced Dimension?
+Starts climbing at gen 7
+Exploration 46 deg, step size 0.42
+Slowly growing at 13 gens.
+16gens 38.5 deg
+20 gens 34.5 deg, step 0.303
+Plateaued super early around 16 gens cannot improve anymore.
+30 gens Exploration 29.2, step size 0.227.
+Oscillating around 27-32 gens, step size too large here?
+38 gens 27.3 deg
+34 mins for 38 blocks, 37 mins for 42 blocks.Gets to 46 blocks!
+Completed</t>
+  </si>
+  <si>
     <t>Manifold</t>
   </si>
   <si>
@@ -2361,8 +2482,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2421,23 +2542,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2479,7 +2592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2511,27 +2624,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2563,24 +2658,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2756,20 +2833,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H172"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F173" sqref="F173"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="100.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2795,21 +2866,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="D2" t="s">
-        <v>499</v>
+        <v>516</v>
       </c>
       <c r="E2" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2821,21 +2892,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="D3" t="s">
-        <v>500</v>
+        <v>517</v>
       </c>
       <c r="E3" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2847,21 +2918,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>518</v>
       </c>
       <c r="E4" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -2873,21 +2944,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="D5" t="s">
-        <v>502</v>
+        <v>519</v>
       </c>
       <c r="E5" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2899,21 +2970,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="D6" t="s">
-        <v>503</v>
+        <v>520</v>
       </c>
       <c r="E6" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2925,21 +2996,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="D7" t="s">
-        <v>504</v>
+        <v>521</v>
       </c>
       <c r="E7" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -2951,21 +3022,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C8" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="D8" t="s">
-        <v>505</v>
+        <v>522</v>
       </c>
       <c r="E8" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2977,21 +3048,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C9" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="D9" t="s">
-        <v>506</v>
+        <v>523</v>
       </c>
       <c r="E9" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -3003,21 +3074,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s">
-        <v>507</v>
+        <v>524</v>
       </c>
       <c r="E10" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -3029,21 +3100,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="D11" t="s">
-        <v>508</v>
+        <v>525</v>
       </c>
       <c r="E11" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -3055,21 +3126,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="D12" t="s">
-        <v>509</v>
+        <v>526</v>
       </c>
       <c r="E12" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3081,21 +3152,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C13" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="D13" t="s">
-        <v>510</v>
+        <v>527</v>
       </c>
       <c r="E13" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3107,21 +3178,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C14" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
       <c r="D14" t="s">
-        <v>511</v>
+        <v>528</v>
       </c>
       <c r="E14" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -3133,21 +3204,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="D15" t="s">
-        <v>512</v>
+        <v>529</v>
       </c>
       <c r="E15" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -3159,21 +3230,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="D16" t="s">
-        <v>513</v>
+        <v>530</v>
       </c>
       <c r="E16" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -3185,21 +3256,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="D17" t="s">
-        <v>514</v>
+        <v>531</v>
       </c>
       <c r="E17" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -3211,21 +3282,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C18" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
       <c r="D18" t="s">
-        <v>515</v>
+        <v>532</v>
       </c>
       <c r="E18" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -3237,21 +3308,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C19" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="D19" t="s">
-        <v>516</v>
+        <v>533</v>
       </c>
       <c r="E19" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -3263,21 +3334,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C20" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="D20" t="s">
-        <v>517</v>
+        <v>534</v>
       </c>
       <c r="E20" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3289,21 +3360,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C21" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="D21" t="s">
-        <v>518</v>
+        <v>535</v>
       </c>
       <c r="E21" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3315,21 +3386,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C22" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="D22" t="s">
-        <v>519</v>
+        <v>536</v>
       </c>
       <c r="E22" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -3341,21 +3412,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C23" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="D23" t="s">
-        <v>520</v>
+        <v>537</v>
       </c>
       <c r="E23" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -3367,21 +3438,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="D24" t="s">
-        <v>521</v>
+        <v>538</v>
       </c>
       <c r="E24" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -3393,21 +3464,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C25" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="D25" t="s">
-        <v>522</v>
+        <v>539</v>
       </c>
       <c r="E25" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -3419,21 +3490,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C26" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="D26" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="E26" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -3445,21 +3516,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C27" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="D27" t="s">
-        <v>524</v>
+        <v>541</v>
       </c>
       <c r="E27" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -3471,21 +3542,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C28" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="D28" t="s">
-        <v>525</v>
+        <v>542</v>
       </c>
       <c r="E28" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -3497,21 +3568,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C29" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="D29" t="s">
-        <v>526</v>
+        <v>543</v>
       </c>
       <c r="E29" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -3523,21 +3594,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C30" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="D30" t="s">
-        <v>527</v>
+        <v>544</v>
       </c>
       <c r="E30" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -3549,21 +3620,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C31" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="D31" t="s">
-        <v>528</v>
+        <v>545</v>
       </c>
       <c r="E31" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -3575,21 +3646,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C32" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="D32" t="s">
-        <v>529</v>
+        <v>546</v>
       </c>
       <c r="E32" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -3601,21 +3672,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C33" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="D33" t="s">
-        <v>530</v>
+        <v>547</v>
       </c>
       <c r="E33" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -3627,21 +3698,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C34" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="D34" t="s">
-        <v>531</v>
+        <v>548</v>
       </c>
       <c r="E34" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -3653,21 +3724,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C35" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="D35" t="s">
-        <v>532</v>
+        <v>549</v>
       </c>
       <c r="E35" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -3679,21 +3750,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C36" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="D36" t="s">
-        <v>533</v>
+        <v>550</v>
       </c>
       <c r="E36" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -3705,21 +3776,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C37" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="D37" t="s">
-        <v>534</v>
+        <v>551</v>
       </c>
       <c r="E37" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -3731,21 +3802,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C38" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="D38" t="s">
-        <v>535</v>
+        <v>552</v>
       </c>
       <c r="E38" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -3757,21 +3828,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C39" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="D39" t="s">
-        <v>536</v>
+        <v>553</v>
       </c>
       <c r="E39" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -3783,21 +3854,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C40" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="D40" t="s">
-        <v>537</v>
+        <v>554</v>
       </c>
       <c r="E40" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -3809,21 +3880,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C41" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="D41" t="s">
-        <v>538</v>
+        <v>555</v>
       </c>
       <c r="E41" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -3835,21 +3906,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="C42" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="D42" t="s">
-        <v>539</v>
+        <v>556</v>
       </c>
       <c r="E42" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -3861,21 +3932,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="D43" t="s">
-        <v>540</v>
+        <v>557</v>
       </c>
       <c r="E43" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -3887,21 +3958,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C44" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="D44" t="s">
-        <v>541</v>
+        <v>558</v>
       </c>
       <c r="E44" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -3913,21 +3984,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C45" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D45" t="s">
-        <v>542</v>
+        <v>559</v>
       </c>
       <c r="E45" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -3939,21 +4010,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C46" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="D46" t="s">
-        <v>543</v>
+        <v>560</v>
       </c>
       <c r="E46" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -3965,21 +4036,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C47" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="D47" t="s">
-        <v>544</v>
+        <v>561</v>
       </c>
       <c r="E47" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -3991,21 +4062,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C48" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="D48" t="s">
-        <v>545</v>
+        <v>562</v>
       </c>
       <c r="E48" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F48">
         <v>23</v>
@@ -4017,21 +4088,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C49" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="D49" t="s">
-        <v>546</v>
+        <v>563</v>
       </c>
       <c r="E49" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F49">
         <v>23</v>
@@ -4043,21 +4114,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C50" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="D50" t="s">
-        <v>547</v>
+        <v>564</v>
       </c>
       <c r="E50" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F50">
         <v>24</v>
@@ -4069,21 +4140,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C51" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="D51" t="s">
-        <v>548</v>
+        <v>565</v>
       </c>
       <c r="E51" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -4095,21 +4166,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C52" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="D52" t="s">
-        <v>549</v>
+        <v>566</v>
       </c>
       <c r="E52" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F52">
         <v>24</v>
@@ -4121,18 +4192,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C53" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="D53" t="s">
-        <v>550</v>
+        <v>567</v>
       </c>
       <c r="F53">
         <v>24</v>
@@ -4144,21 +4215,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C54" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
       <c r="D54" t="s">
-        <v>551</v>
+        <v>568</v>
       </c>
       <c r="E54" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -4170,21 +4241,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C55" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="D55" t="s">
-        <v>552</v>
+        <v>569</v>
       </c>
       <c r="E55" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F55">
         <v>25</v>
@@ -4196,21 +4267,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C56" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
       <c r="D56" t="s">
-        <v>553</v>
+        <v>570</v>
       </c>
       <c r="E56" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F56">
         <v>25</v>
@@ -4222,21 +4293,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C57" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="D57" t="s">
-        <v>554</v>
+        <v>571</v>
       </c>
       <c r="E57" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -4248,21 +4319,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C58" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="D58" t="s">
-        <v>555</v>
+        <v>572</v>
       </c>
       <c r="E58" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -4274,21 +4345,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C59" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
       <c r="D59" t="s">
-        <v>556</v>
+        <v>573</v>
       </c>
       <c r="E59" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -4300,21 +4371,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C60" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="D60" t="s">
-        <v>557</v>
+        <v>574</v>
       </c>
       <c r="E60" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F60">
         <v>27</v>
@@ -4326,21 +4397,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C61" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="D61" t="s">
-        <v>558</v>
+        <v>575</v>
       </c>
       <c r="E61" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F61">
         <v>27</v>
@@ -4352,21 +4423,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C62" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="D62" t="s">
-        <v>559</v>
+        <v>576</v>
       </c>
       <c r="E62" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F62">
         <v>27</v>
@@ -4378,21 +4449,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C63" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="D63" t="s">
-        <v>560</v>
+        <v>577</v>
       </c>
       <c r="E63" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -4404,21 +4475,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C64" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="D64" t="s">
-        <v>561</v>
+        <v>578</v>
       </c>
       <c r="E64" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -4430,21 +4501,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C65" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
       <c r="D65" t="s">
-        <v>562</v>
+        <v>579</v>
       </c>
       <c r="E65" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -4456,21 +4527,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C66" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="D66" t="s">
-        <v>563</v>
+        <v>580</v>
       </c>
       <c r="E66" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -4482,21 +4553,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C67" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="D67" t="s">
-        <v>564</v>
+        <v>581</v>
       </c>
       <c r="E67" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -4508,21 +4579,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C68" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="D68" t="s">
-        <v>565</v>
+        <v>582</v>
       </c>
       <c r="E68" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -4534,21 +4605,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C69" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="D69" t="s">
-        <v>566</v>
+        <v>583</v>
       </c>
       <c r="E69" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -4560,21 +4631,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C70" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="D70" t="s">
-        <v>567</v>
+        <v>584</v>
       </c>
       <c r="E70" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -4586,21 +4657,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C71" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="D71" t="s">
-        <v>568</v>
+        <v>585</v>
       </c>
       <c r="E71" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -4612,21 +4683,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C72" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
       <c r="D72" t="s">
-        <v>569</v>
+        <v>586</v>
       </c>
       <c r="E72" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -4638,21 +4709,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C73" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="D73" t="s">
-        <v>570</v>
+        <v>587</v>
       </c>
       <c r="E73" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -4664,21 +4735,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C74" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
       <c r="D74" t="s">
-        <v>571</v>
+        <v>588</v>
       </c>
       <c r="E74" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -4690,21 +4761,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C75" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="D75" t="s">
-        <v>572</v>
+        <v>589</v>
       </c>
       <c r="E75" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -4716,21 +4787,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C76" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="D76" t="s">
-        <v>573</v>
+        <v>590</v>
       </c>
       <c r="E76" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -4742,21 +4813,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C77" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="D77" t="s">
-        <v>574</v>
+        <v>591</v>
       </c>
       <c r="E77" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -4768,21 +4839,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C78" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="D78" t="s">
-        <v>575</v>
+        <v>592</v>
       </c>
       <c r="E78" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -4794,21 +4865,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C79" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="D79" t="s">
-        <v>576</v>
+        <v>593</v>
       </c>
       <c r="E79" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -4820,21 +4891,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C80" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="D80" t="s">
-        <v>577</v>
+        <v>594</v>
       </c>
       <c r="E80" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -4846,18 +4917,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C81" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="D81" t="s">
-        <v>578</v>
+        <v>595</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -4869,18 +4940,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C82" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="D82" t="s">
-        <v>579</v>
+        <v>596</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -4892,18 +4963,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>89</v>
       </c>
       <c r="C83" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="D83" t="s">
-        <v>580</v>
+        <v>597</v>
       </c>
       <c r="E83" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -4915,21 +4986,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="C84" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="D84" t="s">
-        <v>581</v>
+        <v>598</v>
       </c>
       <c r="E84" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -4941,21 +5012,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>91</v>
       </c>
       <c r="B85" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C85" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="D85" t="s">
-        <v>582</v>
+        <v>599</v>
       </c>
       <c r="E85" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F85">
         <v>35</v>
@@ -4967,21 +5038,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C86" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="D86" t="s">
-        <v>583</v>
+        <v>600</v>
       </c>
       <c r="E86" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -4993,21 +5064,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C87" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="D87" t="s">
-        <v>584</v>
+        <v>601</v>
       </c>
       <c r="E87" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F87">
         <v>36</v>
@@ -5019,21 +5090,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C88" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
       <c r="D88" t="s">
-        <v>585</v>
+        <v>602</v>
       </c>
       <c r="E88" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -5045,21 +5116,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>95</v>
       </c>
       <c r="B89" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C89" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="D89" t="s">
-        <v>586</v>
+        <v>603</v>
       </c>
       <c r="E89" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -5071,21 +5142,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C90" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="D90" t="s">
-        <v>587</v>
+        <v>604</v>
       </c>
       <c r="E90" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F90">
         <v>37</v>
@@ -5097,21 +5168,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C91" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="D91" t="s">
-        <v>588</v>
+        <v>605</v>
       </c>
       <c r="E91" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -5123,21 +5194,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C92" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="D92" t="s">
-        <v>589</v>
+        <v>606</v>
       </c>
       <c r="E92" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F92">
         <v>38</v>
@@ -5149,21 +5220,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C93" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="D93" t="s">
-        <v>590</v>
+        <v>607</v>
       </c>
       <c r="E93" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -5175,21 +5246,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C94" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="D94" t="s">
-        <v>591</v>
+        <v>608</v>
       </c>
       <c r="E94" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -5201,21 +5272,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>101</v>
       </c>
       <c r="B95" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C95" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="D95" t="s">
-        <v>592</v>
+        <v>609</v>
       </c>
       <c r="E95" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F95">
         <v>39</v>
@@ -5227,21 +5298,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C96" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="D96" t="s">
-        <v>593</v>
+        <v>610</v>
       </c>
       <c r="E96" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -5253,21 +5324,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C97" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="D97" t="s">
-        <v>594</v>
+        <v>611</v>
       </c>
       <c r="E97" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -5279,21 +5350,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C98" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="D98" t="s">
-        <v>595</v>
+        <v>612</v>
       </c>
       <c r="E98" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -5305,21 +5376,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>105</v>
       </c>
       <c r="B99" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C99" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="D99" t="s">
-        <v>596</v>
+        <v>613</v>
       </c>
       <c r="E99" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -5331,21 +5402,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>106</v>
       </c>
       <c r="B100" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C100" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="D100" t="s">
-        <v>597</v>
+        <v>614</v>
       </c>
       <c r="E100" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F100">
         <v>41</v>
@@ -5357,41 +5428,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>107</v>
       </c>
       <c r="B101" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C101" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="D101" t="s">
-        <v>598</v>
+        <v>615</v>
       </c>
       <c r="E101" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
       <c r="F101">
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>108</v>
       </c>
       <c r="B102" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="C102" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="D102" t="s">
-        <v>599</v>
+        <v>616</v>
       </c>
       <c r="E102" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -5403,21 +5474,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C103" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="D103" t="s">
-        <v>600</v>
+        <v>617</v>
       </c>
       <c r="E103" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -5429,21 +5500,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C104" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="D104" t="s">
-        <v>601</v>
+        <v>618</v>
       </c>
       <c r="E104" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F104">
         <v>42</v>
@@ -5455,21 +5526,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C105" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="D105" t="s">
-        <v>602</v>
+        <v>619</v>
       </c>
       <c r="E105" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -5481,21 +5552,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>112</v>
       </c>
       <c r="B106" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C106" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="D106" t="s">
-        <v>603</v>
+        <v>620</v>
       </c>
       <c r="E106" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -5507,21 +5578,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>113</v>
       </c>
       <c r="B107" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C107" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="D107" t="s">
-        <v>604</v>
+        <v>621</v>
       </c>
       <c r="E107" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F107">
         <v>43</v>
@@ -5533,61 +5604,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C108" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="D108" t="s">
-        <v>605</v>
+        <v>622</v>
       </c>
       <c r="E108" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
       <c r="F108">
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>115</v>
       </c>
       <c r="B109" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C109" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="D109" t="s">
-        <v>606</v>
+        <v>623</v>
       </c>
       <c r="E109" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
       <c r="F109">
         <v>43</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>116</v>
       </c>
       <c r="B110" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C110" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="D110" t="s">
-        <v>607</v>
+        <v>624</v>
       </c>
       <c r="E110" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -5599,21 +5670,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C111" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="D111" t="s">
-        <v>608</v>
+        <v>625</v>
       </c>
       <c r="E111" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -5625,21 +5696,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C112" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="D112" t="s">
-        <v>609</v>
+        <v>626</v>
       </c>
       <c r="E112" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F112">
         <v>44</v>
@@ -5651,21 +5722,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>119</v>
       </c>
       <c r="B113" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C113" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="D113" t="s">
-        <v>610</v>
+        <v>627</v>
       </c>
       <c r="E113" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -5677,21 +5748,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>120</v>
       </c>
       <c r="B114" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C114" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="D114" t="s">
-        <v>611</v>
+        <v>628</v>
       </c>
       <c r="E114" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -5703,21 +5774,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>121</v>
       </c>
       <c r="B115" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C115" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="D115" t="s">
-        <v>612</v>
+        <v>629</v>
       </c>
       <c r="E115" t="s">
-        <v>670</v>
+        <v>693</v>
       </c>
       <c r="F115">
         <v>45</v>
@@ -5729,41 +5800,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C116" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="D116" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="E116" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="H116">
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C117" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="D117" t="s">
-        <v>614</v>
+        <v>631</v>
       </c>
       <c r="E117" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -5775,41 +5846,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C118" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="D118" t="s">
-        <v>615</v>
+        <v>632</v>
       </c>
       <c r="E118" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="H118">
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C119" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="D119" t="s">
-        <v>616</v>
+        <v>633</v>
       </c>
       <c r="E119" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -5821,21 +5892,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>126</v>
       </c>
       <c r="B120" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C120" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="D120" t="s">
-        <v>617</v>
+        <v>634</v>
       </c>
       <c r="E120" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -5847,41 +5918,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>127</v>
       </c>
       <c r="B121" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C121" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="D121" t="s">
-        <v>618</v>
+        <v>635</v>
       </c>
       <c r="E121" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="H121">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>128</v>
       </c>
       <c r="B122" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C122" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="D122" t="s">
-        <v>619</v>
+        <v>636</v>
       </c>
       <c r="E122" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -5893,18 +5964,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="C123" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="D123" t="s">
-        <v>620</v>
+        <v>637</v>
       </c>
       <c r="G123">
         <v>41</v>
@@ -5913,61 +5984,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="C124" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="D124" t="s">
-        <v>621</v>
+        <v>638</v>
       </c>
       <c r="E124" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="H124">
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="C125" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="D125" t="s">
-        <v>622</v>
+        <v>639</v>
       </c>
       <c r="E125" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="H125">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="C126" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="D126" t="s">
-        <v>623</v>
+        <v>640</v>
       </c>
       <c r="E126" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="F126">
         <v>5</v>
@@ -5979,35 +6050,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>133</v>
       </c>
       <c r="B127" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="C127" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
       <c r="D127" t="s">
-        <v>624</v>
+        <v>641</v>
       </c>
       <c r="E127" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="C128" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="D128" t="s">
-        <v>625</v>
+        <v>642</v>
       </c>
       <c r="G128">
         <v>26</v>
@@ -6016,21 +6087,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="C129" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="D129" t="s">
-        <v>626</v>
+        <v>643</v>
       </c>
       <c r="E129" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -6042,55 +6113,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>136</v>
       </c>
       <c r="B130" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="C130" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="D130" t="s">
-        <v>627</v>
+        <v>644</v>
       </c>
       <c r="H130">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="C131" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="D131" t="s">
-        <v>628</v>
+        <v>645</v>
       </c>
       <c r="H131">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C132" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="D132" t="s">
-        <v>629</v>
+        <v>646</v>
       </c>
       <c r="E132" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -6102,21 +6173,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C133" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="D133" t="s">
-        <v>630</v>
+        <v>647</v>
       </c>
       <c r="E133" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="F133">
         <v>7</v>
@@ -6128,61 +6199,61 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>140</v>
       </c>
       <c r="B134" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C134" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="D134" t="s">
-        <v>631</v>
+        <v>648</v>
       </c>
       <c r="E134" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="H134">
         <v>0.75</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>141</v>
       </c>
       <c r="B135" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="C135" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="D135" t="s">
-        <v>632</v>
+        <v>649</v>
       </c>
       <c r="E135" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="H135">
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>142</v>
       </c>
       <c r="B136" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="C136" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="D136" t="s">
-        <v>633</v>
+        <v>650</v>
       </c>
       <c r="E136" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -6194,21 +6265,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>143</v>
       </c>
       <c r="B137" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C137" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="D137" t="s">
-        <v>634</v>
+        <v>651</v>
       </c>
       <c r="E137" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="F137">
         <v>2</v>
@@ -6220,21 +6291,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="C138" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="D138" t="s">
-        <v>635</v>
+        <v>652</v>
       </c>
       <c r="E138" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="F138">
         <v>3</v>
@@ -6246,21 +6317,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="C139" t="s">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="D139" t="s">
-        <v>636</v>
+        <v>653</v>
       </c>
       <c r="E139" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="F139">
         <v>4</v>
@@ -6272,61 +6343,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>146</v>
       </c>
       <c r="B140" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="C140" t="s">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="D140" t="s">
-        <v>637</v>
+        <v>654</v>
       </c>
       <c r="E140" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="H140">
         <v>0.75</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>147</v>
       </c>
       <c r="B141" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C141" t="s">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="D141" t="s">
-        <v>638</v>
+        <v>655</v>
       </c>
       <c r="E141" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="H141">
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="C142" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
       <c r="D142" t="s">
-        <v>639</v>
+        <v>656</v>
       </c>
       <c r="E142" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="F142">
         <v>5</v>
@@ -6338,21 +6409,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="C143" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="D143" t="s">
-        <v>640</v>
+        <v>657</v>
       </c>
       <c r="E143" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="F143">
         <v>6</v>
@@ -6364,61 +6435,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="C144" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="D144" t="s">
-        <v>641</v>
+        <v>658</v>
       </c>
       <c r="E144" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="H144">
         <v>0.75</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="C145" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="D145" t="s">
-        <v>642</v>
+        <v>659</v>
       </c>
       <c r="E145" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="H145">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C146" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="D146" t="s">
-        <v>643</v>
+        <v>660</v>
       </c>
       <c r="E146" t="s">
-        <v>674</v>
+        <v>697</v>
       </c>
       <c r="F146">
         <v>101</v>
@@ -6430,21 +6501,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>153</v>
       </c>
       <c r="B147" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="C147" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="D147" t="s">
-        <v>644</v>
+        <v>661</v>
       </c>
       <c r="E147" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="G147">
         <v>24</v>
@@ -6453,21 +6524,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>154</v>
       </c>
       <c r="B148" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="C148" t="s">
-        <v>483</v>
+        <v>495</v>
       </c>
       <c r="D148" t="s">
-        <v>645</v>
+        <v>662</v>
       </c>
       <c r="E148" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -6479,61 +6550,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>155</v>
       </c>
       <c r="B149" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="C149" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="D149" t="s">
-        <v>646</v>
+        <v>663</v>
       </c>
       <c r="E149" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="H149">
         <v>0.75</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>156</v>
       </c>
       <c r="B150" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="C150" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="D150" t="s">
-        <v>647</v>
+        <v>664</v>
       </c>
       <c r="E150" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="H150">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>157</v>
       </c>
       <c r="B151" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="C151" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="D151" t="s">
-        <v>648</v>
+        <v>665</v>
       </c>
       <c r="E151" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -6545,21 +6616,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>158</v>
       </c>
       <c r="B152" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="C152" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
       <c r="D152" t="s">
-        <v>649</v>
+        <v>666</v>
       </c>
       <c r="E152" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="F152">
         <v>3</v>
@@ -6571,35 +6642,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>159</v>
       </c>
       <c r="B153" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D153" t="s">
-        <v>650</v>
+        <v>667</v>
       </c>
       <c r="E153" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
         <v>160</v>
       </c>
       <c r="B154" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C154" t="s">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="D154" t="s">
-        <v>651</v>
+        <v>668</v>
       </c>
       <c r="E154" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="G154">
         <v>24</v>
@@ -6608,276 +6679,276 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
         <v>161</v>
       </c>
       <c r="B155" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="D155" t="s">
-        <v>652</v>
+        <v>669</v>
       </c>
       <c r="E155" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
         <v>162</v>
       </c>
       <c r="B156" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="D156" t="s">
-        <v>653</v>
+        <v>670</v>
       </c>
       <c r="E156" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
       <c r="A157" t="s">
         <v>163</v>
       </c>
       <c r="B157" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="C157" t="s">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="D157" t="s">
-        <v>654</v>
+        <v>671</v>
       </c>
       <c r="E157" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="G157">
         <v>39</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8">
       <c r="A158" t="s">
         <v>164</v>
       </c>
       <c r="B158" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C158" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="D158" t="s">
-        <v>655</v>
+        <v>672</v>
       </c>
       <c r="E158" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
       <c r="A159" t="s">
         <v>165</v>
       </c>
       <c r="B159" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="D159" t="s">
-        <v>656</v>
+        <v>673</v>
       </c>
       <c r="E159" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
       <c r="A160" t="s">
         <v>166</v>
       </c>
       <c r="B160" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="C160" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
       <c r="D160" t="s">
-        <v>657</v>
+        <v>674</v>
       </c>
       <c r="E160" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="G160">
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8">
       <c r="A161" t="s">
         <v>167</v>
       </c>
       <c r="B161" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C161" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="D161" t="s">
-        <v>658</v>
+        <v>675</v>
       </c>
       <c r="E161" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
         <v>168</v>
       </c>
       <c r="B162" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="C162" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="D162" t="s">
-        <v>659</v>
+        <v>676</v>
       </c>
       <c r="E162" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
         <v>169</v>
       </c>
       <c r="B163" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C163" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="D163" t="s">
-        <v>660</v>
+        <v>677</v>
       </c>
       <c r="E163" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="G163">
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>170</v>
       </c>
       <c r="B164" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C164" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="D164" t="s">
-        <v>661</v>
+        <v>678</v>
       </c>
       <c r="E164" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="G164">
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>171</v>
       </c>
       <c r="B165" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="D165" t="s">
-        <v>662</v>
+        <v>679</v>
       </c>
       <c r="E165" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>172</v>
       </c>
       <c r="B166" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="D166" t="s">
-        <v>663</v>
+        <v>680</v>
       </c>
       <c r="E166" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>173</v>
       </c>
       <c r="B167" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C167" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="D167" t="s">
-        <v>664</v>
+        <v>681</v>
       </c>
       <c r="E167" t="s">
-        <v>673</v>
+        <v>696</v>
       </c>
       <c r="G167">
         <v>41</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>174</v>
       </c>
       <c r="B168" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="C168" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="D168" t="s">
-        <v>665</v>
+        <v>682</v>
       </c>
       <c r="E168" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>175</v>
       </c>
       <c r="B169" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="C169" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="D169" t="s">
-        <v>666</v>
+        <v>683</v>
       </c>
       <c r="E169" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>176</v>
       </c>
       <c r="B170" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="C170" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="D170" t="s">
-        <v>667</v>
+        <v>684</v>
       </c>
       <c r="E170" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="F170">
         <v>4</v>
@@ -6889,21 +6960,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>177</v>
       </c>
       <c r="B171" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="C171" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="D171" t="s">
-        <v>668</v>
+        <v>685</v>
       </c>
       <c r="E171" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="F171">
         <v>5</v>
@@ -6915,21 +6986,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>178</v>
       </c>
       <c r="B172" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C172" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="D172" t="s">
-        <v>669</v>
+        <v>686</v>
       </c>
       <c r="E172" t="s">
-        <v>675</v>
+        <v>698</v>
       </c>
       <c r="F172">
         <v>6</v>
@@ -6939,6 +7010,108 @@
       </c>
       <c r="H172">
         <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8">
+      <c r="A173" t="s">
+        <v>179</v>
+      </c>
+      <c r="B173" t="s">
+        <v>355</v>
+      </c>
+      <c r="C173" t="s">
+        <v>511</v>
+      </c>
+      <c r="D173" t="s">
+        <v>687</v>
+      </c>
+      <c r="E173" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8">
+      <c r="A174" t="s">
+        <v>180</v>
+      </c>
+      <c r="B174" t="s">
+        <v>356</v>
+      </c>
+      <c r="C174" t="s">
+        <v>511</v>
+      </c>
+      <c r="D174" t="s">
+        <v>688</v>
+      </c>
+      <c r="E174" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8">
+      <c r="A175" t="s">
+        <v>181</v>
+      </c>
+      <c r="B175" t="s">
+        <v>357</v>
+      </c>
+      <c r="C175" t="s">
+        <v>512</v>
+      </c>
+      <c r="D175" t="s">
+        <v>689</v>
+      </c>
+      <c r="E175" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8">
+      <c r="A176" t="s">
+        <v>182</v>
+      </c>
+      <c r="B176" t="s">
+        <v>358</v>
+      </c>
+      <c r="C176" t="s">
+        <v>513</v>
+      </c>
+      <c r="D176" t="s">
+        <v>690</v>
+      </c>
+      <c r="E176" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>183</v>
+      </c>
+      <c r="B177" t="s">
+        <v>359</v>
+      </c>
+      <c r="C177" t="s">
+        <v>514</v>
+      </c>
+      <c r="D177" t="s">
+        <v>691</v>
+      </c>
+      <c r="E177" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>184</v>
+      </c>
+      <c r="B178" t="s">
+        <v>360</v>
+      </c>
+      <c r="C178" t="s">
+        <v>515</v>
+      </c>
+      <c r="D178" t="s">
+        <v>692</v>
+      </c>
+      <c r="E178" t="s">
+        <v>698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update exp table curation and loading
Support sorting exp record to 2 monkey's different dests
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="730">
   <si>
     <t>ephysFN</t>
   </si>
@@ -571,6 +571,30 @@
     <t>Beto-17032020-007</t>
   </si>
   <si>
+    <t>Beto-18032020-001</t>
+  </si>
+  <si>
+    <t>Beto-18032020-002</t>
+  </si>
+  <si>
+    <t>Beto-18032020-003</t>
+  </si>
+  <si>
+    <t>Beto-18032020-004</t>
+  </si>
+  <si>
+    <t>Beto-18032020-005</t>
+  </si>
+  <si>
+    <t>Beto-18032020-006</t>
+  </si>
+  <si>
+    <t>Beto-18032020-007</t>
+  </si>
+  <si>
+    <t>Beto-18032020-008</t>
+  </si>
+  <si>
     <t>191002_Beto_selectivity_basic(1)</t>
   </si>
   <si>
@@ -1099,6 +1123,30 @@
     <t>200317_Beto_generate_integrated(4)</t>
   </si>
   <si>
+    <t>200318_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200318_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200318_Beto_rfMapper_basic(2)</t>
+  </si>
+  <si>
+    <t>200318_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200318_Beto_generate_integrated(2)</t>
+  </si>
+  <si>
+    <t>200318_Beto_generate_integrated(3)</t>
+  </si>
+  <si>
+    <t>200318_Beto_generate_integrated(4)</t>
+  </si>
+  <si>
+    <t>200318_Beto_generate_integrated(5)</t>
+  </si>
+  <si>
     <t>\\storage1.ris.wustl.edu\crponce\Active\Stimuli\2019-Selectivity\2019-10-02a-beto</t>
   </si>
   <si>
@@ -1562,6 +1610,24 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-17-Beto-04\2020-03-17-14-42-52</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-18-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-18-Beto-01\2020-03-18-12-07-15</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-18-Beto-02\2020-03-18-12-21-38</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-18-Beto-03\2020-03-18-12-51-20</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-18-Beto-04\2020-03-18-13-30-57</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-18-Beto-05\2020-03-18-14-10-20</t>
   </si>
   <si>
     <t>Derived from PCs of Ch 29 evolution 191002. 373 images {11*11 in PC2,PC3; PC49 PC50; RND RND space respectively, +10 last gen}</t>
@@ -2461,6 +2527,84 @@
 Completed</t>
   </si>
   <si>
+    <t>001 RFMapping 11:
+-8:8:8 
+Carlos' huge image test
+Completed</t>
+  </si>
+  <si>
+    <t>002 RFMapping starts 11:35
+-8:2:8
+Completed</t>
+  </si>
+  <si>
+    <t>003 RFMapping starts 11:49
+-4:1:4
+8 mins similar RF position
+Completed</t>
+  </si>
+  <si>
+    <t>004 Generate Integrated
+24 [-1.5 1.5 ] 4 1 CMAES
+Trying out basic optimizer, see if it can evolve!
+Seems work, Evolving very fast.
+Seems plateau really fast as well around 10 gens. Only 6 mins! Wow. Maybe 20 blocks
+Why Stuck so early? Gets some local maxima? 
+Completed</t>
+  </si>
+  <si>
+    <t>005 Generate Integrated
+24 [-1.5 1.5 ] 4 1 ZOHA_Sphere_lr_euclid
+24 [-1.5 1.5 ] 4 1 ZOHA_Sphere_lr_euclid_RD
+Test the reduced Dimension Comparison.
+Use the inverse decay exploration range. lr=1.5
+Inverse decay's initial learning rate is too large, should make it smaller. And learning rate * exploration exceeds pi/2 it's insane.
+(Gen 5 explor is 58.3 deg, step is 0.88 or 0.64)
+Gen 12 42 degs, step 0.474, 0.314, this is good.
+Gap exist! But quite small. (only 14 mins now! )
+Plateau around 15 gens
+Completed</t>
+  </si>
+  <si>
+    <t>006 Generate Integrated
+24 [-1.5 1.5 ] 4 1 ZOHA_Sphere_lr_euclid
+24 [-1.5 1.5 ] 4 1 ZOHA_Sphere_lr_euclid_RD
+Redo the reduced Dimension Comparison.
+Use the inverse decay exploration range. Lr=1.2 Decrease this to avoid overshoot. And this makes Sphere lr euclid grow just as fast as CMAES! No delay!
+gen 11, 45 deg 0.321.
+Interestingly, the reduced starts to grow at around gen 12. Making gap smaller.
+Finished in 30 mins
+Completed</t>
+  </si>
+  <si>
+    <t>007 Generate Integrated starts 13:30
+64 [-1.5 -2.5 ] 5 1 ZOHA_Sphere_lr_euclid
+64 [-1.5 -2.5 ] 5 1 ZOHA_Sphere_lr_euclid_RD
+Test the Reduced Dimension for V4 channel on Beto.
+ZOHA full saturates pretty fast!
+Seems there is still a gap and it's not small……
+Wow, gap gets closed…… as expected.
+Really the same as expected! It closes the gap finally.
+takes 35 min to get to 25 blocks! Good job.
+Completed</t>
+  </si>
+  <si>
+    <t>008 Generate Integrated starts 14:10
+64 [-1.5 -2.5 ] 5 1 ZOHA_Sphere_lr_euclid_RD
+64 [-1.5 -2.5 ] 5 1 ZOHA_Sphere_lr_euclid_RD
+Test the Reduced Dimension for V4 channel on Beto.
+See how large is the trial variability.
+The first one saturates pretty fast as well.
+the first one gets even higher than full, seemingly! OMG.
+At gen 10 the step size is around 0.376!
+Oh get back to normal… seems higher than Full evolution is just fluctuation.
+Gen 13 exploration aaround 41.8.
+Around 18 gens the 1st evolution grows again! Find something new to add to the image.
+Gets to ~ 30 gens……
+Add 100mL water to him!
+Completed</t>
+  </si>
+  <si>
     <t>Manifold</t>
   </si>
   <si>
@@ -2477,6 +2621,9 @@
   </si>
   <si>
     <t>Optim_tuning</t>
+  </si>
+  <si>
+    <t>ReducDimen_Evol</t>
   </si>
 </sst>
 </file>
@@ -2834,7 +2981,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H178"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2871,16 +3018,16 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>361</v>
+        <v>377</v>
       </c>
       <c r="D2" t="s">
-        <v>516</v>
+        <v>538</v>
       </c>
       <c r="E2" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2897,16 +3044,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>362</v>
+        <v>378</v>
       </c>
       <c r="D3" t="s">
-        <v>517</v>
+        <v>539</v>
       </c>
       <c r="E3" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2923,16 +3070,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>363</v>
+        <v>379</v>
       </c>
       <c r="D4" t="s">
-        <v>518</v>
+        <v>540</v>
       </c>
       <c r="E4" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -2949,16 +3096,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>364</v>
+        <v>380</v>
       </c>
       <c r="D5" t="s">
-        <v>519</v>
+        <v>541</v>
       </c>
       <c r="E5" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2975,16 +3122,16 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
-        <v>365</v>
+        <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>520</v>
+        <v>542</v>
       </c>
       <c r="E6" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -3001,16 +3148,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>366</v>
+        <v>382</v>
       </c>
       <c r="D7" t="s">
-        <v>521</v>
+        <v>543</v>
       </c>
       <c r="E7" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -3027,16 +3174,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C8" t="s">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="D8" t="s">
-        <v>522</v>
+        <v>544</v>
       </c>
       <c r="E8" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -3053,16 +3200,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C9" t="s">
-        <v>368</v>
+        <v>384</v>
       </c>
       <c r="D9" t="s">
-        <v>523</v>
+        <v>545</v>
       </c>
       <c r="E9" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -3079,16 +3226,16 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C10" t="s">
-        <v>369</v>
+        <v>385</v>
       </c>
       <c r="D10" t="s">
-        <v>524</v>
+        <v>546</v>
       </c>
       <c r="E10" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -3105,16 +3252,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s">
-        <v>370</v>
+        <v>386</v>
       </c>
       <c r="D11" t="s">
-        <v>525</v>
+        <v>547</v>
       </c>
       <c r="E11" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -3131,16 +3278,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C12" t="s">
-        <v>371</v>
+        <v>387</v>
       </c>
       <c r="D12" t="s">
-        <v>526</v>
+        <v>548</v>
       </c>
       <c r="E12" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3157,16 +3304,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>372</v>
+        <v>388</v>
       </c>
       <c r="D13" t="s">
-        <v>527</v>
+        <v>549</v>
       </c>
       <c r="E13" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3183,16 +3330,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>373</v>
+        <v>389</v>
       </c>
       <c r="D14" t="s">
-        <v>528</v>
+        <v>550</v>
       </c>
       <c r="E14" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -3209,16 +3356,16 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>374</v>
+        <v>390</v>
       </c>
       <c r="D15" t="s">
-        <v>529</v>
+        <v>551</v>
       </c>
       <c r="E15" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -3235,16 +3382,16 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>375</v>
+        <v>391</v>
       </c>
       <c r="D16" t="s">
-        <v>530</v>
+        <v>552</v>
       </c>
       <c r="E16" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -3261,16 +3408,16 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
-        <v>376</v>
+        <v>392</v>
       </c>
       <c r="D17" t="s">
-        <v>531</v>
+        <v>553</v>
       </c>
       <c r="E17" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -3287,16 +3434,16 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s">
-        <v>377</v>
+        <v>393</v>
       </c>
       <c r="D18" t="s">
-        <v>532</v>
+        <v>554</v>
       </c>
       <c r="E18" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -3313,16 +3460,16 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C19" t="s">
-        <v>378</v>
+        <v>394</v>
       </c>
       <c r="D19" t="s">
-        <v>533</v>
+        <v>555</v>
       </c>
       <c r="E19" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -3339,16 +3486,16 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C20" t="s">
-        <v>379</v>
+        <v>395</v>
       </c>
       <c r="D20" t="s">
-        <v>534</v>
+        <v>556</v>
       </c>
       <c r="E20" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3365,16 +3512,16 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C21" t="s">
-        <v>380</v>
+        <v>396</v>
       </c>
       <c r="D21" t="s">
-        <v>535</v>
+        <v>557</v>
       </c>
       <c r="E21" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3391,16 +3538,16 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="C22" t="s">
-        <v>381</v>
+        <v>397</v>
       </c>
       <c r="D22" t="s">
-        <v>536</v>
+        <v>558</v>
       </c>
       <c r="E22" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -3417,16 +3564,16 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C23" t="s">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="D23" t="s">
-        <v>537</v>
+        <v>559</v>
       </c>
       <c r="E23" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -3443,16 +3590,16 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C24" t="s">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="D24" t="s">
-        <v>538</v>
+        <v>560</v>
       </c>
       <c r="E24" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -3469,16 +3616,16 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="C25" t="s">
-        <v>384</v>
+        <v>400</v>
       </c>
       <c r="D25" t="s">
-        <v>539</v>
+        <v>561</v>
       </c>
       <c r="E25" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -3495,16 +3642,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C26" t="s">
-        <v>385</v>
+        <v>401</v>
       </c>
       <c r="D26" t="s">
-        <v>540</v>
+        <v>562</v>
       </c>
       <c r="E26" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -3521,16 +3668,16 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C27" t="s">
-        <v>386</v>
+        <v>402</v>
       </c>
       <c r="D27" t="s">
-        <v>541</v>
+        <v>563</v>
       </c>
       <c r="E27" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -3547,16 +3694,16 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="C28" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="D28" t="s">
-        <v>542</v>
+        <v>564</v>
       </c>
       <c r="E28" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -3573,16 +3720,16 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C29" t="s">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="D29" t="s">
-        <v>543</v>
+        <v>565</v>
       </c>
       <c r="E29" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -3599,16 +3746,16 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C30" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="D30" t="s">
-        <v>544</v>
+        <v>566</v>
       </c>
       <c r="E30" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -3625,16 +3772,16 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C31" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="D31" t="s">
-        <v>545</v>
+        <v>567</v>
       </c>
       <c r="E31" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -3651,16 +3798,16 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C32" t="s">
-        <v>391</v>
+        <v>407</v>
       </c>
       <c r="D32" t="s">
-        <v>546</v>
+        <v>568</v>
       </c>
       <c r="E32" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -3677,16 +3824,16 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="C33" t="s">
-        <v>392</v>
+        <v>408</v>
       </c>
       <c r="D33" t="s">
-        <v>547</v>
+        <v>569</v>
       </c>
       <c r="E33" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -3703,16 +3850,16 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C34" t="s">
-        <v>393</v>
+        <v>409</v>
       </c>
       <c r="D34" t="s">
-        <v>548</v>
+        <v>570</v>
       </c>
       <c r="E34" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -3729,16 +3876,16 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="C35" t="s">
-        <v>394</v>
+        <v>410</v>
       </c>
       <c r="D35" t="s">
-        <v>549</v>
+        <v>571</v>
       </c>
       <c r="E35" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -3755,16 +3902,16 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C36" t="s">
-        <v>395</v>
+        <v>411</v>
       </c>
       <c r="D36" t="s">
-        <v>550</v>
+        <v>572</v>
       </c>
       <c r="E36" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -3781,16 +3928,16 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C37" t="s">
-        <v>396</v>
+        <v>412</v>
       </c>
       <c r="D37" t="s">
-        <v>551</v>
+        <v>573</v>
       </c>
       <c r="E37" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -3807,16 +3954,16 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C38" t="s">
-        <v>397</v>
+        <v>413</v>
       </c>
       <c r="D38" t="s">
-        <v>552</v>
+        <v>574</v>
       </c>
       <c r="E38" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -3833,16 +3980,16 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="C39" t="s">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="D39" t="s">
-        <v>553</v>
+        <v>575</v>
       </c>
       <c r="E39" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -3859,16 +4006,16 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="C40" t="s">
-        <v>399</v>
+        <v>415</v>
       </c>
       <c r="D40" t="s">
-        <v>554</v>
+        <v>576</v>
       </c>
       <c r="E40" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -3885,16 +4032,16 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C41" t="s">
-        <v>400</v>
+        <v>416</v>
       </c>
       <c r="D41" t="s">
-        <v>555</v>
+        <v>577</v>
       </c>
       <c r="E41" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -3911,16 +4058,16 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C42" t="s">
-        <v>401</v>
+        <v>417</v>
       </c>
       <c r="D42" t="s">
-        <v>556</v>
+        <v>578</v>
       </c>
       <c r="E42" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -3937,16 +4084,16 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="C43" t="s">
-        <v>402</v>
+        <v>418</v>
       </c>
       <c r="D43" t="s">
-        <v>557</v>
+        <v>579</v>
       </c>
       <c r="E43" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -3963,16 +4110,16 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="C44" t="s">
-        <v>403</v>
+        <v>419</v>
       </c>
       <c r="D44" t="s">
-        <v>558</v>
+        <v>580</v>
       </c>
       <c r="E44" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -3989,16 +4136,16 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C45" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="D45" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="E45" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -4015,16 +4162,16 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="C46" t="s">
-        <v>405</v>
+        <v>421</v>
       </c>
       <c r="D46" t="s">
-        <v>560</v>
+        <v>582</v>
       </c>
       <c r="E46" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -4041,16 +4188,16 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C47" t="s">
-        <v>406</v>
+        <v>422</v>
       </c>
       <c r="D47" t="s">
-        <v>561</v>
+        <v>583</v>
       </c>
       <c r="E47" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -4067,16 +4214,16 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="C48" t="s">
-        <v>407</v>
+        <v>423</v>
       </c>
       <c r="D48" t="s">
-        <v>562</v>
+        <v>584</v>
       </c>
       <c r="E48" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F48">
         <v>23</v>
@@ -4093,16 +4240,16 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C49" t="s">
-        <v>408</v>
+        <v>424</v>
       </c>
       <c r="D49" t="s">
-        <v>563</v>
+        <v>585</v>
       </c>
       <c r="E49" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F49">
         <v>23</v>
@@ -4119,16 +4266,16 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="C50" t="s">
-        <v>409</v>
+        <v>425</v>
       </c>
       <c r="D50" t="s">
-        <v>564</v>
+        <v>586</v>
       </c>
       <c r="E50" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F50">
         <v>24</v>
@@ -4145,16 +4292,16 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C51" t="s">
-        <v>410</v>
+        <v>426</v>
       </c>
       <c r="D51" t="s">
-        <v>565</v>
+        <v>587</v>
       </c>
       <c r="E51" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -4171,16 +4318,16 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C52" t="s">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="D52" t="s">
-        <v>566</v>
+        <v>588</v>
       </c>
       <c r="E52" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F52">
         <v>24</v>
@@ -4197,13 +4344,13 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="C53" t="s">
-        <v>412</v>
+        <v>428</v>
       </c>
       <c r="D53" t="s">
-        <v>567</v>
+        <v>589</v>
       </c>
       <c r="F53">
         <v>24</v>
@@ -4220,16 +4367,16 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="C54" t="s">
-        <v>413</v>
+        <v>429</v>
       </c>
       <c r="D54" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="E54" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -4246,16 +4393,16 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C55" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="D55" t="s">
-        <v>569</v>
+        <v>591</v>
       </c>
       <c r="E55" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F55">
         <v>25</v>
@@ -4272,16 +4419,16 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C56" t="s">
-        <v>415</v>
+        <v>431</v>
       </c>
       <c r="D56" t="s">
-        <v>570</v>
+        <v>592</v>
       </c>
       <c r="E56" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F56">
         <v>25</v>
@@ -4298,16 +4445,16 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C57" t="s">
-        <v>416</v>
+        <v>432</v>
       </c>
       <c r="D57" t="s">
-        <v>571</v>
+        <v>593</v>
       </c>
       <c r="E57" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -4324,16 +4471,16 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="C58" t="s">
-        <v>417</v>
+        <v>433</v>
       </c>
       <c r="D58" t="s">
-        <v>572</v>
+        <v>594</v>
       </c>
       <c r="E58" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -4350,16 +4497,16 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="C59" t="s">
-        <v>418</v>
+        <v>434</v>
       </c>
       <c r="D59" t="s">
-        <v>573</v>
+        <v>595</v>
       </c>
       <c r="E59" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -4376,16 +4523,16 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="C60" t="s">
-        <v>419</v>
+        <v>435</v>
       </c>
       <c r="D60" t="s">
-        <v>574</v>
+        <v>596</v>
       </c>
       <c r="E60" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F60">
         <v>27</v>
@@ -4402,16 +4549,16 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="C61" t="s">
-        <v>420</v>
+        <v>436</v>
       </c>
       <c r="D61" t="s">
-        <v>575</v>
+        <v>597</v>
       </c>
       <c r="E61" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F61">
         <v>27</v>
@@ -4428,16 +4575,16 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="C62" t="s">
-        <v>421</v>
+        <v>437</v>
       </c>
       <c r="D62" t="s">
-        <v>576</v>
+        <v>598</v>
       </c>
       <c r="E62" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F62">
         <v>27</v>
@@ -4454,16 +4601,16 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C63" t="s">
-        <v>422</v>
+        <v>438</v>
       </c>
       <c r="D63" t="s">
-        <v>577</v>
+        <v>599</v>
       </c>
       <c r="E63" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -4480,16 +4627,16 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="C64" t="s">
-        <v>423</v>
+        <v>439</v>
       </c>
       <c r="D64" t="s">
-        <v>578</v>
+        <v>600</v>
       </c>
       <c r="E64" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -4506,16 +4653,16 @@
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C65" t="s">
-        <v>424</v>
+        <v>440</v>
       </c>
       <c r="D65" t="s">
-        <v>579</v>
+        <v>601</v>
       </c>
       <c r="E65" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -4532,16 +4679,16 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C66" t="s">
-        <v>425</v>
+        <v>441</v>
       </c>
       <c r="D66" t="s">
-        <v>580</v>
+        <v>602</v>
       </c>
       <c r="E66" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -4558,16 +4705,16 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="C67" t="s">
-        <v>423</v>
+        <v>439</v>
       </c>
       <c r="D67" t="s">
-        <v>581</v>
+        <v>603</v>
       </c>
       <c r="E67" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -4584,16 +4731,16 @@
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C68" t="s">
-        <v>426</v>
+        <v>442</v>
       </c>
       <c r="D68" t="s">
-        <v>582</v>
+        <v>604</v>
       </c>
       <c r="E68" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -4610,16 +4757,16 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C69" t="s">
-        <v>427</v>
+        <v>443</v>
       </c>
       <c r="D69" t="s">
-        <v>583</v>
+        <v>605</v>
       </c>
       <c r="E69" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -4636,16 +4783,16 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C70" t="s">
-        <v>428</v>
+        <v>444</v>
       </c>
       <c r="D70" t="s">
-        <v>584</v>
+        <v>606</v>
       </c>
       <c r="E70" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -4662,16 +4809,16 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C71" t="s">
-        <v>429</v>
+        <v>445</v>
       </c>
       <c r="D71" t="s">
-        <v>585</v>
+        <v>607</v>
       </c>
       <c r="E71" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -4688,16 +4835,16 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C72" t="s">
-        <v>430</v>
+        <v>446</v>
       </c>
       <c r="D72" t="s">
-        <v>586</v>
+        <v>608</v>
       </c>
       <c r="E72" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -4714,16 +4861,16 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="C73" t="s">
-        <v>431</v>
+        <v>447</v>
       </c>
       <c r="D73" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="E73" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -4740,16 +4887,16 @@
         <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C74" t="s">
-        <v>432</v>
+        <v>448</v>
       </c>
       <c r="D74" t="s">
-        <v>588</v>
+        <v>610</v>
       </c>
       <c r="E74" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -4766,16 +4913,16 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C75" t="s">
-        <v>433</v>
+        <v>449</v>
       </c>
       <c r="D75" t="s">
-        <v>589</v>
+        <v>611</v>
       </c>
       <c r="E75" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -4792,16 +4939,16 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="C76" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
       <c r="D76" t="s">
-        <v>590</v>
+        <v>612</v>
       </c>
       <c r="E76" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -4818,16 +4965,16 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="C77" t="s">
-        <v>435</v>
+        <v>451</v>
       </c>
       <c r="D77" t="s">
-        <v>591</v>
+        <v>613</v>
       </c>
       <c r="E77" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -4844,16 +4991,16 @@
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="C78" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="D78" t="s">
-        <v>592</v>
+        <v>614</v>
       </c>
       <c r="E78" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -4870,16 +5017,16 @@
         <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="C79" t="s">
-        <v>437</v>
+        <v>453</v>
       </c>
       <c r="D79" t="s">
-        <v>593</v>
+        <v>615</v>
       </c>
       <c r="E79" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -4896,16 +5043,16 @@
         <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C80" t="s">
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="D80" t="s">
-        <v>594</v>
+        <v>616</v>
       </c>
       <c r="E80" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -4922,13 +5069,13 @@
         <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="C81" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="D81" t="s">
-        <v>595</v>
+        <v>617</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -4945,13 +5092,13 @@
         <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C82" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="D82" t="s">
-        <v>596</v>
+        <v>618</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -4968,13 +5115,13 @@
         <v>89</v>
       </c>
       <c r="C83" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="D83" t="s">
-        <v>597</v>
+        <v>619</v>
       </c>
       <c r="E83" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -4991,16 +5138,16 @@
         <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C84" t="s">
-        <v>440</v>
+        <v>456</v>
       </c>
       <c r="D84" t="s">
-        <v>598</v>
+        <v>620</v>
       </c>
       <c r="E84" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -5017,16 +5164,16 @@
         <v>91</v>
       </c>
       <c r="B85" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="C85" t="s">
-        <v>441</v>
+        <v>457</v>
       </c>
       <c r="D85" t="s">
-        <v>599</v>
+        <v>621</v>
       </c>
       <c r="E85" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F85">
         <v>35</v>
@@ -5043,16 +5190,16 @@
         <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="C86" t="s">
-        <v>442</v>
+        <v>458</v>
       </c>
       <c r="D86" t="s">
-        <v>600</v>
+        <v>622</v>
       </c>
       <c r="E86" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -5069,16 +5216,16 @@
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C87" t="s">
-        <v>443</v>
+        <v>459</v>
       </c>
       <c r="D87" t="s">
-        <v>601</v>
+        <v>623</v>
       </c>
       <c r="E87" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F87">
         <v>36</v>
@@ -5095,16 +5242,16 @@
         <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="C88" t="s">
-        <v>444</v>
+        <v>460</v>
       </c>
       <c r="D88" t="s">
-        <v>602</v>
+        <v>624</v>
       </c>
       <c r="E88" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -5121,16 +5268,16 @@
         <v>95</v>
       </c>
       <c r="B89" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="C89" t="s">
-        <v>445</v>
+        <v>461</v>
       </c>
       <c r="D89" t="s">
-        <v>603</v>
+        <v>625</v>
       </c>
       <c r="E89" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -5147,16 +5294,16 @@
         <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C90" t="s">
-        <v>446</v>
+        <v>462</v>
       </c>
       <c r="D90" t="s">
-        <v>604</v>
+        <v>626</v>
       </c>
       <c r="E90" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F90">
         <v>37</v>
@@ -5173,16 +5320,16 @@
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="C91" t="s">
-        <v>447</v>
+        <v>463</v>
       </c>
       <c r="D91" t="s">
-        <v>605</v>
+        <v>627</v>
       </c>
       <c r="E91" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -5199,16 +5346,16 @@
         <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="C92" t="s">
-        <v>448</v>
+        <v>464</v>
       </c>
       <c r="D92" t="s">
-        <v>606</v>
+        <v>628</v>
       </c>
       <c r="E92" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F92">
         <v>38</v>
@@ -5225,16 +5372,16 @@
         <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C93" t="s">
-        <v>449</v>
+        <v>465</v>
       </c>
       <c r="D93" t="s">
-        <v>607</v>
+        <v>629</v>
       </c>
       <c r="E93" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -5251,16 +5398,16 @@
         <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="C94" t="s">
-        <v>450</v>
+        <v>466</v>
       </c>
       <c r="D94" t="s">
-        <v>608</v>
+        <v>630</v>
       </c>
       <c r="E94" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -5277,16 +5424,16 @@
         <v>101</v>
       </c>
       <c r="B95" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="C95" t="s">
-        <v>451</v>
+        <v>467</v>
       </c>
       <c r="D95" t="s">
-        <v>609</v>
+        <v>631</v>
       </c>
       <c r="E95" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F95">
         <v>39</v>
@@ -5303,16 +5450,16 @@
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C96" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="D96" t="s">
-        <v>610</v>
+        <v>632</v>
       </c>
       <c r="E96" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -5329,16 +5476,16 @@
         <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="C97" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
       <c r="D97" t="s">
-        <v>611</v>
+        <v>633</v>
       </c>
       <c r="E97" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -5355,16 +5502,16 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C98" t="s">
-        <v>454</v>
+        <v>470</v>
       </c>
       <c r="D98" t="s">
-        <v>612</v>
+        <v>634</v>
       </c>
       <c r="E98" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -5381,16 +5528,16 @@
         <v>105</v>
       </c>
       <c r="B99" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C99" t="s">
-        <v>455</v>
+        <v>471</v>
       </c>
       <c r="D99" t="s">
-        <v>613</v>
+        <v>635</v>
       </c>
       <c r="E99" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -5407,16 +5554,16 @@
         <v>106</v>
       </c>
       <c r="B100" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>456</v>
+        <v>472</v>
       </c>
       <c r="D100" t="s">
-        <v>614</v>
+        <v>636</v>
       </c>
       <c r="E100" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F100">
         <v>41</v>
@@ -5433,16 +5580,16 @@
         <v>107</v>
       </c>
       <c r="B101" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="C101" t="s">
-        <v>457</v>
+        <v>473</v>
       </c>
       <c r="D101" t="s">
-        <v>615</v>
+        <v>637</v>
       </c>
       <c r="E101" t="s">
-        <v>694</v>
+        <v>724</v>
       </c>
       <c r="F101">
         <v>41</v>
@@ -5453,16 +5600,16 @@
         <v>108</v>
       </c>
       <c r="B102" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="C102" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="D102" t="s">
-        <v>616</v>
+        <v>638</v>
       </c>
       <c r="E102" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -5479,16 +5626,16 @@
         <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="C103" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="D103" t="s">
-        <v>617</v>
+        <v>639</v>
       </c>
       <c r="E103" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -5505,16 +5652,16 @@
         <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C104" t="s">
-        <v>460</v>
+        <v>476</v>
       </c>
       <c r="D104" t="s">
-        <v>618</v>
+        <v>640</v>
       </c>
       <c r="E104" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F104">
         <v>42</v>
@@ -5531,16 +5678,16 @@
         <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="C105" t="s">
-        <v>461</v>
+        <v>477</v>
       </c>
       <c r="D105" t="s">
-        <v>619</v>
+        <v>641</v>
       </c>
       <c r="E105" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -5557,16 +5704,16 @@
         <v>112</v>
       </c>
       <c r="B106" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="C106" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="D106" t="s">
-        <v>620</v>
+        <v>642</v>
       </c>
       <c r="E106" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -5583,16 +5730,16 @@
         <v>113</v>
       </c>
       <c r="B107" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="C107" t="s">
-        <v>462</v>
+        <v>478</v>
       </c>
       <c r="D107" t="s">
-        <v>621</v>
+        <v>643</v>
       </c>
       <c r="E107" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F107">
         <v>43</v>
@@ -5609,16 +5756,16 @@
         <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C108" t="s">
-        <v>463</v>
+        <v>479</v>
       </c>
       <c r="D108" t="s">
-        <v>622</v>
+        <v>644</v>
       </c>
       <c r="E108" t="s">
-        <v>694</v>
+        <v>724</v>
       </c>
       <c r="F108">
         <v>43</v>
@@ -5629,16 +5776,16 @@
         <v>115</v>
       </c>
       <c r="B109" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="C109" t="s">
-        <v>463</v>
+        <v>479</v>
       </c>
       <c r="D109" t="s">
-        <v>623</v>
+        <v>645</v>
       </c>
       <c r="E109" t="s">
-        <v>694</v>
+        <v>724</v>
       </c>
       <c r="F109">
         <v>43</v>
@@ -5649,16 +5796,16 @@
         <v>116</v>
       </c>
       <c r="B110" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="C110" t="s">
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="D110" t="s">
-        <v>624</v>
+        <v>646</v>
       </c>
       <c r="E110" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -5675,16 +5822,16 @@
         <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C111" t="s">
-        <v>465</v>
+        <v>481</v>
       </c>
       <c r="D111" t="s">
-        <v>625</v>
+        <v>647</v>
       </c>
       <c r="E111" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -5701,16 +5848,16 @@
         <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C112" t="s">
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="D112" t="s">
-        <v>626</v>
+        <v>648</v>
       </c>
       <c r="E112" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F112">
         <v>44</v>
@@ -5727,16 +5874,16 @@
         <v>119</v>
       </c>
       <c r="B113" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="C113" t="s">
-        <v>466</v>
+        <v>482</v>
       </c>
       <c r="D113" t="s">
-        <v>627</v>
+        <v>649</v>
       </c>
       <c r="E113" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -5753,16 +5900,16 @@
         <v>120</v>
       </c>
       <c r="B114" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C114" t="s">
-        <v>467</v>
+        <v>483</v>
       </c>
       <c r="D114" t="s">
-        <v>628</v>
+        <v>650</v>
       </c>
       <c r="E114" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -5779,16 +5926,16 @@
         <v>121</v>
       </c>
       <c r="B115" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C115" t="s">
-        <v>468</v>
+        <v>484</v>
       </c>
       <c r="D115" t="s">
-        <v>629</v>
+        <v>651</v>
       </c>
       <c r="E115" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="F115">
         <v>45</v>
@@ -5805,16 +5952,16 @@
         <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C116" t="s">
-        <v>469</v>
+        <v>485</v>
       </c>
       <c r="D116" t="s">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="E116" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -5825,16 +5972,16 @@
         <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C117" t="s">
-        <v>470</v>
+        <v>486</v>
       </c>
       <c r="D117" t="s">
-        <v>631</v>
+        <v>653</v>
       </c>
       <c r="E117" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -5851,16 +5998,16 @@
         <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="C118" t="s">
-        <v>471</v>
+        <v>487</v>
       </c>
       <c r="D118" t="s">
-        <v>632</v>
+        <v>654</v>
       </c>
       <c r="E118" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="H118">
         <v>2</v>
@@ -5871,16 +6018,16 @@
         <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="C119" t="s">
-        <v>472</v>
+        <v>488</v>
       </c>
       <c r="D119" t="s">
-        <v>633</v>
+        <v>655</v>
       </c>
       <c r="E119" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -5897,16 +6044,16 @@
         <v>126</v>
       </c>
       <c r="B120" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C120" t="s">
-        <v>473</v>
+        <v>489</v>
       </c>
       <c r="D120" t="s">
-        <v>634</v>
+        <v>656</v>
       </c>
       <c r="E120" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -5923,16 +6070,16 @@
         <v>127</v>
       </c>
       <c r="B121" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C121" t="s">
-        <v>474</v>
+        <v>490</v>
       </c>
       <c r="D121" t="s">
-        <v>635</v>
+        <v>657</v>
       </c>
       <c r="E121" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="H121">
         <v>2</v>
@@ -5943,16 +6090,16 @@
         <v>128</v>
       </c>
       <c r="B122" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="C122" t="s">
-        <v>475</v>
+        <v>491</v>
       </c>
       <c r="D122" t="s">
-        <v>636</v>
+        <v>658</v>
       </c>
       <c r="E122" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -5969,13 +6116,13 @@
         <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C123" t="s">
-        <v>476</v>
+        <v>492</v>
       </c>
       <c r="D123" t="s">
-        <v>637</v>
+        <v>659</v>
       </c>
       <c r="G123">
         <v>41</v>
@@ -5989,16 +6136,16 @@
         <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="C124" t="s">
-        <v>474</v>
+        <v>490</v>
       </c>
       <c r="D124" t="s">
-        <v>638</v>
+        <v>660</v>
       </c>
       <c r="E124" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="H124">
         <v>3</v>
@@ -6009,16 +6156,16 @@
         <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C125" t="s">
-        <v>474</v>
+        <v>490</v>
       </c>
       <c r="D125" t="s">
-        <v>639</v>
+        <v>661</v>
       </c>
       <c r="E125" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -6029,16 +6176,16 @@
         <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="C126" t="s">
-        <v>477</v>
+        <v>493</v>
       </c>
       <c r="D126" t="s">
-        <v>640</v>
+        <v>662</v>
       </c>
       <c r="E126" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="F126">
         <v>5</v>
@@ -6055,16 +6202,16 @@
         <v>133</v>
       </c>
       <c r="B127" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="C127" t="s">
-        <v>478</v>
+        <v>494</v>
       </c>
       <c r="D127" t="s">
-        <v>641</v>
+        <v>663</v>
       </c>
       <c r="E127" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -6072,13 +6219,13 @@
         <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C128" t="s">
-        <v>479</v>
+        <v>495</v>
       </c>
       <c r="D128" t="s">
-        <v>642</v>
+        <v>664</v>
       </c>
       <c r="G128">
         <v>26</v>
@@ -6092,16 +6239,16 @@
         <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="C129" t="s">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="D129" t="s">
-        <v>643</v>
+        <v>665</v>
       </c>
       <c r="E129" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -6118,13 +6265,13 @@
         <v>136</v>
       </c>
       <c r="B130" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C130" t="s">
-        <v>481</v>
+        <v>497</v>
       </c>
       <c r="D130" t="s">
-        <v>644</v>
+        <v>666</v>
       </c>
       <c r="H130">
         <v>2</v>
@@ -6135,13 +6282,13 @@
         <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C131" t="s">
-        <v>481</v>
+        <v>497</v>
       </c>
       <c r="D131" t="s">
-        <v>645</v>
+        <v>667</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -6152,16 +6299,16 @@
         <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C132" t="s">
-        <v>482</v>
+        <v>498</v>
       </c>
       <c r="D132" t="s">
-        <v>646</v>
+        <v>668</v>
       </c>
       <c r="E132" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -6178,16 +6325,16 @@
         <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C133" t="s">
-        <v>483</v>
+        <v>499</v>
       </c>
       <c r="D133" t="s">
-        <v>647</v>
+        <v>669</v>
       </c>
       <c r="E133" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="F133">
         <v>7</v>
@@ -6204,16 +6351,16 @@
         <v>140</v>
       </c>
       <c r="B134" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="C134" t="s">
-        <v>484</v>
+        <v>500</v>
       </c>
       <c r="D134" t="s">
-        <v>648</v>
+        <v>670</v>
       </c>
       <c r="E134" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="H134">
         <v>0.75</v>
@@ -6224,16 +6371,16 @@
         <v>141</v>
       </c>
       <c r="B135" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C135" t="s">
-        <v>484</v>
+        <v>500</v>
       </c>
       <c r="D135" t="s">
-        <v>649</v>
+        <v>671</v>
       </c>
       <c r="E135" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="H135">
         <v>2</v>
@@ -6244,16 +6391,16 @@
         <v>142</v>
       </c>
       <c r="B136" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="C136" t="s">
-        <v>485</v>
+        <v>501</v>
       </c>
       <c r="D136" t="s">
-        <v>650</v>
+        <v>672</v>
       </c>
       <c r="E136" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -6270,16 +6417,16 @@
         <v>143</v>
       </c>
       <c r="B137" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="C137" t="s">
-        <v>486</v>
+        <v>502</v>
       </c>
       <c r="D137" t="s">
-        <v>651</v>
+        <v>673</v>
       </c>
       <c r="E137" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="F137">
         <v>2</v>
@@ -6296,16 +6443,16 @@
         <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C138" t="s">
-        <v>487</v>
+        <v>503</v>
       </c>
       <c r="D138" t="s">
-        <v>652</v>
+        <v>674</v>
       </c>
       <c r="E138" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="F138">
         <v>3</v>
@@ -6322,16 +6469,16 @@
         <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="C139" t="s">
-        <v>488</v>
+        <v>504</v>
       </c>
       <c r="D139" t="s">
-        <v>653</v>
+        <v>675</v>
       </c>
       <c r="E139" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="F139">
         <v>4</v>
@@ -6348,16 +6495,16 @@
         <v>146</v>
       </c>
       <c r="B140" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C140" t="s">
-        <v>489</v>
+        <v>505</v>
       </c>
       <c r="D140" t="s">
-        <v>654</v>
+        <v>676</v>
       </c>
       <c r="E140" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="H140">
         <v>0.75</v>
@@ -6368,16 +6515,16 @@
         <v>147</v>
       </c>
       <c r="B141" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="C141" t="s">
-        <v>489</v>
+        <v>505</v>
       </c>
       <c r="D141" t="s">
-        <v>655</v>
+        <v>677</v>
       </c>
       <c r="E141" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="H141">
         <v>2</v>
@@ -6388,16 +6535,16 @@
         <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="C142" t="s">
-        <v>490</v>
+        <v>506</v>
       </c>
       <c r="D142" t="s">
-        <v>656</v>
+        <v>678</v>
       </c>
       <c r="E142" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="F142">
         <v>5</v>
@@ -6414,16 +6561,16 @@
         <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="C143" t="s">
-        <v>491</v>
+        <v>507</v>
       </c>
       <c r="D143" t="s">
-        <v>657</v>
+        <v>679</v>
       </c>
       <c r="E143" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="F143">
         <v>6</v>
@@ -6440,16 +6587,16 @@
         <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="C144" t="s">
-        <v>492</v>
+        <v>508</v>
       </c>
       <c r="D144" t="s">
-        <v>658</v>
+        <v>680</v>
       </c>
       <c r="E144" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="H144">
         <v>0.75</v>
@@ -6460,16 +6607,16 @@
         <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="C145" t="s">
-        <v>492</v>
+        <v>508</v>
       </c>
       <c r="D145" t="s">
-        <v>659</v>
+        <v>681</v>
       </c>
       <c r="E145" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="H145">
         <v>2</v>
@@ -6480,16 +6627,16 @@
         <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="C146" t="s">
-        <v>493</v>
+        <v>509</v>
       </c>
       <c r="D146" t="s">
-        <v>660</v>
+        <v>682</v>
       </c>
       <c r="E146" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="F146">
         <v>101</v>
@@ -6506,16 +6653,16 @@
         <v>153</v>
       </c>
       <c r="B147" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C147" t="s">
-        <v>494</v>
+        <v>510</v>
       </c>
       <c r="D147" t="s">
-        <v>661</v>
+        <v>683</v>
       </c>
       <c r="E147" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="G147">
         <v>24</v>
@@ -6529,16 +6676,16 @@
         <v>154</v>
       </c>
       <c r="B148" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="C148" t="s">
-        <v>495</v>
+        <v>511</v>
       </c>
       <c r="D148" t="s">
-        <v>662</v>
+        <v>684</v>
       </c>
       <c r="E148" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -6555,16 +6702,16 @@
         <v>155</v>
       </c>
       <c r="B149" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C149" t="s">
-        <v>496</v>
+        <v>512</v>
       </c>
       <c r="D149" t="s">
-        <v>663</v>
+        <v>685</v>
       </c>
       <c r="E149" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="H149">
         <v>0.75</v>
@@ -6575,16 +6722,16 @@
         <v>156</v>
       </c>
       <c r="B150" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="C150" t="s">
-        <v>496</v>
+        <v>512</v>
       </c>
       <c r="D150" t="s">
-        <v>664</v>
+        <v>686</v>
       </c>
       <c r="E150" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="H150">
         <v>2</v>
@@ -6595,16 +6742,16 @@
         <v>157</v>
       </c>
       <c r="B151" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="C151" t="s">
-        <v>497</v>
+        <v>513</v>
       </c>
       <c r="D151" t="s">
-        <v>665</v>
+        <v>687</v>
       </c>
       <c r="E151" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -6621,16 +6768,16 @@
         <v>158</v>
       </c>
       <c r="B152" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="C152" t="s">
-        <v>498</v>
+        <v>514</v>
       </c>
       <c r="D152" t="s">
-        <v>666</v>
+        <v>688</v>
       </c>
       <c r="E152" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="F152">
         <v>3</v>
@@ -6647,13 +6794,13 @@
         <v>159</v>
       </c>
       <c r="B153" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="D153" t="s">
-        <v>667</v>
+        <v>689</v>
       </c>
       <c r="E153" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -6661,16 +6808,16 @@
         <v>160</v>
       </c>
       <c r="B154" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="C154" t="s">
-        <v>499</v>
+        <v>515</v>
       </c>
       <c r="D154" t="s">
-        <v>668</v>
+        <v>690</v>
       </c>
       <c r="E154" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="G154">
         <v>24</v>
@@ -6684,13 +6831,13 @@
         <v>161</v>
       </c>
       <c r="B155" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="D155" t="s">
-        <v>669</v>
+        <v>691</v>
       </c>
       <c r="E155" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -6698,13 +6845,13 @@
         <v>162</v>
       </c>
       <c r="B156" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="D156" t="s">
-        <v>670</v>
+        <v>692</v>
       </c>
       <c r="E156" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -6712,16 +6859,16 @@
         <v>163</v>
       </c>
       <c r="B157" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="C157" t="s">
-        <v>500</v>
+        <v>516</v>
       </c>
       <c r="D157" t="s">
-        <v>671</v>
+        <v>693</v>
       </c>
       <c r="E157" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="G157">
         <v>39</v>
@@ -6732,16 +6879,16 @@
         <v>164</v>
       </c>
       <c r="B158" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="C158" t="s">
-        <v>501</v>
+        <v>517</v>
       </c>
       <c r="D158" t="s">
-        <v>672</v>
+        <v>694</v>
       </c>
       <c r="E158" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -6749,13 +6896,13 @@
         <v>165</v>
       </c>
       <c r="B159" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="D159" t="s">
-        <v>673</v>
+        <v>695</v>
       </c>
       <c r="E159" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -6763,16 +6910,16 @@
         <v>166</v>
       </c>
       <c r="B160" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C160" t="s">
-        <v>502</v>
+        <v>518</v>
       </c>
       <c r="D160" t="s">
-        <v>674</v>
+        <v>696</v>
       </c>
       <c r="E160" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="G160">
         <v>39</v>
@@ -6783,16 +6930,16 @@
         <v>167</v>
       </c>
       <c r="B161" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="C161" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="D161" t="s">
-        <v>675</v>
+        <v>697</v>
       </c>
       <c r="E161" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -6800,16 +6947,16 @@
         <v>168</v>
       </c>
       <c r="B162" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="C162" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="D162" t="s">
-        <v>676</v>
+        <v>698</v>
       </c>
       <c r="E162" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -6817,16 +6964,16 @@
         <v>169</v>
       </c>
       <c r="B163" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="C163" t="s">
-        <v>504</v>
+        <v>520</v>
       </c>
       <c r="D163" t="s">
-        <v>677</v>
+        <v>699</v>
       </c>
       <c r="E163" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="G163">
         <v>39</v>
@@ -6837,16 +6984,16 @@
         <v>170</v>
       </c>
       <c r="B164" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="C164" t="s">
-        <v>505</v>
+        <v>521</v>
       </c>
       <c r="D164" t="s">
-        <v>678</v>
+        <v>700</v>
       </c>
       <c r="E164" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="G164">
         <v>25</v>
@@ -6857,13 +7004,13 @@
         <v>171</v>
       </c>
       <c r="B165" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="D165" t="s">
-        <v>679</v>
+        <v>701</v>
       </c>
       <c r="E165" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6871,13 +7018,13 @@
         <v>172</v>
       </c>
       <c r="B166" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="D166" t="s">
-        <v>680</v>
+        <v>702</v>
       </c>
       <c r="E166" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6885,16 +7032,16 @@
         <v>173</v>
       </c>
       <c r="B167" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="C167" t="s">
-        <v>506</v>
+        <v>522</v>
       </c>
       <c r="D167" t="s">
-        <v>681</v>
+        <v>703</v>
       </c>
       <c r="E167" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="G167">
         <v>41</v>
@@ -6905,16 +7052,16 @@
         <v>174</v>
       </c>
       <c r="B168" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="C168" t="s">
-        <v>507</v>
+        <v>523</v>
       </c>
       <c r="D168" t="s">
-        <v>682</v>
+        <v>704</v>
       </c>
       <c r="E168" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6922,16 +7069,16 @@
         <v>175</v>
       </c>
       <c r="B169" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="C169" t="s">
-        <v>507</v>
+        <v>523</v>
       </c>
       <c r="D169" t="s">
-        <v>683</v>
+        <v>705</v>
       </c>
       <c r="E169" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6939,16 +7086,16 @@
         <v>176</v>
       </c>
       <c r="B170" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C170" t="s">
-        <v>508</v>
+        <v>524</v>
       </c>
       <c r="D170" t="s">
-        <v>684</v>
+        <v>706</v>
       </c>
       <c r="E170" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="F170">
         <v>4</v>
@@ -6965,16 +7112,16 @@
         <v>177</v>
       </c>
       <c r="B171" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="C171" t="s">
-        <v>509</v>
+        <v>525</v>
       </c>
       <c r="D171" t="s">
-        <v>685</v>
+        <v>707</v>
       </c>
       <c r="E171" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="F171">
         <v>5</v>
@@ -6991,16 +7138,16 @@
         <v>178</v>
       </c>
       <c r="B172" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="C172" t="s">
-        <v>510</v>
+        <v>526</v>
       </c>
       <c r="D172" t="s">
-        <v>686</v>
+        <v>708</v>
       </c>
       <c r="E172" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="F172">
         <v>6</v>
@@ -7017,16 +7164,16 @@
         <v>179</v>
       </c>
       <c r="B173" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="C173" t="s">
-        <v>511</v>
+        <v>527</v>
       </c>
       <c r="D173" t="s">
-        <v>687</v>
+        <v>709</v>
       </c>
       <c r="E173" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -7034,16 +7181,16 @@
         <v>180</v>
       </c>
       <c r="B174" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="C174" t="s">
-        <v>511</v>
+        <v>527</v>
       </c>
       <c r="D174" t="s">
-        <v>688</v>
+        <v>710</v>
       </c>
       <c r="E174" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -7051,16 +7198,16 @@
         <v>181</v>
       </c>
       <c r="B175" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="C175" t="s">
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="D175" t="s">
-        <v>689</v>
+        <v>711</v>
       </c>
       <c r="E175" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -7068,16 +7215,16 @@
         <v>182</v>
       </c>
       <c r="B176" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="C176" t="s">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="D176" t="s">
-        <v>690</v>
+        <v>712</v>
       </c>
       <c r="E176" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -7085,16 +7232,16 @@
         <v>183</v>
       </c>
       <c r="B177" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="C177" t="s">
-        <v>514</v>
+        <v>530</v>
       </c>
       <c r="D177" t="s">
-        <v>691</v>
+        <v>713</v>
       </c>
       <c r="E177" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -7102,16 +7249,152 @@
         <v>184</v>
       </c>
       <c r="B178" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="C178" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
       <c r="D178" t="s">
-        <v>692</v>
+        <v>714</v>
       </c>
       <c r="E178" t="s">
-        <v>698</v>
+        <v>728</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>185</v>
+      </c>
+      <c r="B179" t="s">
+        <v>369</v>
+      </c>
+      <c r="C179" t="s">
+        <v>532</v>
+      </c>
+      <c r="D179" t="s">
+        <v>715</v>
+      </c>
+      <c r="E179" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>186</v>
+      </c>
+      <c r="B180" t="s">
+        <v>370</v>
+      </c>
+      <c r="C180" t="s">
+        <v>532</v>
+      </c>
+      <c r="D180" t="s">
+        <v>716</v>
+      </c>
+      <c r="E180" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>187</v>
+      </c>
+      <c r="B181" t="s">
+        <v>371</v>
+      </c>
+      <c r="C181" t="s">
+        <v>532</v>
+      </c>
+      <c r="D181" t="s">
+        <v>717</v>
+      </c>
+      <c r="E181" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" t="s">
+        <v>188</v>
+      </c>
+      <c r="B182" t="s">
+        <v>372</v>
+      </c>
+      <c r="C182" t="s">
+        <v>533</v>
+      </c>
+      <c r="D182" t="s">
+        <v>718</v>
+      </c>
+      <c r="E182" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" t="s">
+        <v>189</v>
+      </c>
+      <c r="B183" t="s">
+        <v>373</v>
+      </c>
+      <c r="C183" t="s">
+        <v>534</v>
+      </c>
+      <c r="D183" t="s">
+        <v>719</v>
+      </c>
+      <c r="E183" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" t="s">
+        <v>190</v>
+      </c>
+      <c r="B184" t="s">
+        <v>374</v>
+      </c>
+      <c r="C184" t="s">
+        <v>535</v>
+      </c>
+      <c r="D184" t="s">
+        <v>720</v>
+      </c>
+      <c r="E184" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" t="s">
+        <v>191</v>
+      </c>
+      <c r="B185" t="s">
+        <v>375</v>
+      </c>
+      <c r="C185" t="s">
+        <v>536</v>
+      </c>
+      <c r="D185" t="s">
+        <v>721</v>
+      </c>
+      <c r="E185" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" t="s">
+        <v>192</v>
+      </c>
+      <c r="B186" t="s">
+        <v>376</v>
+      </c>
+      <c r="C186" t="s">
+        <v>537</v>
+      </c>
+      <c r="D186" t="s">
+        <v>722</v>
+      </c>
+      <c r="E186" t="s">
+        <v>729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add path to new drive, add handy python script to handle the exp record appending thing
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="777">
   <si>
     <t>ephysFN</t>
   </si>
@@ -595,6 +595,45 @@
     <t>Beto-18032020-008</t>
   </si>
   <si>
+    <t>Beto-19032020-001</t>
+  </si>
+  <si>
+    <t>Beto-19032020-002</t>
+  </si>
+  <si>
+    <t>Beto-19032020-003</t>
+  </si>
+  <si>
+    <t>Beto-19032020-004</t>
+  </si>
+  <si>
+    <t>Beto-19032020-005</t>
+  </si>
+  <si>
+    <t>Beto-19032020-006</t>
+  </si>
+  <si>
+    <t>Beto-20032020-001</t>
+  </si>
+  <si>
+    <t>Beto-20032020-002</t>
+  </si>
+  <si>
+    <t>Beto-20032020-003</t>
+  </si>
+  <si>
+    <t>Beto-20032020-004</t>
+  </si>
+  <si>
+    <t>Beto-20032020-005</t>
+  </si>
+  <si>
+    <t>Beto-20032020-006</t>
+  </si>
+  <si>
+    <t>Beto-20032020-007</t>
+  </si>
+  <si>
     <t>191002_Beto_selectivity_basic(1)</t>
   </si>
   <si>
@@ -1147,6 +1186,45 @@
     <t>200318_Beto_generate_integrated(5)</t>
   </si>
   <si>
+    <t>200319_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200319_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200319_Beto_rfMapper_basic(2)</t>
+  </si>
+  <si>
+    <t>200319_Beto_generate_integrated</t>
+  </si>
+  <si>
+    <t>200319_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200319_Beto_generate_integrated(2)</t>
+  </si>
+  <si>
+    <t>200320_Beto_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200320_Beto_rfMapper_basic(1)</t>
+  </si>
+  <si>
+    <t>200320_Beto_rfMapper_basic(2)</t>
+  </si>
+  <si>
+    <t>200320_Beto_rfMapper_basic(3)</t>
+  </si>
+  <si>
+    <t>200320_Beto_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200320_Beto_generate_integrated</t>
+  </si>
+  <si>
+    <t>200320_Beto_generate_integrated(3)</t>
+  </si>
+  <si>
     <t>\\storage1.ris.wustl.edu\crponce\Active\Stimuli\2019-Selectivity\2019-10-02a-beto</t>
   </si>
   <si>
@@ -1628,6 +1706,30 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-18-Beto-05\2020-03-18-14-10-20</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-19-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-19-Beto-01\2020-03-19-14-06-29</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-19-Beto-02\2020-03-19-15-07-34</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-19-Beto-03\2020-03-19-15-50-58</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-20-Beto</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-20-Beto-01\2020-03-20-09-41-52</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-20-Beto-02\2020-03-20-10-36-13</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-20-Beto-03\2020-03-20-11-17-46</t>
   </si>
   <si>
     <t>Derived from PCs of Ch 29 evolution 191002. 373 images {11*11 in PC2,PC3; PC49 PC50; RND RND space respectively, +10 last gen}</t>
@@ -2602,6 +2704,112 @@
 Around 18 gens the 1st evolution grows again! Find something new to add to the image.
 Gets to ~ 30 gens……
 Add 100mL water to him!
+Completed</t>
+  </si>
+  <si>
+    <t>001 RFMapping 13:
+-8:8:8 
+Carlos' huge image test
+Completed</t>
+  </si>
+  <si>
+    <t>002 RFMapping starts 13:36
+-8:2:8
+Mid image, 6mins
+Completed</t>
+  </si>
+  <si>
+    <t>003 RFMapping starts 13:49
+-2:1:2
+Completed</t>
+  </si>
+  <si>
+    <t>004 Generate Integrated starts 14:06
+25 [-1 -1.5 ] 4 1 ZOHA_Sphere_lr_euclid
+25 [-1 -1.5 ] 4 1 ZOHA_Sphere_lr_euclid_RD
+A little bit single unit, Maybe we should not split this unit.
+Still use the Inverse decay + 1.2 learning rate protocol
+Response is sparse.
+Starts taking off around gen 7, very slowly.
+Not very success to take off
+Not very successful in both……Not an informative comparison?
+Gen 13, Exploration 41.8 deg seems to take off…… Not really just flucturation.
+It's a good sign, Full evolution starts to dominate around 20 gens. Around 25 gens reduced starts to take off as well.
+Interestingly this evolution is pretty unstable, the score keep going up and down.
+Seems they plateau at around very different spots.
+Still growing! Exploration 29.2 - 28.2 degs. (This cell is more sensititve to finer changes? )
+Pretty large gap!
+27.3 deg, the cell still growng… Maybe single units really likes small exploration? The interaction goes.
+Really taking off! Around 45!
+Seems you really need to have a small learning rate for this cell to get to the top of mountain right?
+How could we test the sharpness of mountain hypothesis? Successfulness of different learning rate tuning schedule? 
+Great evolution! 51gens, the ZOHA full finally plateaued. 51 gens
+Completed</t>
+  </si>
+  <si>
+    <t>005 Generate Integrated starts 15:07
+25 [-1 -1.5 ] 4 1 CMAES
+See if CMAES can replicate the really late growing of response.
+Just curious, not relavent to current exp series, but can serve as control for the final activation level and the learning curve.
+CMAES goes up and down pretty fast.
+Seems CMAES's learning curve is smoother.
+Starts bumpping around.
+Seems it plateaus pretty early and didn't get the peak up there! Ends 60gens
+Completed</t>
+  </si>
+  <si>
+    <t>006 Generate Integrated starts 15:50
+39 [0 0 ] 3 2 ZOHA_Sphere_lr_euclid
+39 [0 0 ] 3 2 ZOHA_Sphere_lr_euclid_RD
+A fast V1 Hash Evolution comparison.
+Comes pretty close, just as predicted.
+maybe 11 generations are enough. Bump him up. 16mins 15 gens
+Completed</t>
+  </si>
+  <si>
+    <t>001 rf mapping -8:8:8
+Completed</t>
+  </si>
+  <si>
+    <t>002 rf mapping -4:4:4j
+Completed</t>
+  </si>
+  <si>
+    <t>003 rf mapping -2:2:2
+Completed</t>
+  </si>
+  <si>
+    <t>004 rf mapping -4:2:4
+Completed</t>
+  </si>
+  <si>
+    <t>005 at 941 AM
+integrated
+5 (0,0) 4 1 ZOHA full
+5 (0,0) 4 1 ZOHA red
+finished, 40 gens
+The BHV files seem to be deleted at first so I recover it and it's correct now!
+Basis saved.
+Completed</t>
+  </si>
+  <si>
+    <t>006 at 1036
+33 (0,0) 3 1 zoha full
+33 (0,0) 3 1 zoha red
+1046 AM complaining
+31 blocks completed…
+complaining
+BHV name is strange but it's coV name is strange burrect!
+Basis saved.
+Completed</t>
+  </si>
+  <si>
+    <t>007 1117
+58 (0,0) 3 1  zoha full
+58 (0,0) 3 1 zoha red
+Blasting him, last evolution for the day
+Bumping 1148
+Basis saved.
 Completed</t>
   </si>
   <si>
@@ -2981,7 +3189,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H186"/>
+  <dimension ref="A1:H199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3018,16 +3226,16 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>377</v>
+        <v>403</v>
       </c>
       <c r="D2" t="s">
-        <v>538</v>
+        <v>572</v>
       </c>
       <c r="E2" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3044,16 +3252,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>378</v>
+        <v>404</v>
       </c>
       <c r="D3" t="s">
-        <v>539</v>
+        <v>573</v>
       </c>
       <c r="E3" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3070,16 +3278,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>379</v>
+        <v>405</v>
       </c>
       <c r="D4" t="s">
-        <v>540</v>
+        <v>574</v>
       </c>
       <c r="E4" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -3096,16 +3304,16 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
-        <v>380</v>
+        <v>406</v>
       </c>
       <c r="D5" t="s">
-        <v>541</v>
+        <v>575</v>
       </c>
       <c r="E5" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -3122,16 +3330,16 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="D6" t="s">
-        <v>542</v>
+        <v>576</v>
       </c>
       <c r="E6" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -3148,16 +3356,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="D7" t="s">
-        <v>543</v>
+        <v>577</v>
       </c>
       <c r="E7" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -3174,16 +3382,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C8" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="D8" t="s">
-        <v>544</v>
+        <v>578</v>
       </c>
       <c r="E8" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -3200,16 +3408,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="D9" t="s">
-        <v>545</v>
+        <v>579</v>
       </c>
       <c r="E9" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -3226,16 +3434,16 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s">
-        <v>385</v>
+        <v>411</v>
       </c>
       <c r="D10" t="s">
-        <v>546</v>
+        <v>580</v>
       </c>
       <c r="E10" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -3252,16 +3460,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="C11" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="D11" t="s">
-        <v>547</v>
+        <v>581</v>
       </c>
       <c r="E11" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -3278,16 +3486,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="D12" t="s">
-        <v>548</v>
+        <v>582</v>
       </c>
       <c r="E12" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3304,16 +3512,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="C13" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="D13" t="s">
-        <v>549</v>
+        <v>583</v>
       </c>
       <c r="E13" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3330,16 +3538,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="C14" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="D14" t="s">
-        <v>550</v>
+        <v>584</v>
       </c>
       <c r="E14" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -3356,16 +3564,16 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="C15" t="s">
-        <v>390</v>
+        <v>416</v>
       </c>
       <c r="D15" t="s">
-        <v>551</v>
+        <v>585</v>
       </c>
       <c r="E15" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -3382,16 +3590,16 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C16" t="s">
-        <v>391</v>
+        <v>417</v>
       </c>
       <c r="D16" t="s">
-        <v>552</v>
+        <v>586</v>
       </c>
       <c r="E16" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -3408,16 +3616,16 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="C17" t="s">
-        <v>392</v>
+        <v>418</v>
       </c>
       <c r="D17" t="s">
-        <v>553</v>
+        <v>587</v>
       </c>
       <c r="E17" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -3434,16 +3642,16 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="C18" t="s">
-        <v>393</v>
+        <v>419</v>
       </c>
       <c r="D18" t="s">
-        <v>554</v>
+        <v>588</v>
       </c>
       <c r="E18" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -3460,16 +3668,16 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="C19" t="s">
-        <v>394</v>
+        <v>420</v>
       </c>
       <c r="D19" t="s">
-        <v>555</v>
+        <v>589</v>
       </c>
       <c r="E19" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -3486,16 +3694,16 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="C20" t="s">
-        <v>395</v>
+        <v>421</v>
       </c>
       <c r="D20" t="s">
-        <v>556</v>
+        <v>590</v>
       </c>
       <c r="E20" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3512,16 +3720,16 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>396</v>
+        <v>422</v>
       </c>
       <c r="D21" t="s">
-        <v>557</v>
+        <v>591</v>
       </c>
       <c r="E21" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3538,16 +3746,16 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
-        <v>397</v>
+        <v>423</v>
       </c>
       <c r="D22" t="s">
-        <v>558</v>
+        <v>592</v>
       </c>
       <c r="E22" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -3564,16 +3772,16 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="C23" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="D23" t="s">
-        <v>559</v>
+        <v>593</v>
       </c>
       <c r="E23" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -3590,16 +3798,16 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="C24" t="s">
-        <v>399</v>
+        <v>425</v>
       </c>
       <c r="D24" t="s">
-        <v>560</v>
+        <v>594</v>
       </c>
       <c r="E24" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -3616,16 +3824,16 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="C25" t="s">
-        <v>400</v>
+        <v>426</v>
       </c>
       <c r="D25" t="s">
-        <v>561</v>
+        <v>595</v>
       </c>
       <c r="E25" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -3642,16 +3850,16 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="C26" t="s">
-        <v>401</v>
+        <v>427</v>
       </c>
       <c r="D26" t="s">
-        <v>562</v>
+        <v>596</v>
       </c>
       <c r="E26" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -3668,16 +3876,16 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="C27" t="s">
-        <v>402</v>
+        <v>428</v>
       </c>
       <c r="D27" t="s">
-        <v>563</v>
+        <v>597</v>
       </c>
       <c r="E27" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -3694,16 +3902,16 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="C28" t="s">
-        <v>403</v>
+        <v>429</v>
       </c>
       <c r="D28" t="s">
-        <v>564</v>
+        <v>598</v>
       </c>
       <c r="E28" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -3720,16 +3928,16 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="C29" t="s">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="D29" t="s">
-        <v>565</v>
+        <v>599</v>
       </c>
       <c r="E29" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -3746,16 +3954,16 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="C30" t="s">
-        <v>405</v>
+        <v>431</v>
       </c>
       <c r="D30" t="s">
-        <v>566</v>
+        <v>600</v>
       </c>
       <c r="E30" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -3772,16 +3980,16 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="C31" t="s">
-        <v>406</v>
+        <v>432</v>
       </c>
       <c r="D31" t="s">
-        <v>567</v>
+        <v>601</v>
       </c>
       <c r="E31" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -3798,16 +4006,16 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="C32" t="s">
-        <v>407</v>
+        <v>433</v>
       </c>
       <c r="D32" t="s">
-        <v>568</v>
+        <v>602</v>
       </c>
       <c r="E32" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -3824,16 +4032,16 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="C33" t="s">
-        <v>408</v>
+        <v>434</v>
       </c>
       <c r="D33" t="s">
-        <v>569</v>
+        <v>603</v>
       </c>
       <c r="E33" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -3850,16 +4058,16 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="C34" t="s">
-        <v>409</v>
+        <v>435</v>
       </c>
       <c r="D34" t="s">
-        <v>570</v>
+        <v>604</v>
       </c>
       <c r="E34" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -3876,16 +4084,16 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="C35" t="s">
-        <v>410</v>
+        <v>436</v>
       </c>
       <c r="D35" t="s">
-        <v>571</v>
+        <v>605</v>
       </c>
       <c r="E35" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -3902,16 +4110,16 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="C36" t="s">
-        <v>411</v>
+        <v>437</v>
       </c>
       <c r="D36" t="s">
-        <v>572</v>
+        <v>606</v>
       </c>
       <c r="E36" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -3928,16 +4136,16 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="C37" t="s">
-        <v>412</v>
+        <v>438</v>
       </c>
       <c r="D37" t="s">
-        <v>573</v>
+        <v>607</v>
       </c>
       <c r="E37" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -3954,16 +4162,16 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="C38" t="s">
-        <v>413</v>
+        <v>439</v>
       </c>
       <c r="D38" t="s">
-        <v>574</v>
+        <v>608</v>
       </c>
       <c r="E38" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -3980,16 +4188,16 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="C39" t="s">
-        <v>414</v>
+        <v>440</v>
       </c>
       <c r="D39" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
       <c r="E39" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -4006,16 +4214,16 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="C40" t="s">
-        <v>415</v>
+        <v>441</v>
       </c>
       <c r="D40" t="s">
-        <v>576</v>
+        <v>610</v>
       </c>
       <c r="E40" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -4032,16 +4240,16 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="C41" t="s">
-        <v>416</v>
+        <v>442</v>
       </c>
       <c r="D41" t="s">
-        <v>577</v>
+        <v>611</v>
       </c>
       <c r="E41" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -4058,16 +4266,16 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="C42" t="s">
-        <v>417</v>
+        <v>443</v>
       </c>
       <c r="D42" t="s">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="E42" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -4084,16 +4292,16 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="C43" t="s">
-        <v>418</v>
+        <v>444</v>
       </c>
       <c r="D43" t="s">
-        <v>579</v>
+        <v>613</v>
       </c>
       <c r="E43" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -4110,16 +4318,16 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="C44" t="s">
-        <v>419</v>
+        <v>445</v>
       </c>
       <c r="D44" t="s">
-        <v>580</v>
+        <v>614</v>
       </c>
       <c r="E44" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -4136,16 +4344,16 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="C45" t="s">
-        <v>420</v>
+        <v>446</v>
       </c>
       <c r="D45" t="s">
-        <v>581</v>
+        <v>615</v>
       </c>
       <c r="E45" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -4162,16 +4370,16 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C46" t="s">
-        <v>421</v>
+        <v>447</v>
       </c>
       <c r="D46" t="s">
-        <v>582</v>
+        <v>616</v>
       </c>
       <c r="E46" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -4188,16 +4396,16 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C47" t="s">
-        <v>422</v>
+        <v>448</v>
       </c>
       <c r="D47" t="s">
-        <v>583</v>
+        <v>617</v>
       </c>
       <c r="E47" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -4214,16 +4422,16 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="C48" t="s">
-        <v>423</v>
+        <v>449</v>
       </c>
       <c r="D48" t="s">
-        <v>584</v>
+        <v>618</v>
       </c>
       <c r="E48" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F48">
         <v>23</v>
@@ -4240,16 +4448,16 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="C49" t="s">
-        <v>424</v>
+        <v>450</v>
       </c>
       <c r="D49" t="s">
-        <v>585</v>
+        <v>619</v>
       </c>
       <c r="E49" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F49">
         <v>23</v>
@@ -4266,16 +4474,16 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="C50" t="s">
-        <v>425</v>
+        <v>451</v>
       </c>
       <c r="D50" t="s">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="E50" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F50">
         <v>24</v>
@@ -4292,16 +4500,16 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="C51" t="s">
-        <v>426</v>
+        <v>452</v>
       </c>
       <c r="D51" t="s">
-        <v>587</v>
+        <v>621</v>
       </c>
       <c r="E51" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -4318,16 +4526,16 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="C52" t="s">
-        <v>427</v>
+        <v>453</v>
       </c>
       <c r="D52" t="s">
-        <v>588</v>
+        <v>622</v>
       </c>
       <c r="E52" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F52">
         <v>24</v>
@@ -4344,13 +4552,13 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="C53" t="s">
-        <v>428</v>
+        <v>454</v>
       </c>
       <c r="D53" t="s">
-        <v>589</v>
+        <v>623</v>
       </c>
       <c r="F53">
         <v>24</v>
@@ -4367,16 +4575,16 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="C54" t="s">
-        <v>429</v>
+        <v>455</v>
       </c>
       <c r="D54" t="s">
-        <v>590</v>
+        <v>624</v>
       </c>
       <c r="E54" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -4393,16 +4601,16 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="C55" t="s">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="D55" t="s">
-        <v>591</v>
+        <v>625</v>
       </c>
       <c r="E55" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F55">
         <v>25</v>
@@ -4419,16 +4627,16 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="C56" t="s">
-        <v>431</v>
+        <v>457</v>
       </c>
       <c r="D56" t="s">
-        <v>592</v>
+        <v>626</v>
       </c>
       <c r="E56" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F56">
         <v>25</v>
@@ -4445,16 +4653,16 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="C57" t="s">
-        <v>432</v>
+        <v>458</v>
       </c>
       <c r="D57" t="s">
-        <v>593</v>
+        <v>627</v>
       </c>
       <c r="E57" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -4471,16 +4679,16 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C58" t="s">
-        <v>433</v>
+        <v>459</v>
       </c>
       <c r="D58" t="s">
-        <v>594</v>
+        <v>628</v>
       </c>
       <c r="E58" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -4497,16 +4705,16 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="C59" t="s">
-        <v>434</v>
+        <v>460</v>
       </c>
       <c r="D59" t="s">
-        <v>595</v>
+        <v>629</v>
       </c>
       <c r="E59" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -4523,16 +4731,16 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="C60" t="s">
-        <v>435</v>
+        <v>461</v>
       </c>
       <c r="D60" t="s">
-        <v>596</v>
+        <v>630</v>
       </c>
       <c r="E60" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F60">
         <v>27</v>
@@ -4549,16 +4757,16 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="C61" t="s">
-        <v>436</v>
+        <v>462</v>
       </c>
       <c r="D61" t="s">
-        <v>597</v>
+        <v>631</v>
       </c>
       <c r="E61" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F61">
         <v>27</v>
@@ -4575,16 +4783,16 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="C62" t="s">
-        <v>437</v>
+        <v>463</v>
       </c>
       <c r="D62" t="s">
-        <v>598</v>
+        <v>632</v>
       </c>
       <c r="E62" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F62">
         <v>27</v>
@@ -4601,16 +4809,16 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="C63" t="s">
-        <v>438</v>
+        <v>464</v>
       </c>
       <c r="D63" t="s">
-        <v>599</v>
+        <v>633</v>
       </c>
       <c r="E63" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -4627,16 +4835,16 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="C64" t="s">
-        <v>439</v>
+        <v>465</v>
       </c>
       <c r="D64" t="s">
-        <v>600</v>
+        <v>634</v>
       </c>
       <c r="E64" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -4653,16 +4861,16 @@
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="C65" t="s">
-        <v>440</v>
+        <v>466</v>
       </c>
       <c r="D65" t="s">
-        <v>601</v>
+        <v>635</v>
       </c>
       <c r="E65" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -4679,16 +4887,16 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="C66" t="s">
-        <v>441</v>
+        <v>467</v>
       </c>
       <c r="D66" t="s">
-        <v>602</v>
+        <v>636</v>
       </c>
       <c r="E66" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -4705,16 +4913,16 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="C67" t="s">
-        <v>439</v>
+        <v>465</v>
       </c>
       <c r="D67" t="s">
-        <v>603</v>
+        <v>637</v>
       </c>
       <c r="E67" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -4731,16 +4939,16 @@
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="C68" t="s">
-        <v>442</v>
+        <v>468</v>
       </c>
       <c r="D68" t="s">
-        <v>604</v>
+        <v>638</v>
       </c>
       <c r="E68" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -4757,16 +4965,16 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="C69" t="s">
-        <v>443</v>
+        <v>469</v>
       </c>
       <c r="D69" t="s">
-        <v>605</v>
+        <v>639</v>
       </c>
       <c r="E69" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -4783,16 +4991,16 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="C70" t="s">
-        <v>444</v>
+        <v>470</v>
       </c>
       <c r="D70" t="s">
-        <v>606</v>
+        <v>640</v>
       </c>
       <c r="E70" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -4809,16 +5017,16 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="C71" t="s">
-        <v>445</v>
+        <v>471</v>
       </c>
       <c r="D71" t="s">
-        <v>607</v>
+        <v>641</v>
       </c>
       <c r="E71" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -4835,16 +5043,16 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="C72" t="s">
-        <v>446</v>
+        <v>472</v>
       </c>
       <c r="D72" t="s">
-        <v>608</v>
+        <v>642</v>
       </c>
       <c r="E72" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -4861,16 +5069,16 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="C73" t="s">
-        <v>447</v>
+        <v>473</v>
       </c>
       <c r="D73" t="s">
-        <v>609</v>
+        <v>643</v>
       </c>
       <c r="E73" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -4887,16 +5095,16 @@
         <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="C74" t="s">
-        <v>448</v>
+        <v>474</v>
       </c>
       <c r="D74" t="s">
-        <v>610</v>
+        <v>644</v>
       </c>
       <c r="E74" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -4913,16 +5121,16 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="C75" t="s">
-        <v>449</v>
+        <v>475</v>
       </c>
       <c r="D75" t="s">
-        <v>611</v>
+        <v>645</v>
       </c>
       <c r="E75" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -4939,16 +5147,16 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="C76" t="s">
-        <v>450</v>
+        <v>476</v>
       </c>
       <c r="D76" t="s">
-        <v>612</v>
+        <v>646</v>
       </c>
       <c r="E76" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -4965,16 +5173,16 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="C77" t="s">
-        <v>451</v>
+        <v>477</v>
       </c>
       <c r="D77" t="s">
-        <v>613</v>
+        <v>647</v>
       </c>
       <c r="E77" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -4991,16 +5199,16 @@
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="C78" t="s">
-        <v>452</v>
+        <v>478</v>
       </c>
       <c r="D78" t="s">
-        <v>614</v>
+        <v>648</v>
       </c>
       <c r="E78" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -5017,16 +5225,16 @@
         <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="C79" t="s">
-        <v>453</v>
+        <v>479</v>
       </c>
       <c r="D79" t="s">
-        <v>615</v>
+        <v>649</v>
       </c>
       <c r="E79" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -5043,16 +5251,16 @@
         <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="C80" t="s">
-        <v>454</v>
+        <v>480</v>
       </c>
       <c r="D80" t="s">
-        <v>616</v>
+        <v>650</v>
       </c>
       <c r="E80" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -5069,13 +5277,13 @@
         <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="C81" t="s">
-        <v>455</v>
+        <v>481</v>
       </c>
       <c r="D81" t="s">
-        <v>617</v>
+        <v>651</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -5092,13 +5300,13 @@
         <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="C82" t="s">
-        <v>455</v>
+        <v>481</v>
       </c>
       <c r="D82" t="s">
-        <v>618</v>
+        <v>652</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -5115,13 +5323,13 @@
         <v>89</v>
       </c>
       <c r="C83" t="s">
-        <v>455</v>
+        <v>481</v>
       </c>
       <c r="D83" t="s">
-        <v>619</v>
+        <v>653</v>
       </c>
       <c r="E83" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -5138,16 +5346,16 @@
         <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="C84" t="s">
-        <v>456</v>
+        <v>482</v>
       </c>
       <c r="D84" t="s">
-        <v>620</v>
+        <v>654</v>
       </c>
       <c r="E84" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -5164,16 +5372,16 @@
         <v>91</v>
       </c>
       <c r="B85" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="C85" t="s">
-        <v>457</v>
+        <v>483</v>
       </c>
       <c r="D85" t="s">
-        <v>621</v>
+        <v>655</v>
       </c>
       <c r="E85" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F85">
         <v>35</v>
@@ -5190,16 +5398,16 @@
         <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="C86" t="s">
-        <v>458</v>
+        <v>484</v>
       </c>
       <c r="D86" t="s">
-        <v>622</v>
+        <v>656</v>
       </c>
       <c r="E86" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -5216,16 +5424,16 @@
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="C87" t="s">
-        <v>459</v>
+        <v>485</v>
       </c>
       <c r="D87" t="s">
-        <v>623</v>
+        <v>657</v>
       </c>
       <c r="E87" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F87">
         <v>36</v>
@@ -5242,16 +5450,16 @@
         <v>94</v>
       </c>
       <c r="B88" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="C88" t="s">
-        <v>460</v>
+        <v>486</v>
       </c>
       <c r="D88" t="s">
-        <v>624</v>
+        <v>658</v>
       </c>
       <c r="E88" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -5268,16 +5476,16 @@
         <v>95</v>
       </c>
       <c r="B89" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="C89" t="s">
-        <v>461</v>
+        <v>487</v>
       </c>
       <c r="D89" t="s">
-        <v>625</v>
+        <v>659</v>
       </c>
       <c r="E89" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -5294,16 +5502,16 @@
         <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="C90" t="s">
-        <v>462</v>
+        <v>488</v>
       </c>
       <c r="D90" t="s">
-        <v>626</v>
+        <v>660</v>
       </c>
       <c r="E90" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F90">
         <v>37</v>
@@ -5320,16 +5528,16 @@
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="C91" t="s">
-        <v>463</v>
+        <v>489</v>
       </c>
       <c r="D91" t="s">
-        <v>627</v>
+        <v>661</v>
       </c>
       <c r="E91" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -5346,16 +5554,16 @@
         <v>98</v>
       </c>
       <c r="B92" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="C92" t="s">
-        <v>464</v>
+        <v>490</v>
       </c>
       <c r="D92" t="s">
-        <v>628</v>
+        <v>662</v>
       </c>
       <c r="E92" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F92">
         <v>38</v>
@@ -5372,16 +5580,16 @@
         <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="C93" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="D93" t="s">
-        <v>629</v>
+        <v>663</v>
       </c>
       <c r="E93" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -5398,16 +5606,16 @@
         <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="C94" t="s">
-        <v>466</v>
+        <v>492</v>
       </c>
       <c r="D94" t="s">
-        <v>630</v>
+        <v>664</v>
       </c>
       <c r="E94" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -5424,16 +5632,16 @@
         <v>101</v>
       </c>
       <c r="B95" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="C95" t="s">
-        <v>467</v>
+        <v>493</v>
       </c>
       <c r="D95" t="s">
-        <v>631</v>
+        <v>665</v>
       </c>
       <c r="E95" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F95">
         <v>39</v>
@@ -5450,16 +5658,16 @@
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="C96" t="s">
-        <v>468</v>
+        <v>494</v>
       </c>
       <c r="D96" t="s">
-        <v>632</v>
+        <v>666</v>
       </c>
       <c r="E96" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -5476,16 +5684,16 @@
         <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="C97" t="s">
-        <v>469</v>
+        <v>495</v>
       </c>
       <c r="D97" t="s">
-        <v>633</v>
+        <v>667</v>
       </c>
       <c r="E97" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -5502,16 +5710,16 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="C98" t="s">
-        <v>470</v>
+        <v>496</v>
       </c>
       <c r="D98" t="s">
-        <v>634</v>
+        <v>668</v>
       </c>
       <c r="E98" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -5528,16 +5736,16 @@
         <v>105</v>
       </c>
       <c r="B99" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="C99" t="s">
-        <v>471</v>
+        <v>497</v>
       </c>
       <c r="D99" t="s">
-        <v>635</v>
+        <v>669</v>
       </c>
       <c r="E99" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -5554,16 +5762,16 @@
         <v>106</v>
       </c>
       <c r="B100" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="C100" t="s">
-        <v>472</v>
+        <v>498</v>
       </c>
       <c r="D100" t="s">
-        <v>636</v>
+        <v>670</v>
       </c>
       <c r="E100" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F100">
         <v>41</v>
@@ -5580,16 +5788,16 @@
         <v>107</v>
       </c>
       <c r="B101" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="C101" t="s">
-        <v>473</v>
+        <v>499</v>
       </c>
       <c r="D101" t="s">
-        <v>637</v>
+        <v>671</v>
       </c>
       <c r="E101" t="s">
-        <v>724</v>
+        <v>771</v>
       </c>
       <c r="F101">
         <v>41</v>
@@ -5600,16 +5808,16 @@
         <v>108</v>
       </c>
       <c r="B102" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="C102" t="s">
-        <v>474</v>
+        <v>500</v>
       </c>
       <c r="D102" t="s">
-        <v>638</v>
+        <v>672</v>
       </c>
       <c r="E102" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -5626,16 +5834,16 @@
         <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="C103" t="s">
-        <v>475</v>
+        <v>501</v>
       </c>
       <c r="D103" t="s">
-        <v>639</v>
+        <v>673</v>
       </c>
       <c r="E103" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -5652,16 +5860,16 @@
         <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="C104" t="s">
-        <v>476</v>
+        <v>502</v>
       </c>
       <c r="D104" t="s">
-        <v>640</v>
+        <v>674</v>
       </c>
       <c r="E104" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F104">
         <v>42</v>
@@ -5678,16 +5886,16 @@
         <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="C105" t="s">
-        <v>477</v>
+        <v>503</v>
       </c>
       <c r="D105" t="s">
-        <v>641</v>
+        <v>675</v>
       </c>
       <c r="E105" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -5704,16 +5912,16 @@
         <v>112</v>
       </c>
       <c r="B106" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="C106" t="s">
-        <v>475</v>
+        <v>501</v>
       </c>
       <c r="D106" t="s">
-        <v>642</v>
+        <v>676</v>
       </c>
       <c r="E106" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -5730,16 +5938,16 @@
         <v>113</v>
       </c>
       <c r="B107" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="C107" t="s">
-        <v>478</v>
+        <v>504</v>
       </c>
       <c r="D107" t="s">
-        <v>643</v>
+        <v>677</v>
       </c>
       <c r="E107" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F107">
         <v>43</v>
@@ -5756,16 +5964,16 @@
         <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="C108" t="s">
-        <v>479</v>
+        <v>505</v>
       </c>
       <c r="D108" t="s">
-        <v>644</v>
+        <v>678</v>
       </c>
       <c r="E108" t="s">
-        <v>724</v>
+        <v>771</v>
       </c>
       <c r="F108">
         <v>43</v>
@@ -5776,16 +5984,16 @@
         <v>115</v>
       </c>
       <c r="B109" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C109" t="s">
-        <v>479</v>
+        <v>505</v>
       </c>
       <c r="D109" t="s">
-        <v>645</v>
+        <v>679</v>
       </c>
       <c r="E109" t="s">
-        <v>724</v>
+        <v>771</v>
       </c>
       <c r="F109">
         <v>43</v>
@@ -5796,16 +6004,16 @@
         <v>116</v>
       </c>
       <c r="B110" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="C110" t="s">
-        <v>480</v>
+        <v>506</v>
       </c>
       <c r="D110" t="s">
-        <v>646</v>
+        <v>680</v>
       </c>
       <c r="E110" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -5822,16 +6030,16 @@
         <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="C111" t="s">
-        <v>481</v>
+        <v>507</v>
       </c>
       <c r="D111" t="s">
-        <v>647</v>
+        <v>681</v>
       </c>
       <c r="E111" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -5848,16 +6056,16 @@
         <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="C112" t="s">
-        <v>480</v>
+        <v>506</v>
       </c>
       <c r="D112" t="s">
-        <v>648</v>
+        <v>682</v>
       </c>
       <c r="E112" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F112">
         <v>44</v>
@@ -5874,16 +6082,16 @@
         <v>119</v>
       </c>
       <c r="B113" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="C113" t="s">
-        <v>482</v>
+        <v>508</v>
       </c>
       <c r="D113" t="s">
-        <v>649</v>
+        <v>683</v>
       </c>
       <c r="E113" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -5900,16 +6108,16 @@
         <v>120</v>
       </c>
       <c r="B114" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="C114" t="s">
-        <v>483</v>
+        <v>509</v>
       </c>
       <c r="D114" t="s">
-        <v>650</v>
+        <v>684</v>
       </c>
       <c r="E114" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -5926,16 +6134,16 @@
         <v>121</v>
       </c>
       <c r="B115" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="C115" t="s">
-        <v>484</v>
+        <v>510</v>
       </c>
       <c r="D115" t="s">
-        <v>651</v>
+        <v>685</v>
       </c>
       <c r="E115" t="s">
-        <v>723</v>
+        <v>770</v>
       </c>
       <c r="F115">
         <v>45</v>
@@ -5952,16 +6160,16 @@
         <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="C116" t="s">
-        <v>485</v>
+        <v>511</v>
       </c>
       <c r="D116" t="s">
-        <v>652</v>
+        <v>686</v>
       </c>
       <c r="E116" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -5972,16 +6180,16 @@
         <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="C117" t="s">
-        <v>486</v>
+        <v>512</v>
       </c>
       <c r="D117" t="s">
-        <v>653</v>
+        <v>687</v>
       </c>
       <c r="E117" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -5998,16 +6206,16 @@
         <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="C118" t="s">
-        <v>487</v>
+        <v>513</v>
       </c>
       <c r="D118" t="s">
-        <v>654</v>
+        <v>688</v>
       </c>
       <c r="E118" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="H118">
         <v>2</v>
@@ -6018,16 +6226,16 @@
         <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="C119" t="s">
-        <v>488</v>
+        <v>514</v>
       </c>
       <c r="D119" t="s">
-        <v>655</v>
+        <v>689</v>
       </c>
       <c r="E119" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -6044,16 +6252,16 @@
         <v>126</v>
       </c>
       <c r="B120" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="C120" t="s">
-        <v>489</v>
+        <v>515</v>
       </c>
       <c r="D120" t="s">
-        <v>656</v>
+        <v>690</v>
       </c>
       <c r="E120" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -6070,16 +6278,16 @@
         <v>127</v>
       </c>
       <c r="B121" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="C121" t="s">
-        <v>490</v>
+        <v>516</v>
       </c>
       <c r="D121" t="s">
-        <v>657</v>
+        <v>691</v>
       </c>
       <c r="E121" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="H121">
         <v>2</v>
@@ -6090,16 +6298,16 @@
         <v>128</v>
       </c>
       <c r="B122" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="C122" t="s">
-        <v>491</v>
+        <v>517</v>
       </c>
       <c r="D122" t="s">
-        <v>658</v>
+        <v>692</v>
       </c>
       <c r="E122" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -6116,13 +6324,13 @@
         <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="C123" t="s">
-        <v>492</v>
+        <v>518</v>
       </c>
       <c r="D123" t="s">
-        <v>659</v>
+        <v>693</v>
       </c>
       <c r="G123">
         <v>41</v>
@@ -6136,16 +6344,16 @@
         <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C124" t="s">
-        <v>490</v>
+        <v>516</v>
       </c>
       <c r="D124" t="s">
-        <v>660</v>
+        <v>694</v>
       </c>
       <c r="E124" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="H124">
         <v>3</v>
@@ -6156,16 +6364,16 @@
         <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="C125" t="s">
-        <v>490</v>
+        <v>516</v>
       </c>
       <c r="D125" t="s">
-        <v>661</v>
+        <v>695</v>
       </c>
       <c r="E125" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -6176,16 +6384,16 @@
         <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="C126" t="s">
-        <v>493</v>
+        <v>519</v>
       </c>
       <c r="D126" t="s">
-        <v>662</v>
+        <v>696</v>
       </c>
       <c r="E126" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="F126">
         <v>5</v>
@@ -6202,16 +6410,16 @@
         <v>133</v>
       </c>
       <c r="B127" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="C127" t="s">
-        <v>494</v>
+        <v>520</v>
       </c>
       <c r="D127" t="s">
-        <v>663</v>
+        <v>697</v>
       </c>
       <c r="E127" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -6219,13 +6427,13 @@
         <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="C128" t="s">
-        <v>495</v>
+        <v>521</v>
       </c>
       <c r="D128" t="s">
-        <v>664</v>
+        <v>698</v>
       </c>
       <c r="G128">
         <v>26</v>
@@ -6239,16 +6447,16 @@
         <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="C129" t="s">
-        <v>496</v>
+        <v>522</v>
       </c>
       <c r="D129" t="s">
-        <v>665</v>
+        <v>699</v>
       </c>
       <c r="E129" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -6265,13 +6473,13 @@
         <v>136</v>
       </c>
       <c r="B130" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="C130" t="s">
-        <v>497</v>
+        <v>523</v>
       </c>
       <c r="D130" t="s">
-        <v>666</v>
+        <v>700</v>
       </c>
       <c r="H130">
         <v>2</v>
@@ -6282,13 +6490,13 @@
         <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="C131" t="s">
-        <v>497</v>
+        <v>523</v>
       </c>
       <c r="D131" t="s">
-        <v>667</v>
+        <v>701</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -6299,16 +6507,16 @@
         <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="C132" t="s">
-        <v>498</v>
+        <v>524</v>
       </c>
       <c r="D132" t="s">
-        <v>668</v>
+        <v>702</v>
       </c>
       <c r="E132" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -6325,16 +6533,16 @@
         <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="C133" t="s">
-        <v>499</v>
+        <v>525</v>
       </c>
       <c r="D133" t="s">
-        <v>669</v>
+        <v>703</v>
       </c>
       <c r="E133" t="s">
-        <v>725</v>
+        <v>772</v>
       </c>
       <c r="F133">
         <v>7</v>
@@ -6351,16 +6559,16 @@
         <v>140</v>
       </c>
       <c r="B134" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="C134" t="s">
-        <v>500</v>
+        <v>526</v>
       </c>
       <c r="D134" t="s">
-        <v>670</v>
+        <v>704</v>
       </c>
       <c r="E134" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="H134">
         <v>0.75</v>
@@ -6371,16 +6579,16 @@
         <v>141</v>
       </c>
       <c r="B135" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="C135" t="s">
-        <v>500</v>
+        <v>526</v>
       </c>
       <c r="D135" t="s">
-        <v>671</v>
+        <v>705</v>
       </c>
       <c r="E135" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="H135">
         <v>2</v>
@@ -6391,16 +6599,16 @@
         <v>142</v>
       </c>
       <c r="B136" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="C136" t="s">
-        <v>501</v>
+        <v>527</v>
       </c>
       <c r="D136" t="s">
-        <v>672</v>
+        <v>706</v>
       </c>
       <c r="E136" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -6417,16 +6625,16 @@
         <v>143</v>
       </c>
       <c r="B137" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="C137" t="s">
-        <v>502</v>
+        <v>528</v>
       </c>
       <c r="D137" t="s">
-        <v>673</v>
+        <v>707</v>
       </c>
       <c r="E137" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="F137">
         <v>2</v>
@@ -6443,16 +6651,16 @@
         <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="C138" t="s">
-        <v>503</v>
+        <v>529</v>
       </c>
       <c r="D138" t="s">
-        <v>674</v>
+        <v>708</v>
       </c>
       <c r="E138" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="F138">
         <v>3</v>
@@ -6469,16 +6677,16 @@
         <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="C139" t="s">
-        <v>504</v>
+        <v>530</v>
       </c>
       <c r="D139" t="s">
-        <v>675</v>
+        <v>709</v>
       </c>
       <c r="E139" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="F139">
         <v>4</v>
@@ -6495,16 +6703,16 @@
         <v>146</v>
       </c>
       <c r="B140" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="C140" t="s">
-        <v>505</v>
+        <v>531</v>
       </c>
       <c r="D140" t="s">
-        <v>676</v>
+        <v>710</v>
       </c>
       <c r="E140" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="H140">
         <v>0.75</v>
@@ -6515,16 +6723,16 @@
         <v>147</v>
       </c>
       <c r="B141" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="C141" t="s">
-        <v>505</v>
+        <v>531</v>
       </c>
       <c r="D141" t="s">
-        <v>677</v>
+        <v>711</v>
       </c>
       <c r="E141" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="H141">
         <v>2</v>
@@ -6535,16 +6743,16 @@
         <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="C142" t="s">
-        <v>506</v>
+        <v>532</v>
       </c>
       <c r="D142" t="s">
-        <v>678</v>
+        <v>712</v>
       </c>
       <c r="E142" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="F142">
         <v>5</v>
@@ -6561,16 +6769,16 @@
         <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="C143" t="s">
-        <v>507</v>
+        <v>533</v>
       </c>
       <c r="D143" t="s">
-        <v>679</v>
+        <v>713</v>
       </c>
       <c r="E143" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="F143">
         <v>6</v>
@@ -6587,16 +6795,16 @@
         <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="C144" t="s">
-        <v>508</v>
+        <v>534</v>
       </c>
       <c r="D144" t="s">
-        <v>680</v>
+        <v>714</v>
       </c>
       <c r="E144" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="H144">
         <v>0.75</v>
@@ -6607,16 +6815,16 @@
         <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="C145" t="s">
-        <v>508</v>
+        <v>534</v>
       </c>
       <c r="D145" t="s">
-        <v>681</v>
+        <v>715</v>
       </c>
       <c r="E145" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="H145">
         <v>2</v>
@@ -6627,16 +6835,16 @@
         <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="C146" t="s">
-        <v>509</v>
+        <v>535</v>
       </c>
       <c r="D146" t="s">
-        <v>682</v>
+        <v>716</v>
       </c>
       <c r="E146" t="s">
-        <v>727</v>
+        <v>774</v>
       </c>
       <c r="F146">
         <v>101</v>
@@ -6653,16 +6861,16 @@
         <v>153</v>
       </c>
       <c r="B147" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="C147" t="s">
-        <v>510</v>
+        <v>536</v>
       </c>
       <c r="D147" t="s">
-        <v>683</v>
+        <v>717</v>
       </c>
       <c r="E147" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="G147">
         <v>24</v>
@@ -6676,16 +6884,16 @@
         <v>154</v>
       </c>
       <c r="B148" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="C148" t="s">
-        <v>511</v>
+        <v>537</v>
       </c>
       <c r="D148" t="s">
-        <v>684</v>
+        <v>718</v>
       </c>
       <c r="E148" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -6702,16 +6910,16 @@
         <v>155</v>
       </c>
       <c r="B149" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="C149" t="s">
-        <v>512</v>
+        <v>538</v>
       </c>
       <c r="D149" t="s">
-        <v>685</v>
+        <v>719</v>
       </c>
       <c r="E149" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="H149">
         <v>0.75</v>
@@ -6722,16 +6930,16 @@
         <v>156</v>
       </c>
       <c r="B150" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="C150" t="s">
-        <v>512</v>
+        <v>538</v>
       </c>
       <c r="D150" t="s">
-        <v>686</v>
+        <v>720</v>
       </c>
       <c r="E150" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="H150">
         <v>2</v>
@@ -6742,16 +6950,16 @@
         <v>157</v>
       </c>
       <c r="B151" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="C151" t="s">
-        <v>513</v>
+        <v>539</v>
       </c>
       <c r="D151" t="s">
-        <v>687</v>
+        <v>721</v>
       </c>
       <c r="E151" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -6768,16 +6976,16 @@
         <v>158</v>
       </c>
       <c r="B152" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="C152" t="s">
-        <v>514</v>
+        <v>540</v>
       </c>
       <c r="D152" t="s">
-        <v>688</v>
+        <v>722</v>
       </c>
       <c r="E152" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="F152">
         <v>3</v>
@@ -6794,13 +7002,13 @@
         <v>159</v>
       </c>
       <c r="B153" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="D153" t="s">
-        <v>689</v>
+        <v>723</v>
       </c>
       <c r="E153" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -6808,16 +7016,16 @@
         <v>160</v>
       </c>
       <c r="B154" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="C154" t="s">
-        <v>515</v>
+        <v>541</v>
       </c>
       <c r="D154" t="s">
-        <v>690</v>
+        <v>724</v>
       </c>
       <c r="E154" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="G154">
         <v>24</v>
@@ -6831,13 +7039,13 @@
         <v>161</v>
       </c>
       <c r="B155" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="D155" t="s">
-        <v>691</v>
+        <v>725</v>
       </c>
       <c r="E155" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -6845,13 +7053,13 @@
         <v>162</v>
       </c>
       <c r="B156" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="D156" t="s">
-        <v>692</v>
+        <v>726</v>
       </c>
       <c r="E156" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -6859,16 +7067,16 @@
         <v>163</v>
       </c>
       <c r="B157" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="C157" t="s">
-        <v>516</v>
+        <v>542</v>
       </c>
       <c r="D157" t="s">
-        <v>693</v>
+        <v>727</v>
       </c>
       <c r="E157" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="G157">
         <v>39</v>
@@ -6879,16 +7087,16 @@
         <v>164</v>
       </c>
       <c r="B158" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="C158" t="s">
-        <v>517</v>
+        <v>543</v>
       </c>
       <c r="D158" t="s">
-        <v>694</v>
+        <v>728</v>
       </c>
       <c r="E158" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -6896,13 +7104,13 @@
         <v>165</v>
       </c>
       <c r="B159" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="D159" t="s">
-        <v>695</v>
+        <v>729</v>
       </c>
       <c r="E159" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -6910,16 +7118,16 @@
         <v>166</v>
       </c>
       <c r="B160" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="C160" t="s">
-        <v>518</v>
+        <v>544</v>
       </c>
       <c r="D160" t="s">
-        <v>696</v>
+        <v>730</v>
       </c>
       <c r="E160" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="G160">
         <v>39</v>
@@ -6930,16 +7138,16 @@
         <v>167</v>
       </c>
       <c r="B161" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="C161" t="s">
-        <v>519</v>
+        <v>545</v>
       </c>
       <c r="D161" t="s">
-        <v>697</v>
+        <v>731</v>
       </c>
       <c r="E161" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -6947,16 +7155,16 @@
         <v>168</v>
       </c>
       <c r="B162" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="C162" t="s">
-        <v>519</v>
+        <v>545</v>
       </c>
       <c r="D162" t="s">
-        <v>698</v>
+        <v>732</v>
       </c>
       <c r="E162" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -6964,16 +7172,16 @@
         <v>169</v>
       </c>
       <c r="B163" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="C163" t="s">
-        <v>520</v>
+        <v>546</v>
       </c>
       <c r="D163" t="s">
-        <v>699</v>
+        <v>733</v>
       </c>
       <c r="E163" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="G163">
         <v>39</v>
@@ -6984,16 +7192,16 @@
         <v>170</v>
       </c>
       <c r="B164" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="C164" t="s">
-        <v>521</v>
+        <v>547</v>
       </c>
       <c r="D164" t="s">
-        <v>700</v>
+        <v>734</v>
       </c>
       <c r="E164" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="G164">
         <v>25</v>
@@ -7004,13 +7212,13 @@
         <v>171</v>
       </c>
       <c r="B165" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="D165" t="s">
-        <v>701</v>
+        <v>735</v>
       </c>
       <c r="E165" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -7018,13 +7226,13 @@
         <v>172</v>
       </c>
       <c r="B166" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="D166" t="s">
-        <v>702</v>
+        <v>736</v>
       </c>
       <c r="E166" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -7032,16 +7240,16 @@
         <v>173</v>
       </c>
       <c r="B167" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="C167" t="s">
-        <v>522</v>
+        <v>548</v>
       </c>
       <c r="D167" t="s">
-        <v>703</v>
+        <v>737</v>
       </c>
       <c r="E167" t="s">
-        <v>726</v>
+        <v>773</v>
       </c>
       <c r="G167">
         <v>41</v>
@@ -7052,16 +7260,16 @@
         <v>174</v>
       </c>
       <c r="B168" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="C168" t="s">
-        <v>523</v>
+        <v>549</v>
       </c>
       <c r="D168" t="s">
-        <v>704</v>
+        <v>738</v>
       </c>
       <c r="E168" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -7069,16 +7277,16 @@
         <v>175</v>
       </c>
       <c r="B169" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="C169" t="s">
-        <v>523</v>
+        <v>549</v>
       </c>
       <c r="D169" t="s">
-        <v>705</v>
+        <v>739</v>
       </c>
       <c r="E169" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -7086,16 +7294,16 @@
         <v>176</v>
       </c>
       <c r="B170" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="C170" t="s">
-        <v>524</v>
+        <v>550</v>
       </c>
       <c r="D170" t="s">
-        <v>706</v>
+        <v>740</v>
       </c>
       <c r="E170" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="F170">
         <v>4</v>
@@ -7112,16 +7320,16 @@
         <v>177</v>
       </c>
       <c r="B171" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="C171" t="s">
-        <v>525</v>
+        <v>551</v>
       </c>
       <c r="D171" t="s">
-        <v>707</v>
+        <v>741</v>
       </c>
       <c r="E171" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="F171">
         <v>5</v>
@@ -7138,16 +7346,16 @@
         <v>178</v>
       </c>
       <c r="B172" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C172" t="s">
-        <v>526</v>
+        <v>552</v>
       </c>
       <c r="D172" t="s">
-        <v>708</v>
+        <v>742</v>
       </c>
       <c r="E172" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="F172">
         <v>6</v>
@@ -7164,16 +7372,16 @@
         <v>179</v>
       </c>
       <c r="B173" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="C173" t="s">
-        <v>527</v>
+        <v>553</v>
       </c>
       <c r="D173" t="s">
-        <v>709</v>
+        <v>743</v>
       </c>
       <c r="E173" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -7181,16 +7389,16 @@
         <v>180</v>
       </c>
       <c r="B174" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="C174" t="s">
-        <v>527</v>
+        <v>553</v>
       </c>
       <c r="D174" t="s">
-        <v>710</v>
+        <v>744</v>
       </c>
       <c r="E174" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -7198,16 +7406,16 @@
         <v>181</v>
       </c>
       <c r="B175" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="C175" t="s">
-        <v>528</v>
+        <v>554</v>
       </c>
       <c r="D175" t="s">
-        <v>711</v>
+        <v>745</v>
       </c>
       <c r="E175" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -7215,186 +7423,452 @@
         <v>182</v>
       </c>
       <c r="B176" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="C176" t="s">
-        <v>529</v>
+        <v>555</v>
       </c>
       <c r="D176" t="s">
-        <v>712</v>
+        <v>746</v>
       </c>
       <c r="E176" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
         <v>183</v>
       </c>
       <c r="B177" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="C177" t="s">
-        <v>530</v>
+        <v>556</v>
       </c>
       <c r="D177" t="s">
-        <v>713</v>
+        <v>747</v>
       </c>
       <c r="E177" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
         <v>184</v>
       </c>
       <c r="B178" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
       <c r="C178" t="s">
-        <v>531</v>
+        <v>557</v>
       </c>
       <c r="D178" t="s">
-        <v>714</v>
+        <v>748</v>
       </c>
       <c r="E178" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
         <v>185</v>
       </c>
       <c r="B179" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="C179" t="s">
-        <v>532</v>
+        <v>558</v>
       </c>
       <c r="D179" t="s">
-        <v>715</v>
+        <v>749</v>
       </c>
       <c r="E179" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
         <v>186</v>
       </c>
       <c r="B180" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="C180" t="s">
-        <v>532</v>
+        <v>558</v>
       </c>
       <c r="D180" t="s">
-        <v>716</v>
+        <v>750</v>
       </c>
       <c r="E180" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
         <v>187</v>
       </c>
       <c r="B181" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="C181" t="s">
-        <v>532</v>
+        <v>558</v>
       </c>
       <c r="D181" t="s">
-        <v>717</v>
+        <v>751</v>
       </c>
       <c r="E181" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
         <v>188</v>
       </c>
       <c r="B182" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="C182" t="s">
-        <v>533</v>
+        <v>559</v>
       </c>
       <c r="D182" t="s">
-        <v>718</v>
+        <v>752</v>
       </c>
       <c r="E182" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5">
+        <v>776</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182">
+        <v>24</v>
+      </c>
+      <c r="H182">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
       <c r="A183" t="s">
         <v>189</v>
       </c>
       <c r="B183" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="C183" t="s">
-        <v>534</v>
+        <v>560</v>
       </c>
       <c r="D183" t="s">
-        <v>719</v>
+        <v>753</v>
       </c>
       <c r="E183" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5">
+        <v>776</v>
+      </c>
+      <c r="F183">
+        <v>1</v>
+      </c>
+      <c r="G183">
+        <v>24</v>
+      </c>
+      <c r="H183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
         <v>190</v>
       </c>
       <c r="B184" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="C184" t="s">
-        <v>535</v>
+        <v>561</v>
       </c>
       <c r="D184" t="s">
-        <v>720</v>
+        <v>754</v>
       </c>
       <c r="E184" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5">
+        <v>776</v>
+      </c>
+      <c r="F184">
+        <v>2</v>
+      </c>
+      <c r="G184">
+        <v>24</v>
+      </c>
+      <c r="H184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
         <v>191</v>
       </c>
       <c r="B185" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="C185" t="s">
-        <v>536</v>
+        <v>562</v>
       </c>
       <c r="D185" t="s">
-        <v>721</v>
+        <v>755</v>
       </c>
       <c r="E185" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5">
+        <v>776</v>
+      </c>
+      <c r="F185">
+        <v>3</v>
+      </c>
+      <c r="G185">
+        <v>64</v>
+      </c>
+      <c r="H185">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
         <v>192</v>
       </c>
       <c r="B186" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="C186" t="s">
-        <v>537</v>
+        <v>563</v>
       </c>
       <c r="D186" t="s">
-        <v>722</v>
+        <v>756</v>
       </c>
       <c r="E186" t="s">
-        <v>729</v>
+        <v>776</v>
+      </c>
+      <c r="F186">
+        <v>4</v>
+      </c>
+      <c r="G186">
+        <v>64</v>
+      </c>
+      <c r="H186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
+      <c r="A187" t="s">
+        <v>193</v>
+      </c>
+      <c r="B187" t="s">
+        <v>390</v>
+      </c>
+      <c r="C187" t="s">
+        <v>564</v>
+      </c>
+      <c r="D187" t="s">
+        <v>757</v>
+      </c>
+      <c r="E187" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8">
+      <c r="A188" t="s">
+        <v>194</v>
+      </c>
+      <c r="B188" t="s">
+        <v>391</v>
+      </c>
+      <c r="C188" t="s">
+        <v>564</v>
+      </c>
+      <c r="D188" t="s">
+        <v>758</v>
+      </c>
+      <c r="E188" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" t="s">
+        <v>195</v>
+      </c>
+      <c r="B189" t="s">
+        <v>392</v>
+      </c>
+      <c r="C189" t="s">
+        <v>564</v>
+      </c>
+      <c r="D189" t="s">
+        <v>759</v>
+      </c>
+      <c r="E189" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
+      <c r="A190" t="s">
+        <v>196</v>
+      </c>
+      <c r="B190" t="s">
+        <v>393</v>
+      </c>
+      <c r="C190" t="s">
+        <v>565</v>
+      </c>
+      <c r="D190" t="s">
+        <v>760</v>
+      </c>
+      <c r="E190" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8">
+      <c r="A191" t="s">
+        <v>197</v>
+      </c>
+      <c r="B191" t="s">
+        <v>394</v>
+      </c>
+      <c r="C191" t="s">
+        <v>566</v>
+      </c>
+      <c r="D191" t="s">
+        <v>761</v>
+      </c>
+      <c r="E191" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" t="s">
+        <v>198</v>
+      </c>
+      <c r="B192" t="s">
+        <v>395</v>
+      </c>
+      <c r="C192" t="s">
+        <v>567</v>
+      </c>
+      <c r="D192" t="s">
+        <v>762</v>
+      </c>
+      <c r="E192" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" t="s">
+        <v>199</v>
+      </c>
+      <c r="B193" t="s">
+        <v>396</v>
+      </c>
+      <c r="C193" t="s">
+        <v>568</v>
+      </c>
+      <c r="D193" t="s">
+        <v>763</v>
+      </c>
+      <c r="E193" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" t="s">
+        <v>200</v>
+      </c>
+      <c r="B194" t="s">
+        <v>397</v>
+      </c>
+      <c r="C194" t="s">
+        <v>568</v>
+      </c>
+      <c r="D194" t="s">
+        <v>764</v>
+      </c>
+      <c r="E194" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" t="s">
+        <v>201</v>
+      </c>
+      <c r="B195" t="s">
+        <v>398</v>
+      </c>
+      <c r="C195" t="s">
+        <v>568</v>
+      </c>
+      <c r="D195" t="s">
+        <v>765</v>
+      </c>
+      <c r="E195" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" t="s">
+        <v>202</v>
+      </c>
+      <c r="B196" t="s">
+        <v>399</v>
+      </c>
+      <c r="C196" t="s">
+        <v>568</v>
+      </c>
+      <c r="D196" t="s">
+        <v>766</v>
+      </c>
+      <c r="E196" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" t="s">
+        <v>203</v>
+      </c>
+      <c r="B197" t="s">
+        <v>400</v>
+      </c>
+      <c r="C197" t="s">
+        <v>569</v>
+      </c>
+      <c r="D197" t="s">
+        <v>767</v>
+      </c>
+      <c r="E197" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" t="s">
+        <v>204</v>
+      </c>
+      <c r="B198" t="s">
+        <v>401</v>
+      </c>
+      <c r="C198" t="s">
+        <v>570</v>
+      </c>
+      <c r="D198" t="s">
+        <v>768</v>
+      </c>
+      <c r="E198" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" t="s">
+        <v>205</v>
+      </c>
+      <c r="B199" t="s">
+        <v>402</v>
+      </c>
+      <c r="C199" t="s">
+        <v>571</v>
+      </c>
+      <c r="D199" t="s">
+        <v>769</v>
+      </c>
+      <c r="E199" t="s">
+        <v>776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor Multi-thread exp analysis code
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E4D62E-1F37-41A1-915D-6F41F6DA7029}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DAE3C6-4039-4165-8DFE-B8D6356E3FD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="798">
   <si>
     <t>ephysFN</t>
   </si>
@@ -1684,25 +1684,10 @@
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-06-Beto-01\2020-03-06-12-11-33</t>
   </si>
   <si>
-    <t>Stimuli\2019-12-Evolutions\2020-02-10-Beto-01\2020-02-10-14-18-32</t>
-  </si>
-  <si>
-    <t>Stimuli\2019-12-Evolutions\2020-02-10-Beto-02\2020-02-10-14-43-14</t>
-  </si>
-  <si>
-    <t>Stimuli\2019-12-Evolutions\2020-02-07-Beto-02\2020-02-07-10-23-49</t>
-  </si>
-  <si>
     <t>N:\Stimuli\2019-06-RF-mapping\2020-02-14-Beto</t>
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-02-14-Beto-01\2020-02-14-14-23-26</t>
-  </si>
-  <si>
-    <t>Stimuli\2019-12-Evolutions\2020-02-19-Beto-01\2020-02-19-14-23-48</t>
-  </si>
-  <si>
-    <t>Stimuli\2019-12-Evolutions\2020-02-20-Beto-01\2020-02-20-10-29-18</t>
   </si>
   <si>
     <t>N:\Stimuli\2019-06-RF-mapping\2020-03-11-Beto</t>
@@ -2931,6 +2916,21 @@
   </si>
   <si>
     <t>ReducDimen_Evol</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-02-10-Beto-01\2020-02-10-14-18-32</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-02-10-Beto-02\2020-02-10-14-43-14</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-02-07-Beto-02\2020-02-07-10-23-49</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-02-19-Beto-01\2020-02-19-14-23-48</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-02-20-Beto-01\2020-02-20-10-29-18</t>
   </si>
 </sst>
 </file>
@@ -2989,10 +2989,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3334,12 +3337,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="I196" sqref="I196"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="42.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="57.5703125" customWidth="1"/>
@@ -3382,10 +3386,10 @@
         <v>415</v>
       </c>
       <c r="D2" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="E2" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3408,10 +3412,10 @@
         <v>416</v>
       </c>
       <c r="D3" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="E3" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3434,10 +3438,10 @@
         <v>417</v>
       </c>
       <c r="D4" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="E4" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -3460,10 +3464,10 @@
         <v>418</v>
       </c>
       <c r="D5" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="E5" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -3486,10 +3490,10 @@
         <v>419</v>
       </c>
       <c r="D6" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="E6" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -3512,10 +3516,10 @@
         <v>420</v>
       </c>
       <c r="D7" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="E7" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -3538,10 +3542,10 @@
         <v>421</v>
       </c>
       <c r="D8" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="E8" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -3564,10 +3568,10 @@
         <v>422</v>
       </c>
       <c r="D9" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E9" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -3590,10 +3594,10 @@
         <v>423</v>
       </c>
       <c r="D10" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="E10" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -3616,10 +3620,10 @@
         <v>424</v>
       </c>
       <c r="D11" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="E11" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -3642,10 +3646,10 @@
         <v>425</v>
       </c>
       <c r="D12" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="E12" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3668,10 +3672,10 @@
         <v>426</v>
       </c>
       <c r="D13" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="E13" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3694,10 +3698,10 @@
         <v>427</v>
       </c>
       <c r="D14" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="E14" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -3720,10 +3724,10 @@
         <v>428</v>
       </c>
       <c r="D15" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E15" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -3746,10 +3750,10 @@
         <v>429</v>
       </c>
       <c r="D16" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="E16" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -3772,10 +3776,10 @@
         <v>430</v>
       </c>
       <c r="D17" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="E17" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -3798,10 +3802,10 @@
         <v>431</v>
       </c>
       <c r="D18" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E18" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -3824,10 +3828,10 @@
         <v>432</v>
       </c>
       <c r="D19" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="E19" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -3850,10 +3854,10 @@
         <v>433</v>
       </c>
       <c r="D20" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E20" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3876,10 +3880,10 @@
         <v>434</v>
       </c>
       <c r="D21" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E21" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3902,10 +3906,10 @@
         <v>435</v>
       </c>
       <c r="D22" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="E22" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -3928,10 +3932,10 @@
         <v>436</v>
       </c>
       <c r="D23" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="E23" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -3954,10 +3958,10 @@
         <v>437</v>
       </c>
       <c r="D24" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E24" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -3980,10 +3984,10 @@
         <v>438</v>
       </c>
       <c r="D25" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E25" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -4006,10 +4010,10 @@
         <v>439</v>
       </c>
       <c r="D26" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="E26" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -4032,10 +4036,10 @@
         <v>440</v>
       </c>
       <c r="D27" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="E27" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -4058,10 +4062,10 @@
         <v>441</v>
       </c>
       <c r="D28" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E28" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -4084,10 +4088,10 @@
         <v>442</v>
       </c>
       <c r="D29" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="E29" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -4110,10 +4114,10 @@
         <v>443</v>
       </c>
       <c r="D30" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E30" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -4136,10 +4140,10 @@
         <v>444</v>
       </c>
       <c r="D31" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="E31" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -4162,10 +4166,10 @@
         <v>445</v>
       </c>
       <c r="D32" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="E32" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -4188,10 +4192,10 @@
         <v>446</v>
       </c>
       <c r="D33" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E33" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -4214,10 +4218,10 @@
         <v>447</v>
       </c>
       <c r="D34" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="E34" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -4240,10 +4244,10 @@
         <v>448</v>
       </c>
       <c r="D35" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="E35" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -4266,10 +4270,10 @@
         <v>449</v>
       </c>
       <c r="D36" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="E36" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -4292,10 +4296,10 @@
         <v>450</v>
       </c>
       <c r="D37" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="E37" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -4318,10 +4322,10 @@
         <v>451</v>
       </c>
       <c r="D38" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="E38" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -4344,10 +4348,10 @@
         <v>452</v>
       </c>
       <c r="D39" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="E39" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -4370,10 +4374,10 @@
         <v>453</v>
       </c>
       <c r="D40" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E40" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -4396,10 +4400,10 @@
         <v>454</v>
       </c>
       <c r="D41" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="E41" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -4422,10 +4426,10 @@
         <v>455</v>
       </c>
       <c r="D42" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="E42" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -4448,10 +4452,10 @@
         <v>456</v>
       </c>
       <c r="D43" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="E43" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -4474,10 +4478,10 @@
         <v>457</v>
       </c>
       <c r="D44" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="E44" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -4500,10 +4504,10 @@
         <v>458</v>
       </c>
       <c r="D45" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E45" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -4526,10 +4530,10 @@
         <v>459</v>
       </c>
       <c r="D46" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="E46" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -4552,10 +4556,10 @@
         <v>460</v>
       </c>
       <c r="D47" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="E47" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -4578,10 +4582,10 @@
         <v>461</v>
       </c>
       <c r="D48" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="E48" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F48">
         <v>23</v>
@@ -4604,10 +4608,10 @@
         <v>462</v>
       </c>
       <c r="D49" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="E49" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F49">
         <v>23</v>
@@ -4630,10 +4634,10 @@
         <v>463</v>
       </c>
       <c r="D50" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="E50" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F50">
         <v>24</v>
@@ -4656,10 +4660,10 @@
         <v>464</v>
       </c>
       <c r="D51" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="E51" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -4682,10 +4686,10 @@
         <v>465</v>
       </c>
       <c r="D52" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="E52" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F52">
         <v>24</v>
@@ -4708,7 +4712,7 @@
         <v>466</v>
       </c>
       <c r="D53" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="F53">
         <v>24</v>
@@ -4731,10 +4735,10 @@
         <v>467</v>
       </c>
       <c r="D54" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E54" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -4757,10 +4761,10 @@
         <v>468</v>
       </c>
       <c r="D55" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="E55" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F55">
         <v>25</v>
@@ -4783,10 +4787,10 @@
         <v>469</v>
       </c>
       <c r="D56" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="E56" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F56">
         <v>25</v>
@@ -4809,10 +4813,10 @@
         <v>470</v>
       </c>
       <c r="D57" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="E57" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -4835,10 +4839,10 @@
         <v>471</v>
       </c>
       <c r="D58" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="E58" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -4861,10 +4865,10 @@
         <v>472</v>
       </c>
       <c r="D59" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="E59" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -4887,10 +4891,10 @@
         <v>473</v>
       </c>
       <c r="D60" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="E60" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F60">
         <v>27</v>
@@ -4913,10 +4917,10 @@
         <v>474</v>
       </c>
       <c r="D61" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="E61" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F61">
         <v>27</v>
@@ -4939,10 +4943,10 @@
         <v>475</v>
       </c>
       <c r="D62" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="E62" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F62">
         <v>27</v>
@@ -4965,10 +4969,10 @@
         <v>476</v>
       </c>
       <c r="D63" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="E63" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -4991,10 +4995,10 @@
         <v>477</v>
       </c>
       <c r="D64" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="E64" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -5017,10 +5021,10 @@
         <v>478</v>
       </c>
       <c r="D65" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="E65" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -5043,10 +5047,10 @@
         <v>479</v>
       </c>
       <c r="D66" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="E66" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -5069,10 +5073,10 @@
         <v>477</v>
       </c>
       <c r="D67" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="E67" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -5095,10 +5099,10 @@
         <v>480</v>
       </c>
       <c r="D68" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="E68" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -5121,10 +5125,10 @@
         <v>481</v>
       </c>
       <c r="D69" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="E69" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -5147,10 +5151,10 @@
         <v>482</v>
       </c>
       <c r="D70" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="E70" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -5173,10 +5177,10 @@
         <v>483</v>
       </c>
       <c r="D71" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="E71" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -5199,10 +5203,10 @@
         <v>484</v>
       </c>
       <c r="D72" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="E72" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -5225,10 +5229,10 @@
         <v>485</v>
       </c>
       <c r="D73" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="E73" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -5251,10 +5255,10 @@
         <v>486</v>
       </c>
       <c r="D74" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E74" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -5277,10 +5281,10 @@
         <v>487</v>
       </c>
       <c r="D75" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="E75" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -5303,10 +5307,10 @@
         <v>488</v>
       </c>
       <c r="D76" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="E76" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -5329,10 +5333,10 @@
         <v>489</v>
       </c>
       <c r="D77" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="E77" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -5355,10 +5359,10 @@
         <v>490</v>
       </c>
       <c r="D78" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="E78" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -5381,10 +5385,10 @@
         <v>491</v>
       </c>
       <c r="D79" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="E79" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -5407,10 +5411,10 @@
         <v>492</v>
       </c>
       <c r="D80" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="E80" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -5433,7 +5437,7 @@
         <v>493</v>
       </c>
       <c r="D81" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -5456,7 +5460,7 @@
         <v>493</v>
       </c>
       <c r="D82" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -5476,10 +5480,10 @@
         <v>493</v>
       </c>
       <c r="D83" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="E83" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -5502,10 +5506,10 @@
         <v>494</v>
       </c>
       <c r="D84" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="E84" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -5528,10 +5532,10 @@
         <v>495</v>
       </c>
       <c r="D85" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="E85" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F85">
         <v>35</v>
@@ -5554,10 +5558,10 @@
         <v>496</v>
       </c>
       <c r="D86" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="E86" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -5580,10 +5584,10 @@
         <v>497</v>
       </c>
       <c r="D87" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="E87" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F87">
         <v>36</v>
@@ -5606,10 +5610,10 @@
         <v>498</v>
       </c>
       <c r="D88" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="E88" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -5632,10 +5636,10 @@
         <v>499</v>
       </c>
       <c r="D89" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="E89" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -5658,10 +5662,10 @@
         <v>500</v>
       </c>
       <c r="D90" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="E90" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F90">
         <v>37</v>
@@ -5684,10 +5688,10 @@
         <v>501</v>
       </c>
       <c r="D91" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="E91" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -5710,10 +5714,10 @@
         <v>502</v>
       </c>
       <c r="D92" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="E92" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F92">
         <v>38</v>
@@ -5736,10 +5740,10 @@
         <v>503</v>
       </c>
       <c r="D93" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="E93" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -5762,10 +5766,10 @@
         <v>504</v>
       </c>
       <c r="D94" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="E94" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -5788,10 +5792,10 @@
         <v>505</v>
       </c>
       <c r="D95" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="E95" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F95">
         <v>39</v>
@@ -5814,10 +5818,10 @@
         <v>506</v>
       </c>
       <c r="D96" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="E96" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -5840,10 +5844,10 @@
         <v>507</v>
       </c>
       <c r="D97" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="E97" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -5866,10 +5870,10 @@
         <v>508</v>
       </c>
       <c r="D98" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="E98" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -5892,10 +5896,10 @@
         <v>509</v>
       </c>
       <c r="D99" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="E99" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -5918,10 +5922,10 @@
         <v>510</v>
       </c>
       <c r="D100" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="E100" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F100">
         <v>41</v>
@@ -5944,10 +5948,10 @@
         <v>511</v>
       </c>
       <c r="D101" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="E101" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="F101">
         <v>41</v>
@@ -5964,10 +5968,10 @@
         <v>512</v>
       </c>
       <c r="D102" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="E102" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -5990,10 +5994,10 @@
         <v>513</v>
       </c>
       <c r="D103" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="E103" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -6016,10 +6020,10 @@
         <v>514</v>
       </c>
       <c r="D104" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="E104" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F104">
         <v>42</v>
@@ -6042,10 +6046,10 @@
         <v>515</v>
       </c>
       <c r="D105" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="E105" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -6068,10 +6072,10 @@
         <v>513</v>
       </c>
       <c r="D106" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="E106" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -6094,10 +6098,10 @@
         <v>516</v>
       </c>
       <c r="D107" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="E107" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F107">
         <v>43</v>
@@ -6120,10 +6124,10 @@
         <v>517</v>
       </c>
       <c r="D108" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="E108" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="F108">
         <v>43</v>
@@ -6140,10 +6144,10 @@
         <v>517</v>
       </c>
       <c r="D109" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="E109" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="F109">
         <v>43</v>
@@ -6160,10 +6164,10 @@
         <v>518</v>
       </c>
       <c r="D110" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="E110" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -6186,10 +6190,10 @@
         <v>519</v>
       </c>
       <c r="D111" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="E111" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -6212,10 +6216,10 @@
         <v>518</v>
       </c>
       <c r="D112" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="E112" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F112">
         <v>44</v>
@@ -6238,10 +6242,10 @@
         <v>520</v>
       </c>
       <c r="D113" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="E113" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -6264,10 +6268,10 @@
         <v>521</v>
       </c>
       <c r="D114" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="E114" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -6290,10 +6294,10 @@
         <v>522</v>
       </c>
       <c r="D115" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="E115" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F115">
         <v>45</v>
@@ -6316,10 +6320,10 @@
         <v>523</v>
       </c>
       <c r="D116" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="E116" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -6336,10 +6340,10 @@
         <v>524</v>
       </c>
       <c r="D117" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="E117" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -6362,10 +6366,10 @@
         <v>525</v>
       </c>
       <c r="D118" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="E118" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="H118">
         <v>2</v>
@@ -6382,10 +6386,10 @@
         <v>526</v>
       </c>
       <c r="D119" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E119" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -6408,10 +6412,10 @@
         <v>527</v>
       </c>
       <c r="D120" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E120" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -6434,10 +6438,10 @@
         <v>528</v>
       </c>
       <c r="D121" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E121" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="H121">
         <v>2</v>
@@ -6454,10 +6458,10 @@
         <v>529</v>
       </c>
       <c r="D122" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E122" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -6480,7 +6484,7 @@
         <v>530</v>
       </c>
       <c r="D123" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="G123">
         <v>41</v>
@@ -6500,10 +6504,10 @@
         <v>528</v>
       </c>
       <c r="D124" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E124" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="H124">
         <v>3</v>
@@ -6520,10 +6524,10 @@
         <v>528</v>
       </c>
       <c r="D125" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="E125" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -6540,10 +6544,10 @@
         <v>531</v>
       </c>
       <c r="D126" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="E126" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F126">
         <v>5</v>
@@ -6566,10 +6570,10 @@
         <v>532</v>
       </c>
       <c r="D127" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="E127" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -6583,7 +6587,7 @@
         <v>533</v>
       </c>
       <c r="D128" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="G128">
         <v>26</v>
@@ -6603,10 +6607,10 @@
         <v>534</v>
       </c>
       <c r="D129" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="E129" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -6629,7 +6633,7 @@
         <v>535</v>
       </c>
       <c r="D130" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="H130">
         <v>2</v>
@@ -6646,7 +6650,7 @@
         <v>535</v>
       </c>
       <c r="D131" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -6663,10 +6667,10 @@
         <v>536</v>
       </c>
       <c r="D132" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="E132" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -6689,10 +6693,10 @@
         <v>537</v>
       </c>
       <c r="D133" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="E133" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F133">
         <v>7</v>
@@ -6715,10 +6719,10 @@
         <v>538</v>
       </c>
       <c r="D134" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="E134" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="H134">
         <v>0.75</v>
@@ -6735,10 +6739,10 @@
         <v>538</v>
       </c>
       <c r="D135" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="E135" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="H135">
         <v>2</v>
@@ -6755,10 +6759,10 @@
         <v>539</v>
       </c>
       <c r="D136" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="E136" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -6781,10 +6785,10 @@
         <v>540</v>
       </c>
       <c r="D137" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="E137" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F137">
         <v>2</v>
@@ -6807,10 +6811,10 @@
         <v>541</v>
       </c>
       <c r="D138" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="E138" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F138">
         <v>3</v>
@@ -6833,10 +6837,10 @@
         <v>542</v>
       </c>
       <c r="D139" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="E139" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F139">
         <v>4</v>
@@ -6859,10 +6863,10 @@
         <v>543</v>
       </c>
       <c r="D140" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="E140" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="H140">
         <v>0.75</v>
@@ -6879,10 +6883,10 @@
         <v>543</v>
       </c>
       <c r="D141" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="E141" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="H141">
         <v>2</v>
@@ -6899,10 +6903,10 @@
         <v>544</v>
       </c>
       <c r="D142" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="E142" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F142">
         <v>5</v>
@@ -6925,10 +6929,10 @@
         <v>545</v>
       </c>
       <c r="D143" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="E143" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F143">
         <v>6</v>
@@ -6951,10 +6955,10 @@
         <v>546</v>
       </c>
       <c r="D144" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="E144" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="H144">
         <v>0.75</v>
@@ -6971,10 +6975,10 @@
         <v>546</v>
       </c>
       <c r="D145" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="E145" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="H145">
         <v>2</v>
@@ -6991,10 +6995,10 @@
         <v>547</v>
       </c>
       <c r="D146" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="E146" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F146">
         <v>101</v>
@@ -7017,10 +7021,13 @@
         <v>548</v>
       </c>
       <c r="D147" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="E147" t="s">
-        <v>794</v>
+        <v>789</v>
+      </c>
+      <c r="F147">
+        <v>2</v>
       </c>
       <c r="G147">
         <v>24</v>
@@ -7040,10 +7047,10 @@
         <v>549</v>
       </c>
       <c r="D148" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="E148" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -7066,10 +7073,10 @@
         <v>550</v>
       </c>
       <c r="D149" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="E149" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="H149">
         <v>0.75</v>
@@ -7086,10 +7093,10 @@
         <v>550</v>
       </c>
       <c r="D150" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="E150" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="H150">
         <v>2</v>
@@ -7106,10 +7113,10 @@
         <v>551</v>
       </c>
       <c r="D151" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="E151" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -7132,10 +7139,10 @@
         <v>552</v>
       </c>
       <c r="D152" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="E152" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="F152">
         <v>3</v>
@@ -7155,10 +7162,10 @@
         <v>362</v>
       </c>
       <c r="D153" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="E153" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -7172,10 +7179,13 @@
         <v>553</v>
       </c>
       <c r="D154" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="E154" t="s">
-        <v>794</v>
+        <v>789</v>
+      </c>
+      <c r="F154">
+        <v>3</v>
       </c>
       <c r="G154">
         <v>24</v>
@@ -7192,10 +7202,10 @@
         <v>364</v>
       </c>
       <c r="D155" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="E155" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -7206,10 +7216,10 @@
         <v>365</v>
       </c>
       <c r="D156" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="E156" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -7220,13 +7230,10 @@
         <v>366</v>
       </c>
       <c r="C157" t="s">
-        <v>554</v>
+        <v>793</v>
       </c>
       <c r="D157" t="s">
-        <v>742</v>
-      </c>
-      <c r="E157" t="s">
-        <v>794</v>
+        <v>737</v>
       </c>
       <c r="G157">
         <v>39</v>
@@ -7240,13 +7247,16 @@
         <v>367</v>
       </c>
       <c r="C158" t="s">
-        <v>555</v>
+        <v>794</v>
       </c>
       <c r="D158" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="E158" t="s">
-        <v>794</v>
+        <v>789</v>
+      </c>
+      <c r="F158">
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -7257,13 +7267,13 @@
         <v>368</v>
       </c>
       <c r="D159" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="E159" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>166</v>
       </c>
@@ -7271,13 +7281,16 @@
         <v>369</v>
       </c>
       <c r="C160" t="s">
-        <v>556</v>
-      </c>
-      <c r="D160" t="s">
-        <v>745</v>
+        <v>795</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>740</v>
       </c>
       <c r="E160" t="s">
-        <v>794</v>
+        <v>789</v>
+      </c>
+      <c r="F160">
+        <v>5</v>
       </c>
       <c r="G160">
         <v>39</v>
@@ -7291,13 +7304,13 @@
         <v>370</v>
       </c>
       <c r="C161" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D161" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="E161" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -7308,13 +7321,13 @@
         <v>371</v>
       </c>
       <c r="C162" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D162" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="E162" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -7325,13 +7338,16 @@
         <v>372</v>
       </c>
       <c r="C163" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D163" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="E163" t="s">
-        <v>794</v>
+        <v>789</v>
+      </c>
+      <c r="F163">
+        <v>6</v>
       </c>
       <c r="G163">
         <v>39</v>
@@ -7345,13 +7361,16 @@
         <v>373</v>
       </c>
       <c r="C164" t="s">
-        <v>559</v>
+        <v>796</v>
       </c>
       <c r="D164" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="E164" t="s">
-        <v>794</v>
+        <v>789</v>
+      </c>
+      <c r="F164">
+        <v>7</v>
       </c>
       <c r="G164">
         <v>25</v>
@@ -7365,10 +7384,10 @@
         <v>374</v>
       </c>
       <c r="D165" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="E165" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -7379,10 +7398,10 @@
         <v>375</v>
       </c>
       <c r="D166" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="E166" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -7393,13 +7412,16 @@
         <v>376</v>
       </c>
       <c r="C167" t="s">
-        <v>560</v>
+        <v>797</v>
       </c>
       <c r="D167" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="E167" t="s">
-        <v>794</v>
+        <v>789</v>
+      </c>
+      <c r="F167">
+        <v>8</v>
       </c>
       <c r="G167">
         <v>41</v>
@@ -7413,13 +7435,13 @@
         <v>377</v>
       </c>
       <c r="C168" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D168" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="E168" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -7430,13 +7452,13 @@
         <v>378</v>
       </c>
       <c r="C169" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D169" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="E169" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -7447,13 +7469,13 @@
         <v>379</v>
       </c>
       <c r="C170" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D170" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="E170" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="F170">
         <v>4</v>
@@ -7473,13 +7495,13 @@
         <v>380</v>
       </c>
       <c r="C171" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="D171" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="E171" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="F171">
         <v>5</v>
@@ -7499,13 +7521,13 @@
         <v>381</v>
       </c>
       <c r="C172" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="D172" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="E172" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="F172">
         <v>6</v>
@@ -7525,13 +7547,13 @@
         <v>382</v>
       </c>
       <c r="C173" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D173" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="E173" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -7542,13 +7564,13 @@
         <v>383</v>
       </c>
       <c r="C174" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D174" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="E174" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -7559,13 +7581,13 @@
         <v>384</v>
       </c>
       <c r="C175" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D175" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="E175" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -7576,13 +7598,13 @@
         <v>385</v>
       </c>
       <c r="C176" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D176" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="E176" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -7593,13 +7615,13 @@
         <v>386</v>
       </c>
       <c r="C177" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="D177" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="E177" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -7610,13 +7632,13 @@
         <v>387</v>
       </c>
       <c r="C178" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="D178" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="E178" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -7627,13 +7649,13 @@
         <v>388</v>
       </c>
       <c r="C179" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="D179" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="E179" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -7644,13 +7666,13 @@
         <v>389</v>
       </c>
       <c r="C180" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="D180" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="E180" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -7661,13 +7683,13 @@
         <v>390</v>
       </c>
       <c r="C181" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="D181" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E181" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -7678,13 +7700,13 @@
         <v>391</v>
       </c>
       <c r="C182" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="D182" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="E182" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F182">
         <v>0</v>
@@ -7704,13 +7726,13 @@
         <v>392</v>
       </c>
       <c r="C183" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="D183" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="E183" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F183">
         <v>1</v>
@@ -7730,13 +7752,13 @@
         <v>393</v>
       </c>
       <c r="C184" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="D184" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="E184" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F184">
         <v>2</v>
@@ -7756,13 +7778,13 @@
         <v>394</v>
       </c>
       <c r="C185" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="D185" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="E185" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F185">
         <v>3</v>
@@ -7782,13 +7804,13 @@
         <v>395</v>
       </c>
       <c r="C186" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="D186" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="E186" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F186">
         <v>4</v>
@@ -7808,13 +7830,13 @@
         <v>396</v>
       </c>
       <c r="C187" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="D187" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="E187" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -7825,13 +7847,13 @@
         <v>397</v>
       </c>
       <c r="C188" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="D188" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="E188" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -7842,13 +7864,13 @@
         <v>398</v>
       </c>
       <c r="C189" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="D189" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="E189" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -7859,13 +7881,13 @@
         <v>399</v>
       </c>
       <c r="C190" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="D190" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="E190" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F190">
         <v>5</v>
@@ -7885,13 +7907,13 @@
         <v>400</v>
       </c>
       <c r="C191" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="D191" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="E191" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F191">
         <v>6</v>
@@ -7911,13 +7933,13 @@
         <v>401</v>
       </c>
       <c r="C192" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D192" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="E192" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F192">
         <v>7</v>
@@ -7937,13 +7959,13 @@
         <v>402</v>
       </c>
       <c r="C193" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="D193" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="E193" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -7954,13 +7976,13 @@
         <v>403</v>
       </c>
       <c r="C194" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="D194" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="E194" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -7971,13 +7993,13 @@
         <v>404</v>
       </c>
       <c r="C195" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="D195" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="E195" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -7988,13 +8010,13 @@
         <v>405</v>
       </c>
       <c r="C196" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="D196" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="E196" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -8005,13 +8027,13 @@
         <v>406</v>
       </c>
       <c r="C197" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="D197" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="E197" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F197">
         <v>8</v>
@@ -8031,13 +8053,13 @@
         <v>407</v>
       </c>
       <c r="C198" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="D198" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="E198" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F198">
         <v>9</v>
@@ -8057,13 +8079,13 @@
         <v>408</v>
       </c>
       <c r="C199" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="D199" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="E199" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F199">
         <v>10</v>
@@ -8083,10 +8105,10 @@
         <v>409</v>
       </c>
       <c r="D200" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="E200" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -8097,10 +8119,10 @@
         <v>410</v>
       </c>
       <c r="D201" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="E201" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -8111,10 +8133,10 @@
         <v>411</v>
       </c>
       <c r="D202" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="E202" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -8125,13 +8147,13 @@
         <v>412</v>
       </c>
       <c r="C203" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="D203" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="E203" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F203">
         <v>11</v>
@@ -8151,13 +8173,13 @@
         <v>413</v>
       </c>
       <c r="C204" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="D204" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="E204" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F204">
         <v>12</v>
@@ -8177,13 +8199,13 @@
         <v>414</v>
       </c>
       <c r="C205" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="D205" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="E205" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F205">
         <v>13</v>

</xml_diff>

<commit_message>
Add function to collect stats
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DAE3C6-4039-4165-8DFE-B8D6356E3FD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8353D00A-89FD-4F33-BF38-FE8193AB3677}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="799">
   <si>
     <t>ephysFN</t>
   </si>
@@ -2931,6 +2931,9 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-02-20-Beto-01\2020-02-20-10-29-18</t>
+  </si>
+  <si>
+    <t>191125_Beto_selectivity_basic(1)_cmb</t>
   </si>
 </sst>
 </file>
@@ -3337,8 +3340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5476,6 +5479,9 @@
       <c r="A83" t="s">
         <v>89</v>
       </c>
+      <c r="B83" t="s">
+        <v>798</v>
+      </c>
       <c r="C83" t="s">
         <v>493</v>
       </c>

</xml_diff>

<commit_message>
Add code and notes
</commit_message>
<xml_diff>
--- a/ExpSpecTable_Augment.xlsx
+++ b/ExpSpecTable_Augment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285F80B2-0E2B-425B-AD38-C3FA8FB646A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105AA5CA-AD49-464D-8C61-DC6340116AA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2250" windowWidth="26295" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="1560" windowWidth="26295" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2063,9 +2063,6 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-04-10-Beto-01\2020-04-10-14-13-19</t>
-  </si>
-  <si>
-    <t>N:\Stimuli\2019-12-Evolutions\2020-04-10-Beto-02</t>
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-04-10-Beto-03\2020-04-10-15-13-34</t>
@@ -3543,6 +3540,9 @@
   </si>
   <si>
     <t>ReducDimen_Evol</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-04-10-Beto-02\2020-04-10-14-54-53</t>
   </si>
 </sst>
 </file>
@@ -3946,13 +3946,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="F249" sqref="F249"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="92.42578125" customWidth="1"/>
     <col min="4" max="4" width="89.140625" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
   </cols>
@@ -3994,10 +3995,10 @@
         <v>502</v>
       </c>
       <c r="D2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -4020,10 +4021,10 @@
         <v>503</v>
       </c>
       <c r="D3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4046,10 +4047,10 @@
         <v>504</v>
       </c>
       <c r="D4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E4" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -4072,10 +4073,10 @@
         <v>505</v>
       </c>
       <c r="D5" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E5" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -4098,10 +4099,10 @@
         <v>506</v>
       </c>
       <c r="D6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E6" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -4124,10 +4125,10 @@
         <v>507</v>
       </c>
       <c r="D7" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E7" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -4150,10 +4151,10 @@
         <v>508</v>
       </c>
       <c r="D8" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E8" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -4176,10 +4177,10 @@
         <v>509</v>
       </c>
       <c r="D9" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E9" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -4202,10 +4203,10 @@
         <v>510</v>
       </c>
       <c r="D10" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E10" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -4228,10 +4229,10 @@
         <v>511</v>
       </c>
       <c r="D11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E11" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -4254,10 +4255,10 @@
         <v>512</v>
       </c>
       <c r="D12" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E12" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -4280,10 +4281,10 @@
         <v>513</v>
       </c>
       <c r="D13" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E13" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -4306,10 +4307,10 @@
         <v>514</v>
       </c>
       <c r="D14" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E14" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -4332,10 +4333,10 @@
         <v>515</v>
       </c>
       <c r="D15" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E15" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -4358,10 +4359,10 @@
         <v>516</v>
       </c>
       <c r="D16" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E16" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -4384,10 +4385,10 @@
         <v>517</v>
       </c>
       <c r="D17" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E17" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -4410,10 +4411,10 @@
         <v>518</v>
       </c>
       <c r="D18" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E18" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -4436,10 +4437,10 @@
         <v>519</v>
       </c>
       <c r="D19" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E19" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -4462,10 +4463,10 @@
         <v>520</v>
       </c>
       <c r="D20" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E20" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -4488,10 +4489,10 @@
         <v>521</v>
       </c>
       <c r="D21" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E21" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -4514,10 +4515,10 @@
         <v>522</v>
       </c>
       <c r="D22" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E22" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F22">
         <v>11</v>
@@ -4540,10 +4541,10 @@
         <v>523</v>
       </c>
       <c r="D23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E23" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F23">
         <v>11</v>
@@ -4566,10 +4567,10 @@
         <v>524</v>
       </c>
       <c r="D24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E24" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -4592,10 +4593,10 @@
         <v>525</v>
       </c>
       <c r="D25" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F25">
         <v>12</v>
@@ -4618,10 +4619,10 @@
         <v>526</v>
       </c>
       <c r="D26" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E26" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F26">
         <v>13</v>
@@ -4644,10 +4645,10 @@
         <v>527</v>
       </c>
       <c r="D27" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E27" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F27">
         <v>13</v>
@@ -4670,10 +4671,10 @@
         <v>528</v>
       </c>
       <c r="D28" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E28" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -4696,10 +4697,10 @@
         <v>529</v>
       </c>
       <c r="D29" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E29" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F29">
         <v>14</v>
@@ -4722,10 +4723,10 @@
         <v>530</v>
       </c>
       <c r="D30" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E30" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F30">
         <v>15</v>
@@ -4748,10 +4749,10 @@
         <v>531</v>
       </c>
       <c r="D31" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E31" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F31">
         <v>15</v>
@@ -4774,10 +4775,10 @@
         <v>532</v>
       </c>
       <c r="D32" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E32" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F32">
         <v>16</v>
@@ -4800,10 +4801,10 @@
         <v>533</v>
       </c>
       <c r="D33" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E33" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -4826,10 +4827,10 @@
         <v>534</v>
       </c>
       <c r="D34" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E34" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F34">
         <v>17</v>
@@ -4852,10 +4853,10 @@
         <v>535</v>
       </c>
       <c r="D35" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E35" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F35">
         <v>17</v>
@@ -4878,10 +4879,10 @@
         <v>536</v>
       </c>
       <c r="D36" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E36" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F36">
         <v>18</v>
@@ -4904,10 +4905,10 @@
         <v>537</v>
       </c>
       <c r="D37" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E37" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F37">
         <v>18</v>
@@ -4930,10 +4931,10 @@
         <v>538</v>
       </c>
       <c r="D38" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E38" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F38">
         <v>19</v>
@@ -4956,10 +4957,10 @@
         <v>539</v>
       </c>
       <c r="D39" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E39" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F39">
         <v>19</v>
@@ -4982,10 +4983,10 @@
         <v>540</v>
       </c>
       <c r="D40" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E40" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -5008,10 +5009,10 @@
         <v>541</v>
       </c>
       <c r="D41" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E41" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F41">
         <v>20</v>
@@ -5034,10 +5035,10 @@
         <v>542</v>
       </c>
       <c r="D42" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E42" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F42">
         <v>21</v>
@@ -5060,10 +5061,10 @@
         <v>543</v>
       </c>
       <c r="D43" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E43" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F43">
         <v>21</v>
@@ -5086,10 +5087,10 @@
         <v>544</v>
       </c>
       <c r="D44" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E44" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F44">
         <v>22</v>
@@ -5112,10 +5113,10 @@
         <v>545</v>
       </c>
       <c r="D45" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F45">
         <v>22</v>
@@ -5138,10 +5139,10 @@
         <v>546</v>
       </c>
       <c r="D46" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E46" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F46">
         <v>22</v>
@@ -5164,10 +5165,10 @@
         <v>547</v>
       </c>
       <c r="D47" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E47" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F47">
         <v>23</v>
@@ -5190,10 +5191,10 @@
         <v>548</v>
       </c>
       <c r="D48" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E48" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F48">
         <v>23</v>
@@ -5216,10 +5217,10 @@
         <v>549</v>
       </c>
       <c r="D49" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E49" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F49">
         <v>23</v>
@@ -5242,10 +5243,10 @@
         <v>550</v>
       </c>
       <c r="D50" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E50" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F50">
         <v>24</v>
@@ -5268,10 +5269,10 @@
         <v>551</v>
       </c>
       <c r="D51" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E51" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -5294,10 +5295,10 @@
         <v>552</v>
       </c>
       <c r="D52" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E52" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F52">
         <v>24</v>
@@ -5320,7 +5321,7 @@
         <v>553</v>
       </c>
       <c r="D53" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F53">
         <v>24</v>
@@ -5343,10 +5344,10 @@
         <v>554</v>
       </c>
       <c r="D54" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E54" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -5369,10 +5370,10 @@
         <v>555</v>
       </c>
       <c r="D55" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E55" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F55">
         <v>25</v>
@@ -5395,10 +5396,10 @@
         <v>556</v>
       </c>
       <c r="D56" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E56" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F56">
         <v>25</v>
@@ -5421,10 +5422,10 @@
         <v>557</v>
       </c>
       <c r="D57" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E57" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F57">
         <v>26</v>
@@ -5447,10 +5448,10 @@
         <v>558</v>
       </c>
       <c r="D58" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E58" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F58">
         <v>26</v>
@@ -5473,10 +5474,10 @@
         <v>559</v>
       </c>
       <c r="D59" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E59" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F59">
         <v>26</v>
@@ -5499,10 +5500,10 @@
         <v>560</v>
       </c>
       <c r="D60" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E60" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F60">
         <v>27</v>
@@ -5525,10 +5526,10 @@
         <v>561</v>
       </c>
       <c r="D61" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E61" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F61">
         <v>27</v>
@@ -5551,10 +5552,10 @@
         <v>562</v>
       </c>
       <c r="D62" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E62" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F62">
         <v>27</v>
@@ -5577,10 +5578,10 @@
         <v>563</v>
       </c>
       <c r="D63" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E63" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F63">
         <v>28</v>
@@ -5603,10 +5604,10 @@
         <v>564</v>
       </c>
       <c r="D64" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E64" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F64">
         <v>28</v>
@@ -5629,10 +5630,10 @@
         <v>565</v>
       </c>
       <c r="D65" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E65" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -5655,10 +5656,10 @@
         <v>566</v>
       </c>
       <c r="D66" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E66" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F66">
         <v>29</v>
@@ -5681,10 +5682,10 @@
         <v>564</v>
       </c>
       <c r="D67" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E67" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F67">
         <v>29</v>
@@ -5707,10 +5708,10 @@
         <v>567</v>
       </c>
       <c r="D68" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E68" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F68">
         <v>29</v>
@@ -5733,10 +5734,10 @@
         <v>568</v>
       </c>
       <c r="D69" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E69" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F69">
         <v>30</v>
@@ -5759,10 +5760,10 @@
         <v>569</v>
       </c>
       <c r="D70" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E70" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F70">
         <v>30</v>
@@ -5785,10 +5786,10 @@
         <v>570</v>
       </c>
       <c r="D71" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E71" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F71">
         <v>30</v>
@@ -5811,10 +5812,10 @@
         <v>571</v>
       </c>
       <c r="D72" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E72" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F72">
         <v>31</v>
@@ -5837,10 +5838,10 @@
         <v>572</v>
       </c>
       <c r="D73" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E73" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F73">
         <v>31</v>
@@ -5863,10 +5864,10 @@
         <v>573</v>
       </c>
       <c r="D74" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E74" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F74">
         <v>32</v>
@@ -5889,10 +5890,10 @@
         <v>574</v>
       </c>
       <c r="D75" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E75" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F75">
         <v>32</v>
@@ -5915,10 +5916,10 @@
         <v>575</v>
       </c>
       <c r="D76" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E76" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F76">
         <v>33</v>
@@ -5941,10 +5942,10 @@
         <v>576</v>
       </c>
       <c r="D77" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E77" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F77">
         <v>33</v>
@@ -5967,10 +5968,10 @@
         <v>577</v>
       </c>
       <c r="D78" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E78" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F78">
         <v>33</v>
@@ -5993,10 +5994,10 @@
         <v>578</v>
       </c>
       <c r="D79" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E79" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -6019,10 +6020,10 @@
         <v>579</v>
       </c>
       <c r="D80" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E80" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F80">
         <v>34</v>
@@ -6045,7 +6046,7 @@
         <v>580</v>
       </c>
       <c r="D81" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F81">
         <v>35</v>
@@ -6068,7 +6069,7 @@
         <v>580</v>
       </c>
       <c r="D82" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F82">
         <v>35</v>
@@ -6091,10 +6092,10 @@
         <v>580</v>
       </c>
       <c r="D83" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E83" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F83">
         <v>35</v>
@@ -6117,10 +6118,10 @@
         <v>581</v>
       </c>
       <c r="D84" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E84" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F84">
         <v>35</v>
@@ -6143,10 +6144,10 @@
         <v>582</v>
       </c>
       <c r="D85" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E85" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F85">
         <v>35</v>
@@ -6169,10 +6170,10 @@
         <v>583</v>
       </c>
       <c r="D86" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E86" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F86">
         <v>36</v>
@@ -6195,10 +6196,10 @@
         <v>584</v>
       </c>
       <c r="D87" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E87" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F87">
         <v>36</v>
@@ -6221,10 +6222,10 @@
         <v>585</v>
       </c>
       <c r="D88" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E88" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F88">
         <v>37</v>
@@ -6247,10 +6248,10 @@
         <v>586</v>
       </c>
       <c r="D89" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E89" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F89">
         <v>37</v>
@@ -6273,10 +6274,10 @@
         <v>587</v>
       </c>
       <c r="D90" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E90" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F90">
         <v>37</v>
@@ -6299,10 +6300,10 @@
         <v>588</v>
       </c>
       <c r="D91" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E91" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F91">
         <v>38</v>
@@ -6325,10 +6326,10 @@
         <v>589</v>
       </c>
       <c r="D92" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E92" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F92">
         <v>38</v>
@@ -6351,10 +6352,10 @@
         <v>590</v>
       </c>
       <c r="D93" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E93" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -6377,10 +6378,10 @@
         <v>591</v>
       </c>
       <c r="D94" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E94" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F94">
         <v>39</v>
@@ -6403,10 +6404,10 @@
         <v>592</v>
       </c>
       <c r="D95" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E95" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F95">
         <v>39</v>
@@ -6429,10 +6430,10 @@
         <v>593</v>
       </c>
       <c r="D96" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E96" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F96">
         <v>40</v>
@@ -6455,10 +6456,10 @@
         <v>594</v>
       </c>
       <c r="D97" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E97" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -6481,10 +6482,10 @@
         <v>595</v>
       </c>
       <c r="D98" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E98" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F98">
         <v>41</v>
@@ -6507,10 +6508,10 @@
         <v>596</v>
       </c>
       <c r="D99" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E99" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F99">
         <v>41</v>
@@ -6533,10 +6534,10 @@
         <v>597</v>
       </c>
       <c r="D100" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E100" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F100">
         <v>41</v>
@@ -6559,10 +6560,10 @@
         <v>598</v>
       </c>
       <c r="D101" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E101" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F101">
         <v>41</v>
@@ -6579,10 +6580,10 @@
         <v>599</v>
       </c>
       <c r="D102" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E102" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F102">
         <v>42</v>
@@ -6605,10 +6606,10 @@
         <v>600</v>
       </c>
       <c r="D103" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E103" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F103">
         <v>42</v>
@@ -6631,10 +6632,10 @@
         <v>601</v>
       </c>
       <c r="D104" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E104" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F104">
         <v>42</v>
@@ -6657,10 +6658,10 @@
         <v>602</v>
       </c>
       <c r="D105" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E105" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F105">
         <v>43</v>
@@ -6683,10 +6684,10 @@
         <v>600</v>
       </c>
       <c r="D106" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E106" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F106">
         <v>43</v>
@@ -6709,10 +6710,10 @@
         <v>603</v>
       </c>
       <c r="D107" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E107" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F107">
         <v>43</v>
@@ -6735,10 +6736,10 @@
         <v>604</v>
       </c>
       <c r="D108" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E108" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F108">
         <v>43</v>
@@ -6755,10 +6756,10 @@
         <v>604</v>
       </c>
       <c r="D109" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E109" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F109">
         <v>43</v>
@@ -6775,10 +6776,10 @@
         <v>605</v>
       </c>
       <c r="D110" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E110" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F110">
         <v>44</v>
@@ -6801,10 +6802,10 @@
         <v>606</v>
       </c>
       <c r="D111" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E111" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F111">
         <v>44</v>
@@ -6827,10 +6828,10 @@
         <v>605</v>
       </c>
       <c r="D112" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E112" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F112">
         <v>44</v>
@@ -6853,10 +6854,10 @@
         <v>607</v>
       </c>
       <c r="D113" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E113" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F113">
         <v>45</v>
@@ -6879,10 +6880,10 @@
         <v>608</v>
       </c>
       <c r="D114" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E114" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F114">
         <v>45</v>
@@ -6905,10 +6906,10 @@
         <v>609</v>
       </c>
       <c r="D115" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E115" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F115">
         <v>45</v>
@@ -6931,10 +6932,10 @@
         <v>610</v>
       </c>
       <c r="D116" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E116" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -6951,10 +6952,10 @@
         <v>611</v>
       </c>
       <c r="D117" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E117" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -6977,10 +6978,10 @@
         <v>612</v>
       </c>
       <c r="D118" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E118" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H118">
         <v>2</v>
@@ -6997,10 +6998,10 @@
         <v>613</v>
       </c>
       <c r="D119" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E119" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -7023,10 +7024,10 @@
         <v>614</v>
       </c>
       <c r="D120" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E120" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -7049,10 +7050,10 @@
         <v>615</v>
       </c>
       <c r="D121" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E121" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H121">
         <v>2</v>
@@ -7069,10 +7070,10 @@
         <v>616</v>
       </c>
       <c r="D122" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E122" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F122">
         <v>4</v>
@@ -7095,7 +7096,7 @@
         <v>617</v>
       </c>
       <c r="D123" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G123">
         <v>41</v>
@@ -7115,10 +7116,10 @@
         <v>615</v>
       </c>
       <c r="D124" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E124" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H124">
         <v>3</v>
@@ -7135,10 +7136,10 @@
         <v>615</v>
       </c>
       <c r="D125" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E125" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -7155,10 +7156,10 @@
         <v>618</v>
       </c>
       <c r="D126" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E126" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F126">
         <v>5</v>
@@ -7181,10 +7182,10 @@
         <v>619</v>
       </c>
       <c r="D127" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E127" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -7198,7 +7199,7 @@
         <v>620</v>
       </c>
       <c r="D128" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G128">
         <v>26</v>
@@ -7218,10 +7219,10 @@
         <v>621</v>
       </c>
       <c r="D129" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E129" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F129">
         <v>6</v>
@@ -7244,7 +7245,7 @@
         <v>622</v>
       </c>
       <c r="D130" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="H130">
         <v>2</v>
@@ -7261,7 +7262,7 @@
         <v>622</v>
       </c>
       <c r="D131" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -7278,10 +7279,10 @@
         <v>623</v>
       </c>
       <c r="D132" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E132" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -7304,10 +7305,10 @@
         <v>624</v>
       </c>
       <c r="D133" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E133" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F133">
         <v>7</v>
@@ -7330,10 +7331,10 @@
         <v>625</v>
       </c>
       <c r="D134" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E134" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H134">
         <v>0.75</v>
@@ -7350,10 +7351,10 @@
         <v>625</v>
       </c>
       <c r="D135" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E135" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H135">
         <v>2</v>
@@ -7370,10 +7371,10 @@
         <v>626</v>
       </c>
       <c r="D136" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E136" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -7396,10 +7397,10 @@
         <v>627</v>
       </c>
       <c r="D137" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E137" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F137">
         <v>2</v>
@@ -7422,10 +7423,10 @@
         <v>628</v>
       </c>
       <c r="D138" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E138" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F138">
         <v>3</v>
@@ -7448,10 +7449,10 @@
         <v>629</v>
       </c>
       <c r="D139" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E139" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F139">
         <v>4</v>
@@ -7474,10 +7475,10 @@
         <v>630</v>
       </c>
       <c r="D140" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E140" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H140">
         <v>0.75</v>
@@ -7494,10 +7495,10 @@
         <v>630</v>
       </c>
       <c r="D141" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E141" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H141">
         <v>2</v>
@@ -7514,10 +7515,10 @@
         <v>631</v>
       </c>
       <c r="D142" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E142" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F142">
         <v>5</v>
@@ -7540,10 +7541,10 @@
         <v>632</v>
       </c>
       <c r="D143" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E143" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F143">
         <v>6</v>
@@ -7566,10 +7567,10 @@
         <v>633</v>
       </c>
       <c r="D144" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E144" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H144">
         <v>0.75</v>
@@ -7586,10 +7587,10 @@
         <v>633</v>
       </c>
       <c r="D145" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E145" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H145">
         <v>2</v>
@@ -7606,10 +7607,10 @@
         <v>634</v>
       </c>
       <c r="D146" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E146" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F146">
         <v>101</v>
@@ -7632,10 +7633,10 @@
         <v>635</v>
       </c>
       <c r="D147" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E147" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F147">
         <v>2</v>
@@ -7658,10 +7659,10 @@
         <v>636</v>
       </c>
       <c r="D148" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E148" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -7684,10 +7685,10 @@
         <v>637</v>
       </c>
       <c r="D149" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E149" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H149">
         <v>0.75</v>
@@ -7704,10 +7705,10 @@
         <v>637</v>
       </c>
       <c r="D150" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E150" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H150">
         <v>2</v>
@@ -7724,10 +7725,10 @@
         <v>638</v>
       </c>
       <c r="D151" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E151" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -7750,10 +7751,10 @@
         <v>639</v>
       </c>
       <c r="D152" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E152" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F152">
         <v>3</v>
@@ -7773,10 +7774,10 @@
         <v>406</v>
       </c>
       <c r="D153" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E153" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -7790,10 +7791,10 @@
         <v>640</v>
       </c>
       <c r="D154" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E154" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F154">
         <v>3</v>
@@ -7813,10 +7814,10 @@
         <v>408</v>
       </c>
       <c r="D155" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E155" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -7827,10 +7828,10 @@
         <v>409</v>
       </c>
       <c r="D156" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E156" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -7844,7 +7845,7 @@
         <v>641</v>
       </c>
       <c r="D157" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G157">
         <v>39</v>
@@ -7861,10 +7862,10 @@
         <v>642</v>
       </c>
       <c r="D158" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E158" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F158">
         <v>4</v>
@@ -7878,10 +7879,10 @@
         <v>412</v>
       </c>
       <c r="D159" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E159" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -7895,10 +7896,10 @@
         <v>643</v>
       </c>
       <c r="D160" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E160" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F160">
         <v>5</v>
@@ -7918,10 +7919,10 @@
         <v>644</v>
       </c>
       <c r="D161" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E161" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -7935,10 +7936,10 @@
         <v>644</v>
       </c>
       <c r="D162" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E162" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -7952,10 +7953,10 @@
         <v>645</v>
       </c>
       <c r="D163" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E163" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F163">
         <v>6</v>
@@ -7975,10 +7976,10 @@
         <v>646</v>
       </c>
       <c r="D164" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E164" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F164">
         <v>7</v>
@@ -7995,10 +7996,10 @@
         <v>418</v>
       </c>
       <c r="D165" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E165" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -8009,10 +8010,10 @@
         <v>419</v>
       </c>
       <c r="D166" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E166" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -8026,10 +8027,10 @@
         <v>647</v>
       </c>
       <c r="D167" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E167" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F167">
         <v>8</v>
@@ -8049,10 +8050,10 @@
         <v>648</v>
       </c>
       <c r="D168" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E168" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -8066,10 +8067,10 @@
         <v>648</v>
       </c>
       <c r="D169" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E169" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -8083,10 +8084,10 @@
         <v>649</v>
       </c>
       <c r="D170" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E170" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F170">
         <v>4</v>
@@ -8109,10 +8110,10 @@
         <v>650</v>
       </c>
       <c r="D171" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E171" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F171">
         <v>5</v>
@@ -8135,10 +8136,10 @@
         <v>651</v>
       </c>
       <c r="D172" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E172" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F172">
         <v>6</v>
@@ -8161,10 +8162,10 @@
         <v>652</v>
       </c>
       <c r="D173" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E173" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -8178,10 +8179,10 @@
         <v>652</v>
       </c>
       <c r="D174" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E174" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -8195,10 +8196,10 @@
         <v>653</v>
       </c>
       <c r="D175" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E175" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -8212,10 +8213,10 @@
         <v>654</v>
       </c>
       <c r="D176" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E176" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -8229,10 +8230,10 @@
         <v>655</v>
       </c>
       <c r="D177" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E177" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -8246,10 +8247,10 @@
         <v>656</v>
       </c>
       <c r="D178" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E178" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -8263,10 +8264,10 @@
         <v>657</v>
       </c>
       <c r="D179" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="E179" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -8280,10 +8281,10 @@
         <v>657</v>
       </c>
       <c r="D180" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="E180" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -8297,10 +8298,10 @@
         <v>657</v>
       </c>
       <c r="D181" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E181" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -8314,10 +8315,10 @@
         <v>658</v>
       </c>
       <c r="D182" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E182" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F182">
         <v>0</v>
@@ -8340,10 +8341,10 @@
         <v>659</v>
       </c>
       <c r="D183" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E183" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F183">
         <v>1</v>
@@ -8366,10 +8367,10 @@
         <v>660</v>
       </c>
       <c r="D184" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E184" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F184">
         <v>2</v>
@@ -8392,10 +8393,10 @@
         <v>661</v>
       </c>
       <c r="D185" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E185" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F185">
         <v>3</v>
@@ -8418,10 +8419,10 @@
         <v>662</v>
       </c>
       <c r="D186" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E186" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F186">
         <v>4</v>
@@ -8444,10 +8445,10 @@
         <v>663</v>
       </c>
       <c r="D187" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E187" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -8461,10 +8462,10 @@
         <v>663</v>
       </c>
       <c r="D188" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E188" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -8478,10 +8479,10 @@
         <v>663</v>
       </c>
       <c r="D189" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E189" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -8495,10 +8496,10 @@
         <v>664</v>
       </c>
       <c r="D190" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E190" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F190">
         <v>5</v>
@@ -8521,10 +8522,10 @@
         <v>665</v>
       </c>
       <c r="D191" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E191" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F191">
         <v>6</v>
@@ -8547,10 +8548,10 @@
         <v>666</v>
       </c>
       <c r="D192" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E192" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F192">
         <v>7</v>
@@ -8573,10 +8574,10 @@
         <v>667</v>
       </c>
       <c r="D193" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E193" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -8590,10 +8591,10 @@
         <v>667</v>
       </c>
       <c r="D194" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E194" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -8607,10 +8608,10 @@
         <v>667</v>
       </c>
       <c r="D195" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E195" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -8624,10 +8625,10 @@
         <v>667</v>
       </c>
       <c r="D196" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E196" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -8641,10 +8642,10 @@
         <v>668</v>
       </c>
       <c r="D197" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E197" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F197">
         <v>8</v>
@@ -8667,10 +8668,10 @@
         <v>669</v>
       </c>
       <c r="D198" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E198" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F198">
         <v>9</v>
@@ -8693,10 +8694,10 @@
         <v>670</v>
       </c>
       <c r="D199" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E199" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F199">
         <v>10</v>
@@ -8716,10 +8717,10 @@
         <v>453</v>
       </c>
       <c r="D200" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E200" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -8730,10 +8731,10 @@
         <v>454</v>
       </c>
       <c r="D201" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E201" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -8744,10 +8745,10 @@
         <v>455</v>
       </c>
       <c r="D202" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E202" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -8761,10 +8762,10 @@
         <v>671</v>
       </c>
       <c r="D203" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E203" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F203">
         <v>11</v>
@@ -8787,10 +8788,10 @@
         <v>672</v>
       </c>
       <c r="D204" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E204" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F204">
         <v>12</v>
@@ -8813,10 +8814,10 @@
         <v>673</v>
       </c>
       <c r="D205" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E205" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F205">
         <v>13</v>
@@ -8836,10 +8837,10 @@
         <v>459</v>
       </c>
       <c r="D206" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E206" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
@@ -8850,10 +8851,10 @@
         <v>460</v>
       </c>
       <c r="D207" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E207" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -8867,10 +8868,10 @@
         <v>674</v>
       </c>
       <c r="D208" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E208" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F208">
         <v>14</v>
@@ -8893,10 +8894,10 @@
         <v>675</v>
       </c>
       <c r="D209" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E209" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F209">
         <v>15</v>
@@ -8919,10 +8920,10 @@
         <v>676</v>
       </c>
       <c r="D210" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E210" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F210">
         <v>16</v>
@@ -8942,10 +8943,10 @@
         <v>464</v>
       </c>
       <c r="D211" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E211" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -8956,10 +8957,10 @@
         <v>465</v>
       </c>
       <c r="D212" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E212" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -8970,10 +8971,10 @@
         <v>466</v>
       </c>
       <c r="D213" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E213" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -8987,10 +8988,10 @@
         <v>677</v>
       </c>
       <c r="D214" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E214" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F214">
         <v>17</v>
@@ -9013,7 +9014,7 @@
         <v>678</v>
       </c>
       <c r="D215" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -9027,10 +9028,10 @@
         <v>679</v>
       </c>
       <c r="D216" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E216" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F216">
         <v>18</v>
@@ -9050,10 +9051,10 @@
         <v>470</v>
       </c>
       <c r="D217" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E217" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -9064,10 +9065,10 @@
         <v>471</v>
       </c>
       <c r="D218" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E218" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -9078,10 +9079,10 @@
         <v>472</v>
       </c>
       <c r="D219" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E219" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -9095,10 +9096,10 @@
         <v>680</v>
       </c>
       <c r="D220" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E220" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F220">
         <v>19</v>
@@ -9118,13 +9119,13 @@
         <v>474</v>
       </c>
       <c r="C221" t="s">
-        <v>681</v>
+        <v>952</v>
       </c>
       <c r="D221" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E221" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F221">
         <v>20</v>
@@ -9144,13 +9145,13 @@
         <v>475</v>
       </c>
       <c r="C222" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D222" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E222" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F222">
         <v>21</v>
@@ -9170,10 +9171,10 @@
         <v>476</v>
       </c>
       <c r="D223" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E223" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -9184,10 +9185,10 @@
         <v>477</v>
       </c>
       <c r="D224" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E224" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -9198,13 +9199,13 @@
         <v>478</v>
       </c>
       <c r="C225" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D225" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E225" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F225">
         <v>22</v>
@@ -9224,13 +9225,13 @@
         <v>479</v>
       </c>
       <c r="C226" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D226" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E226" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F226">
         <v>23</v>
@@ -9250,13 +9251,13 @@
         <v>480</v>
       </c>
       <c r="C227" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D227" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E227" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F227">
         <v>24</v>
@@ -9276,10 +9277,10 @@
         <v>481</v>
       </c>
       <c r="D228" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E228" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -9290,10 +9291,10 @@
         <v>482</v>
       </c>
       <c r="D229" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E229" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -9304,13 +9305,13 @@
         <v>483</v>
       </c>
       <c r="C230" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D230" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E230" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F230">
         <v>25</v>
@@ -9330,13 +9331,13 @@
         <v>484</v>
       </c>
       <c r="C231" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D231" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E231" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F231">
         <v>26</v>
@@ -9356,10 +9357,10 @@
         <v>485</v>
       </c>
       <c r="D232" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E232" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -9370,10 +9371,10 @@
         <v>486</v>
       </c>
       <c r="D233" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E233" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
@@ -9384,13 +9385,13 @@
         <v>487</v>
       </c>
       <c r="C234" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D234" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E234" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F234">
         <v>27</v>
@@ -9410,13 +9411,13 @@
         <v>488</v>
       </c>
       <c r="C235" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D235" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E235" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F235">
         <v>28</v>
@@ -9436,13 +9437,13 @@
         <v>489</v>
       </c>
       <c r="C236" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D236" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E236" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F236">
         <v>29</v>
@@ -9462,10 +9463,10 @@
         <v>490</v>
       </c>
       <c r="D237" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E237" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
@@ -9476,13 +9477,13 @@
         <v>491</v>
       </c>
       <c r="C238" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D238" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E238" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F238">
         <v>30</v>
@@ -9502,10 +9503,10 @@
         <v>492</v>
       </c>
       <c r="C239" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D239" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
@@ -9516,10 +9517,10 @@
         <v>493</v>
       </c>
       <c r="D240" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E240" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
@@ -9530,7 +9531,7 @@
         <v>494</v>
       </c>
       <c r="D241" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
@@ -9541,13 +9542,13 @@
         <v>495</v>
       </c>
       <c r="C242" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D242" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E242" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F242">
         <v>31</v>
@@ -9567,13 +9568,13 @@
         <v>496</v>
       </c>
       <c r="C243" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D243" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E243" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F243">
         <v>32</v>
@@ -9593,13 +9594,13 @@
         <v>497</v>
       </c>
       <c r="C244" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D244" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E244" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F244">
         <v>33</v>
@@ -9619,10 +9620,10 @@
         <v>498</v>
       </c>
       <c r="D245" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E245" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
@@ -9633,13 +9634,13 @@
         <v>499</v>
       </c>
       <c r="C246" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D246" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="E246" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F246">
         <v>34</v>
@@ -9659,13 +9660,13 @@
         <v>500</v>
       </c>
       <c r="C247" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D247" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="E247" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F247">
         <v>35</v>
@@ -9685,13 +9686,13 @@
         <v>501</v>
       </c>
       <c r="C248" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D248" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="E248" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F248">
         <v>36</v>

</xml_diff>